<commit_message>
added in a new env.py file
</commit_message>
<xml_diff>
--- a/Outputs/SA_MI.xlsx
+++ b/Outputs/SA_MI.xlsx
@@ -23,7 +23,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -167,6 +167,12 @@
       <color indexed="8"/>
       <sz val="14"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="11"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -288,7 +294,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -380,6 +386,27 @@
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -389,28 +416,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -421,6 +427,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -822,7 +829,7 @@
       <selection activeCell="B23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="9.140625" customWidth="1" style="2" min="1" max="1"/>
     <col width="11.140625" customWidth="1" style="3" min="2" max="3"/>
@@ -832,7 +839,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="B1" s="47" t="n"/>
+      <c r="B1" s="54" t="n"/>
       <c r="F1" s="38" t="n"/>
       <c r="G1" s="38" t="n"/>
       <c r="H1" s="38" t="n"/>
@@ -840,7 +847,7 @@
       <c r="J1" s="38" t="n"/>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="B2" s="48" t="inlineStr">
+      <c r="B2" s="55" t="inlineStr">
         <is>
           <t>Source Data &amp; Defintions</t>
         </is>
@@ -852,7 +859,7 @@
       <c r="J2" s="38" t="n"/>
     </row>
     <row r="3" ht="388.5" customHeight="1">
-      <c r="B3" s="49" t="inlineStr">
+      <c r="B3" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">Data source 
 Monthly specialist advice activity returns are collected from Integrated Care Boards (ICBs) as part of the System Elective Recovery Outpatient Collection (System EROC). 
@@ -875,7 +882,7 @@
       <c r="J3" s="5" t="n"/>
     </row>
     <row r="4" ht="6.6" customHeight="1">
-      <c r="B4" s="49" t="n"/>
+      <c r="B4" s="51" t="n"/>
       <c r="F4" s="38" t="n"/>
       <c r="G4" s="38" t="n"/>
       <c r="H4" s="38" t="n"/>
@@ -895,7 +902,7 @@
       <c r="J5" s="38" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="51" t="inlineStr">
+      <c r="B6" s="56" t="inlineStr">
         <is>
           <t>The data are also available by ‘type of specialist advice’, and defines the different types as:</t>
         </is>
@@ -907,7 +914,7 @@
       <c r="J6" s="38" t="n"/>
     </row>
     <row r="7" ht="36.75" customHeight="1">
-      <c r="B7" s="46" t="inlineStr">
+      <c r="B7" s="53" t="inlineStr">
         <is>
           <t>Pre Referral specialist advice (e.g. Advice &amp; Guidance)</t>
         </is>
@@ -919,7 +926,7 @@
       <c r="J7" s="38" t="n"/>
     </row>
     <row r="8" ht="70.5" customFormat="1" customHeight="1" s="3">
-      <c r="B8" s="52" t="inlineStr">
+      <c r="B8" s="47" t="inlineStr">
         <is>
           <t>Specialist advice to support a clinical dialogue, enabling a referring clinician to seek advice from a specialist prior to, or instead of referral about a named patient. This can be synchronous, for example, a telephone call; or  asynchronous, enabled electronically through the NHS e-Referral Service (e-RS) Advice &amp; Guidance channel or other IT platforms / dedicated email addresses where there is agreement from all stakeholders that these will be used to leverage Advice &amp; Guidance</t>
         </is>
@@ -931,7 +938,7 @@
       <c r="J8" s="40" t="n"/>
     </row>
     <row r="9" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B9" s="52" t="inlineStr">
+      <c r="B9" s="47" t="inlineStr">
         <is>
           <t>Pre Referral Specialist advice may be provided by appropriately trained and commissioned specialists including both consultant and non-consultant led services in secondary care community or primary care providers, interface or intermediate services, and referral management systems.</t>
         </is>
@@ -943,7 +950,7 @@
       <c r="J9" s="40" t="n"/>
     </row>
     <row r="10" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B10" s="52" t="inlineStr">
+      <c r="B10" s="47" t="inlineStr">
         <is>
           <t>This will typically be accessed via a digital communication channel and facilitate a two-way dialogue and sharing of relevant clinical information in relation to the management of a named patient where at the outset of the interaction there is no clear intention to refer to secondary care.</t>
         </is>
@@ -955,7 +962,7 @@
       <c r="J10" s="40" t="n"/>
     </row>
     <row r="11" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B11" s="53" t="inlineStr">
+      <c r="B11" s="48" t="inlineStr">
         <is>
           <t>This is non face to face activity, with no referral or booking having yet been made, and as such there has been no RTT Clock Start.</t>
         </is>
@@ -978,7 +985,7 @@
       <c r="J12" s="38" t="n"/>
     </row>
     <row r="13" ht="36.75" customHeight="1">
-      <c r="B13" s="46" t="inlineStr">
+      <c r="B13" s="53" t="inlineStr">
         <is>
           <t>Post Referral Specialist advice (e.g. Referral Triage models that offer Specialist advice)</t>
         </is>
@@ -990,7 +997,7 @@
       <c r="J13" s="38" t="n"/>
     </row>
     <row r="14" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B14" s="52" t="inlineStr">
+      <c r="B14" s="47" t="inlineStr">
         <is>
           <t>Specialist-led assessment of a patient’s clinical referral Information to support a decision on primary care management or the most appropriate onward clinical pathway.</t>
         </is>
@@ -1002,7 +1009,7 @@
       <c r="J14" s="40" t="n"/>
     </row>
     <row r="15" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B15" s="52" t="inlineStr">
+      <c r="B15" s="47" t="inlineStr">
         <is>
           <t>Referrals may be returned to the original referrer with advice to continue to manage in the community, similar to specialist advice, but differ as a referral will have been created with the implicit expectation that onward care would be managed by the service receiving the referral.</t>
         </is>
@@ -1014,7 +1021,7 @@
       <c r="J15" s="40" t="n"/>
     </row>
     <row r="16" ht="59.25" customFormat="1" customHeight="1" s="3">
-      <c r="B16" s="52" t="inlineStr">
+      <c r="B16" s="47" t="inlineStr">
         <is>
           <t>Referral triage can be undertaken by secondary care providers through Referral Assessment Services (RAS) via e-RS, Clinical assessment and triage services (CATS) and referral management centres (RMCs) providing intermediary levels of clinical triage, assessment and treatment between traditional primary and secondary care, or within primary care providers.</t>
         </is>
@@ -1026,21 +1033,21 @@
       <c r="J16" s="40" t="n"/>
     </row>
     <row r="17" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B17" s="53" t="inlineStr">
+      <c r="B17" s="48" t="inlineStr">
         <is>
           <t>This is non-Face to Face activity, but as a referral has been made there has been an RTT Clock Start. However, no booking, or ASI in lieu of a booking, will have been made, and the episode / patient is not automatically registered on provider PTL.</t>
         </is>
       </c>
     </row>
     <row r="18" ht="36.75" customFormat="1" customHeight="1" s="4">
-      <c r="B18" s="55" t="inlineStr">
+      <c r="B18" s="49" t="inlineStr">
         <is>
           <t xml:space="preserve">Other types of specialist advice </t>
         </is>
       </c>
     </row>
     <row r="19" ht="50.1" customFormat="1" customHeight="1" s="3">
-      <c r="B19" s="52" t="inlineStr">
+      <c r="B19" s="47" t="inlineStr">
         <is>
           <t>Other recorded clinical dialogue that facilitates the seeking and/or provision of specialist advice to support a referrer, enabling more patients to be managed without the need for an onward booking and thereby avoiding unnecessary first attendances where these do not add clinical value.</t>
         </is>
@@ -1049,8 +1056,8 @@
     <row r="20">
       <c r="B20" s="43" t="n"/>
       <c r="C20" s="43" t="n"/>
-      <c r="D20" s="51" t="n"/>
-      <c r="E20" s="51" t="n"/>
+      <c r="D20" s="56" t="n"/>
+      <c r="E20" s="56" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="50" t="inlineStr">
@@ -1060,14 +1067,14 @@
       </c>
     </row>
     <row r="22" ht="44.45" customFormat="1" customHeight="1" s="3">
-      <c r="B22" s="49" t="inlineStr">
+      <c r="B22" s="51" t="inlineStr">
         <is>
           <t>The data collection launched in August 2021, making this a relatively new data collection. Please use caution when interpreting this data as we continue to work with ICBs to improve data quality.</t>
         </is>
       </c>
     </row>
     <row r="23" ht="81.95" customFormat="1" customHeight="1" s="3">
-      <c r="B23" s="56" t="inlineStr">
+      <c r="B23" s="52" t="inlineStr">
         <is>
           <t>Data are included from April 2022 to the latest available reporting period. The England level data is an aggregation of the latest available data as reported by ICBs. This means that the latest position is subject to change as we receive more detail relating to the outcome and status of the specialist advice requests. This is particularly relevant when viewing activity data for 'Processed' and 'Diverted' requests, due to a lag in the reporting of outcomes and status' for requests that are raised toward the end of the reporting period. This lag in the underlying data means that there is an expected general downward trend for these measures in the most recent months, this reporting gap should reduce over time as the data is refreshed each month.</t>
         </is>
@@ -1087,7 +1094,7 @@
       </c>
     </row>
     <row r="26" ht="58.5" customHeight="1">
-      <c r="B26" s="49" t="inlineStr">
+      <c r="B26" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">For further information about the published management information relating to outpatient recovery and transformation, please contact us at england.outpatient-transformation@nhs.net.  </t>
         </is>
@@ -1106,7 +1113,7 @@
       <c r="E28" s="38" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="54" t="n"/>
+      <c r="B29" s="46" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -1150,10 +1157,10 @@
   <dimension ref="A2:AF122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25" outlineLevelCol="0"/>
   <cols>
     <col width="3.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="26.7109375" customWidth="1" style="1" min="2" max="2"/>
@@ -1384,24 +1391,24 @@
           <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
         </is>
       </c>
-      <c r="H14" s="60" t="n"/>
-      <c r="I14" s="61" t="n"/>
+      <c r="H14" s="61" t="n"/>
+      <c r="I14" s="62" t="n"/>
       <c r="J14" s="21" t="n"/>
       <c r="K14" s="58" t="inlineStr">
         <is>
           <t>Post Referral Specialist Advice</t>
         </is>
       </c>
-      <c r="L14" s="60" t="n"/>
-      <c r="M14" s="61" t="n"/>
+      <c r="L14" s="61" t="n"/>
+      <c r="M14" s="62" t="n"/>
       <c r="N14" s="21" t="n"/>
       <c r="O14" s="58" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="P14" s="60" t="n"/>
-      <c r="Q14" s="61" t="n"/>
+      <c r="P14" s="61" t="n"/>
+      <c r="Q14" s="62" t="n"/>
     </row>
     <row r="15" ht="60.95" customFormat="1" customHeight="1" s="8">
       <c r="B15" s="7" t="inlineStr">
@@ -3281,40 +3288,40 @@
           <t>February 2025</t>
         </is>
       </c>
-      <c r="C50" s="62" t="n">
+      <c r="C50" s="63" t="n">
         <v>1012366</v>
       </c>
-      <c r="D50" s="62" t="n">
+      <c r="D50" s="63" t="n">
         <v>878460</v>
       </c>
-      <c r="E50" s="62" t="n">
+      <c r="E50" s="63" t="n">
         <v>207333</v>
       </c>
-      <c r="F50" s="63" t="n"/>
-      <c r="G50" s="62" t="n">
+      <c r="F50" s="64" t="n"/>
+      <c r="G50" s="63" t="n">
         <v>241855</v>
       </c>
-      <c r="H50" s="62" t="n">
+      <c r="H50" s="63" t="n">
         <v>203451</v>
       </c>
-      <c r="I50" s="62" t="n">
+      <c r="I50" s="63" t="n">
         <v>99326</v>
       </c>
-      <c r="J50" s="63" t="n"/>
-      <c r="K50" s="62" t="n">
+      <c r="J50" s="64" t="n"/>
+      <c r="K50" s="63" t="n">
         <v>762315</v>
       </c>
-      <c r="L50" s="62" t="n">
+      <c r="L50" s="63" t="n">
         <v>666813</v>
       </c>
-      <c r="M50" s="62" t="n">
+      <c r="M50" s="63" t="n">
         <v>105845</v>
       </c>
-      <c r="N50" s="63" t="n"/>
-      <c r="O50" s="62" t="n">
+      <c r="N50" s="64" t="n"/>
+      <c r="O50" s="63" t="n">
         <v>8196</v>
       </c>
-      <c r="P50" s="62" t="n">
+      <c r="P50" s="63" t="n">
         <v>8196</v>
       </c>
       <c r="Q50" s="36" t="n">
@@ -3334,40 +3341,40 @@
           <t>March 2025</t>
         </is>
       </c>
-      <c r="C51" s="62" t="n">
+      <c r="C51" s="63" t="n">
         <v>1036615</v>
       </c>
-      <c r="D51" s="62" t="n">
+      <c r="D51" s="63" t="n">
         <v>802640</v>
       </c>
-      <c r="E51" s="62" t="n">
+      <c r="E51" s="63" t="n">
         <v>184803</v>
       </c>
-      <c r="F51" s="63" t="n"/>
-      <c r="G51" s="62" t="n">
+      <c r="F51" s="64" t="n"/>
+      <c r="G51" s="63" t="n">
         <v>264299</v>
       </c>
-      <c r="H51" s="62" t="n">
+      <c r="H51" s="63" t="n">
         <v>181485</v>
       </c>
-      <c r="I51" s="62" t="n">
+      <c r="I51" s="63" t="n">
         <v>84357</v>
       </c>
-      <c r="J51" s="63" t="n"/>
-      <c r="K51" s="64" t="n">
+      <c r="J51" s="64" t="n"/>
+      <c r="K51" s="65" t="n">
         <v>763121</v>
       </c>
-      <c r="L51" s="65" t="n">
+      <c r="L51" s="66" t="n">
         <v>611960</v>
       </c>
-      <c r="M51" s="65" t="n">
+      <c r="M51" s="66" t="n">
         <v>97998</v>
       </c>
-      <c r="N51" s="66" t="n"/>
-      <c r="O51" s="65" t="n">
+      <c r="N51" s="67" t="n"/>
+      <c r="O51" s="66" t="n">
         <v>9195</v>
       </c>
-      <c r="P51" s="65" t="n">
+      <c r="P51" s="66" t="n">
         <v>9195</v>
       </c>
       <c r="Q51" s="17" t="n">
@@ -3378,12 +3385,25 @@
       <c r="W51" s="12" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1">
-      <c r="B52" s="29" t="inlineStr">
+      <c r="B52" s="11" t="inlineStr">
         <is>
           <t>Specialist Advice Activity by measure, per working day</t>
         </is>
       </c>
-      <c r="G52" s="16" t="n"/>
+      <c r="C52" s="66" t="n"/>
+      <c r="D52" s="66" t="n"/>
+      <c r="E52" s="66" t="n"/>
+      <c r="F52" s="67" t="n"/>
+      <c r="G52" s="65" t="n"/>
+      <c r="H52" s="66" t="n"/>
+      <c r="I52" s="66" t="n"/>
+      <c r="J52" s="67" t="n"/>
+      <c r="K52" s="66" t="n"/>
+      <c r="L52" s="66" t="n"/>
+      <c r="M52" s="66" t="n"/>
+      <c r="N52" s="67" t="n"/>
+      <c r="O52" s="66" t="n"/>
+      <c r="P52" s="66" t="n"/>
       <c r="T52" s="12" t="n"/>
       <c r="U52" s="12" t="n"/>
       <c r="V52" s="12" t="n"/>
@@ -3408,24 +3428,24 @@
           <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
         </is>
       </c>
-      <c r="H54" s="60" t="n"/>
-      <c r="I54" s="61" t="n"/>
+      <c r="H54" s="61" t="n"/>
+      <c r="I54" s="62" t="n"/>
       <c r="J54" s="21" t="n"/>
       <c r="K54" s="58" t="inlineStr">
         <is>
           <t>Post Referral Specialist Advice</t>
         </is>
       </c>
-      <c r="L54" s="60" t="n"/>
-      <c r="M54" s="61" t="n"/>
+      <c r="L54" s="61" t="n"/>
+      <c r="M54" s="62" t="n"/>
       <c r="N54" s="21" t="n"/>
       <c r="O54" s="58" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="P54" s="60" t="n"/>
-      <c r="Q54" s="61" t="n"/>
+      <c r="P54" s="61" t="n"/>
+      <c r="Q54" s="62" t="n"/>
       <c r="W54" s="25" t="n"/>
       <c r="X54" s="26" t="n"/>
       <c r="Y54" s="12" t="n"/>
@@ -5792,7 +5812,7 @@
         <v>20</v>
       </c>
       <c r="T90" s="12" t="n"/>
-      <c r="U90" s="67" t="n"/>
+      <c r="U90" s="68" t="n"/>
     </row>
     <row r="91">
       <c r="B91" s="25" t="n"/>

</xml_diff>

<commit_message>
redone the formatting to include column 18
</commit_message>
<xml_diff>
--- a/Outputs/SA_MI.xlsx
+++ b/Outputs/SA_MI.xlsx
@@ -829,7 +829,7 @@
       <selection activeCell="B23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="9.140625" customWidth="1" style="2" min="1" max="1"/>
     <col width="11.140625" customWidth="1" style="3" min="2" max="3"/>
@@ -1160,7 +1160,7 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
   <cols>
     <col width="3.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="26.7109375" customWidth="1" style="1" min="2" max="2"/>
@@ -3324,7 +3324,7 @@
       <c r="P50" s="63" t="n">
         <v>8196</v>
       </c>
-      <c r="Q50" s="36" t="n">
+      <c r="Q50" s="63" t="n">
         <v>2162</v>
       </c>
       <c r="S50" s="12" t="n"/>
@@ -3377,7 +3377,7 @@
       <c r="P51" s="66" t="n">
         <v>9195</v>
       </c>
-      <c r="Q51" s="17" t="n">
+      <c r="Q51" s="66" t="n">
         <v>2448</v>
       </c>
       <c r="T51" s="12" t="n"/>
@@ -3385,25 +3385,12 @@
       <c r="W51" s="12" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1">
-      <c r="B52" s="11" t="inlineStr">
+      <c r="B52" s="29" t="inlineStr">
         <is>
           <t>Specialist Advice Activity by measure, per working day</t>
         </is>
       </c>
-      <c r="C52" s="66" t="n"/>
-      <c r="D52" s="66" t="n"/>
-      <c r="E52" s="66" t="n"/>
-      <c r="F52" s="67" t="n"/>
-      <c r="G52" s="65" t="n"/>
-      <c r="H52" s="66" t="n"/>
-      <c r="I52" s="66" t="n"/>
-      <c r="J52" s="67" t="n"/>
-      <c r="K52" s="66" t="n"/>
-      <c r="L52" s="66" t="n"/>
-      <c r="M52" s="66" t="n"/>
-      <c r="N52" s="67" t="n"/>
-      <c r="O52" s="66" t="n"/>
-      <c r="P52" s="66" t="n"/>
+      <c r="G52" s="16" t="n"/>
       <c r="T52" s="12" t="n"/>
       <c r="U52" s="12" t="n"/>
       <c r="V52" s="12" t="n"/>

</xml_diff>

<commit_message>
re merge the cells in second table
</commit_message>
<xml_diff>
--- a/Outputs/SA_MI.xlsx
+++ b/Outputs/SA_MI.xlsx
@@ -1154,7 +1154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AF122"/>
+  <dimension ref="A2:AF123"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
@@ -3384,323 +3384,258 @@
       <c r="V51" s="12" t="n"/>
       <c r="W51" s="12" t="n"/>
     </row>
-    <row r="52" ht="15" customHeight="1">
-      <c r="B52" s="29" t="inlineStr">
+    <row r="52" ht="15" customHeight="1"/>
+    <row r="53">
+      <c r="B53" s="29" t="inlineStr">
         <is>
           <t>Specialist Advice Activity by measure, per working day</t>
         </is>
       </c>
-      <c r="G52" s="16" t="n"/>
-      <c r="T52" s="12" t="n"/>
-      <c r="U52" s="12" t="n"/>
-      <c r="V52" s="12" t="n"/>
-      <c r="W52" s="12" t="n"/>
-      <c r="X52" s="26" t="n"/>
-      <c r="Y52" s="12" t="n"/>
-    </row>
-    <row r="53">
-      <c r="W53" s="25" t="n"/>
+      <c r="G53" s="16" t="n"/>
+      <c r="T53" s="12" t="n"/>
+      <c r="U53" s="12" t="n"/>
+      <c r="V53" s="12" t="n"/>
+      <c r="W53" s="12" t="n"/>
       <c r="X53" s="26" t="n"/>
       <c r="Y53" s="12" t="n"/>
     </row>
     <row r="54" ht="30" customHeight="1">
-      <c r="C54" s="58" t="inlineStr">
-        <is>
-          <t>All types of Specialist Advice</t>
-        </is>
-      </c>
-      <c r="F54" s="21" t="n"/>
-      <c r="G54" s="59" t="inlineStr">
-        <is>
-          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
-        </is>
-      </c>
-      <c r="H54" s="61" t="n"/>
-      <c r="I54" s="62" t="n"/>
-      <c r="J54" s="21" t="n"/>
-      <c r="K54" s="59" t="inlineStr">
-        <is>
-          <t>Post Referral Specialist Advice</t>
-        </is>
-      </c>
-      <c r="L54" s="61" t="n"/>
-      <c r="M54" s="62" t="n"/>
-      <c r="N54" s="21" t="n"/>
-      <c r="O54" s="59" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="P54" s="61" t="n"/>
-      <c r="Q54" s="62" t="n"/>
       <c r="W54" s="25" t="n"/>
       <c r="X54" s="26" t="n"/>
       <c r="Y54" s="12" t="n"/>
     </row>
     <row r="55" ht="73.5" customHeight="1">
-      <c r="B55" s="9" t="inlineStr">
+      <c r="C55" s="58" t="inlineStr">
+        <is>
+          <t>All types of Specialist Advice</t>
+        </is>
+      </c>
+      <c r="F55" s="21" t="n"/>
+      <c r="G55" s="59" t="inlineStr">
+        <is>
+          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
+        </is>
+      </c>
+      <c r="H55" s="61" t="n"/>
+      <c r="I55" s="62" t="n"/>
+      <c r="J55" s="21" t="n"/>
+      <c r="K55" s="59" t="inlineStr">
+        <is>
+          <t>Post Referral Specialist Advice</t>
+        </is>
+      </c>
+      <c r="L55" s="61" t="n"/>
+      <c r="M55" s="62" t="n"/>
+      <c r="N55" s="21" t="n"/>
+      <c r="O55" s="59" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="P55" s="61" t="n"/>
+      <c r="Q55" s="62" t="n"/>
+      <c r="W55" s="25" t="n"/>
+      <c r="X55" s="26" t="n"/>
+      <c r="Y55" s="12" t="n"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Month </t>
         </is>
       </c>
-      <c r="C55" s="9" t="inlineStr">
+      <c r="C56" s="9" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="D55" s="9" t="inlineStr">
+      <c r="D56" s="9" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="E55" s="9" t="inlineStr">
+      <c r="E56" s="9" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="F55" s="22" t="n"/>
-      <c r="G55" s="10" t="inlineStr">
+      <c r="F56" s="22" t="n"/>
+      <c r="G56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="H55" s="10" t="inlineStr">
+      <c r="H56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="I55" s="10" t="inlineStr">
+      <c r="I56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="J55" s="22" t="n"/>
-      <c r="K55" s="10" t="inlineStr">
+      <c r="J56" s="22" t="n"/>
+      <c r="K56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="L55" s="10" t="inlineStr">
+      <c r="L56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="M55" s="10" t="inlineStr">
+      <c r="M56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="N55" s="22" t="n"/>
-      <c r="O55" s="10" t="inlineStr">
+      <c r="N56" s="22" t="n"/>
+      <c r="O56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="P55" s="10" t="inlineStr">
+      <c r="P56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="Q55" s="10" t="inlineStr">
+      <c r="Q56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="S55" s="28" t="inlineStr">
+      <c r="S56" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">No. of working days </t>
         </is>
       </c>
-      <c r="W55" s="25" t="n"/>
-    </row>
-    <row r="56">
-      <c r="B56" s="11">
-        <f>B16</f>
-        <v/>
-      </c>
-      <c r="C56" s="13">
-        <f>C16/$S56</f>
-        <v/>
-      </c>
-      <c r="D56" s="13">
-        <f>D16/$S56</f>
-        <v/>
-      </c>
-      <c r="E56" s="13">
-        <f>E16/$S56</f>
-        <v/>
-      </c>
-      <c r="G56" s="13">
-        <f>G16/$S56</f>
-        <v/>
-      </c>
-      <c r="H56" s="13">
-        <f>H16/$S56</f>
-        <v/>
-      </c>
-      <c r="I56" s="13">
-        <f>I16/$S56</f>
-        <v/>
-      </c>
-      <c r="K56" s="13">
-        <f>K16/$S56</f>
-        <v/>
-      </c>
-      <c r="L56" s="13">
-        <f>L16/$S56</f>
-        <v/>
-      </c>
-      <c r="M56" s="13">
-        <f>M16/$S56</f>
-        <v/>
-      </c>
-      <c r="O56" s="13">
-        <f>O16/$S56</f>
-        <v/>
-      </c>
-      <c r="P56" s="13">
-        <f>P16/$S56</f>
-        <v/>
-      </c>
-      <c r="Q56" s="13">
-        <f>Q16/$S56</f>
-        <v/>
-      </c>
-      <c r="R56" s="12" t="n"/>
-      <c r="S56" s="27" t="n">
-        <v>19</v>
-      </c>
-      <c r="V56" s="24" t="n"/>
-      <c r="W56" s="12" t="n"/>
-      <c r="X56" s="12" t="n"/>
-      <c r="Y56" s="12" t="n"/>
+      <c r="W56" s="25" t="n"/>
     </row>
     <row r="57">
       <c r="B57" s="11">
-        <f>B17</f>
+        <f>B16</f>
         <v/>
       </c>
       <c r="C57" s="13">
-        <f>C17/$S57</f>
+        <f>C16/$S56</f>
         <v/>
       </c>
       <c r="D57" s="13">
-        <f>D17/$S57</f>
+        <f>D16/$S56</f>
         <v/>
       </c>
       <c r="E57" s="13">
-        <f>E17/$S57</f>
+        <f>E16/$S56</f>
         <v/>
       </c>
       <c r="G57" s="13">
-        <f>G17/$S57</f>
+        <f>G16/$S56</f>
         <v/>
       </c>
       <c r="H57" s="13">
-        <f>H17/$S57</f>
+        <f>H16/$S56</f>
         <v/>
       </c>
       <c r="I57" s="13">
-        <f>I17/$S57</f>
+        <f>I16/$S56</f>
         <v/>
       </c>
       <c r="K57" s="13">
-        <f>K17/$S57</f>
+        <f>K16/$S56</f>
         <v/>
       </c>
       <c r="L57" s="13">
-        <f>L17/$S57</f>
+        <f>L16/$S56</f>
         <v/>
       </c>
       <c r="M57" s="13">
-        <f>M17/$S57</f>
+        <f>M16/$S56</f>
         <v/>
       </c>
       <c r="O57" s="13">
-        <f>O17/$S57</f>
+        <f>O16/$S56</f>
         <v/>
       </c>
       <c r="P57" s="13">
-        <f>P17/$S57</f>
+        <f>P16/$S56</f>
         <v/>
       </c>
       <c r="Q57" s="13">
-        <f>Q17/$S57</f>
+        <f>Q16/$S56</f>
         <v/>
       </c>
       <c r="R57" s="12" t="n"/>
       <c r="S57" s="27" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V57" s="24" t="n"/>
       <c r="W57" s="12" t="n"/>
       <c r="X57" s="12" t="n"/>
       <c r="Y57" s="12" t="n"/>
-      <c r="AA57" s="12" t="n"/>
-      <c r="AB57" s="14" t="n"/>
-      <c r="AE57" s="12" t="n"/>
-      <c r="AF57" s="14" t="n"/>
     </row>
     <row r="58">
       <c r="B58" s="11">
-        <f>B18</f>
+        <f>B17</f>
         <v/>
       </c>
       <c r="C58" s="13">
-        <f>C18/$S58</f>
+        <f>C17/$S57</f>
         <v/>
       </c>
       <c r="D58" s="13">
-        <f>D18/$S58</f>
+        <f>D17/$S57</f>
         <v/>
       </c>
       <c r="E58" s="13">
-        <f>E18/$S58</f>
+        <f>E17/$S57</f>
         <v/>
       </c>
       <c r="G58" s="13">
-        <f>G18/$S58</f>
+        <f>G17/$S57</f>
         <v/>
       </c>
       <c r="H58" s="13">
-        <f>H18/$S58</f>
+        <f>H17/$S57</f>
         <v/>
       </c>
       <c r="I58" s="13">
-        <f>I18/$S58</f>
+        <f>I17/$S57</f>
         <v/>
       </c>
       <c r="K58" s="13">
-        <f>K18/$S58</f>
+        <f>K17/$S57</f>
         <v/>
       </c>
       <c r="L58" s="13">
-        <f>L18/$S58</f>
+        <f>L17/$S57</f>
         <v/>
       </c>
       <c r="M58" s="13">
-        <f>M18/$S58</f>
+        <f>M17/$S57</f>
         <v/>
       </c>
       <c r="O58" s="13">
-        <f>O18/$S58</f>
+        <f>O17/$S57</f>
         <v/>
       </c>
       <c r="P58" s="13">
-        <f>P18/$S58</f>
+        <f>P17/$S57</f>
         <v/>
       </c>
       <c r="Q58" s="13">
-        <f>Q18/$S58</f>
+        <f>Q17/$S57</f>
         <v/>
       </c>
       <c r="R58" s="12" t="n"/>
       <c r="S58" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V58" s="24" t="n"/>
       <c r="W58" s="12" t="n"/>
@@ -3713,60 +3648,60 @@
     </row>
     <row r="59">
       <c r="B59" s="11">
-        <f>B19</f>
+        <f>B18</f>
         <v/>
       </c>
       <c r="C59" s="13">
-        <f>C19/$S59</f>
+        <f>C18/$S58</f>
         <v/>
       </c>
       <c r="D59" s="13">
-        <f>D19/$S59</f>
+        <f>D18/$S58</f>
         <v/>
       </c>
       <c r="E59" s="13">
-        <f>E19/$S59</f>
+        <f>E18/$S58</f>
         <v/>
       </c>
       <c r="G59" s="13">
-        <f>G19/$S59</f>
+        <f>G18/$S58</f>
         <v/>
       </c>
       <c r="H59" s="13">
-        <f>H19/$S59</f>
+        <f>H18/$S58</f>
         <v/>
       </c>
       <c r="I59" s="13">
-        <f>I19/$S59</f>
+        <f>I18/$S58</f>
         <v/>
       </c>
       <c r="K59" s="13">
-        <f>K19/$S59</f>
+        <f>K18/$S58</f>
         <v/>
       </c>
       <c r="L59" s="13">
-        <f>L19/$S59</f>
+        <f>L18/$S58</f>
         <v/>
       </c>
       <c r="M59" s="13">
-        <f>M19/$S59</f>
+        <f>M18/$S58</f>
         <v/>
       </c>
       <c r="O59" s="13">
-        <f>O19/$S59</f>
+        <f>O18/$S58</f>
         <v/>
       </c>
       <c r="P59" s="13">
-        <f>P19/$S59</f>
+        <f>P18/$S58</f>
         <v/>
       </c>
       <c r="Q59" s="13">
-        <f>Q19/$S59</f>
+        <f>Q18/$S58</f>
         <v/>
       </c>
       <c r="R59" s="12" t="n"/>
       <c r="S59" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V59" s="24" t="n"/>
       <c r="W59" s="12" t="n"/>
@@ -3779,60 +3714,60 @@
     </row>
     <row r="60">
       <c r="B60" s="11">
-        <f>B20</f>
+        <f>B19</f>
         <v/>
       </c>
       <c r="C60" s="13">
-        <f>C20/$S60</f>
+        <f>C19/$S59</f>
         <v/>
       </c>
       <c r="D60" s="13">
-        <f>D20/$S60</f>
+        <f>D19/$S59</f>
         <v/>
       </c>
       <c r="E60" s="13">
-        <f>E20/$S60</f>
+        <f>E19/$S59</f>
         <v/>
       </c>
       <c r="G60" s="13">
-        <f>G20/$S60</f>
+        <f>G19/$S59</f>
         <v/>
       </c>
       <c r="H60" s="13">
-        <f>H20/$S60</f>
+        <f>H19/$S59</f>
         <v/>
       </c>
       <c r="I60" s="13">
-        <f>I20/$S60</f>
+        <f>I19/$S59</f>
         <v/>
       </c>
       <c r="K60" s="13">
-        <f>K20/$S60</f>
+        <f>K19/$S59</f>
         <v/>
       </c>
       <c r="L60" s="13">
-        <f>L20/$S60</f>
+        <f>L19/$S59</f>
         <v/>
       </c>
       <c r="M60" s="13">
-        <f>M20/$S60</f>
+        <f>M19/$S59</f>
         <v/>
       </c>
       <c r="O60" s="13">
-        <f>O20/$S60</f>
+        <f>O19/$S59</f>
         <v/>
       </c>
       <c r="P60" s="13">
-        <f>P20/$S60</f>
+        <f>P19/$S59</f>
         <v/>
       </c>
       <c r="Q60" s="13">
-        <f>Q20/$S60</f>
+        <f>Q19/$S59</f>
         <v/>
       </c>
       <c r="R60" s="12" t="n"/>
       <c r="S60" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V60" s="24" t="n"/>
       <c r="W60" s="12" t="n"/>
@@ -3845,60 +3780,60 @@
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="B61" s="11">
-        <f>B21</f>
+        <f>B20</f>
         <v/>
       </c>
       <c r="C61" s="13">
-        <f>C21/$S61</f>
+        <f>C20/$S60</f>
         <v/>
       </c>
       <c r="D61" s="13">
-        <f>D21/$S61</f>
+        <f>D20/$S60</f>
         <v/>
       </c>
       <c r="E61" s="13">
-        <f>E21/$S61</f>
+        <f>E20/$S60</f>
         <v/>
       </c>
       <c r="G61" s="13">
-        <f>G21/$S61</f>
+        <f>G20/$S60</f>
         <v/>
       </c>
       <c r="H61" s="13">
-        <f>H21/$S61</f>
+        <f>H20/$S60</f>
         <v/>
       </c>
       <c r="I61" s="13">
-        <f>I21/$S61</f>
+        <f>I20/$S60</f>
         <v/>
       </c>
       <c r="K61" s="13">
-        <f>K21/$S61</f>
+        <f>K20/$S60</f>
         <v/>
       </c>
       <c r="L61" s="13">
-        <f>L21/$S61</f>
+        <f>L20/$S60</f>
         <v/>
       </c>
       <c r="M61" s="13">
-        <f>M21/$S61</f>
+        <f>M20/$S60</f>
         <v/>
       </c>
       <c r="O61" s="13">
-        <f>O21/$S61</f>
+        <f>O20/$S60</f>
         <v/>
       </c>
       <c r="P61" s="13">
-        <f>P21/$S61</f>
+        <f>P20/$S60</f>
         <v/>
       </c>
       <c r="Q61" s="13">
-        <f>Q21/$S61</f>
-        <v/>
-      </c>
-      <c r="R61" s="15" t="n"/>
+        <f>Q20/$S60</f>
+        <v/>
+      </c>
+      <c r="R61" s="12" t="n"/>
       <c r="S61" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V61" s="24" t="n"/>
       <c r="W61" s="12" t="n"/>
@@ -3911,55 +3846,55 @@
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="B62" s="11">
-        <f>B22</f>
+        <f>B21</f>
         <v/>
       </c>
       <c r="C62" s="13">
-        <f>C22/$S62</f>
+        <f>C21/$S61</f>
         <v/>
       </c>
       <c r="D62" s="13">
-        <f>D22/$S62</f>
+        <f>D21/$S61</f>
         <v/>
       </c>
       <c r="E62" s="13">
-        <f>E22/$S62</f>
+        <f>E21/$S61</f>
         <v/>
       </c>
       <c r="G62" s="13">
-        <f>G22/$S62</f>
+        <f>G21/$S61</f>
         <v/>
       </c>
       <c r="H62" s="13">
-        <f>H22/$S62</f>
+        <f>H21/$S61</f>
         <v/>
       </c>
       <c r="I62" s="13">
-        <f>I22/$S62</f>
+        <f>I21/$S61</f>
         <v/>
       </c>
       <c r="K62" s="13">
-        <f>K22/$S62</f>
+        <f>K21/$S61</f>
         <v/>
       </c>
       <c r="L62" s="13">
-        <f>L22/$S62</f>
+        <f>L21/$S61</f>
         <v/>
       </c>
       <c r="M62" s="13">
-        <f>M22/$S62</f>
+        <f>M21/$S61</f>
         <v/>
       </c>
       <c r="O62" s="13">
-        <f>O22/$S62</f>
+        <f>O21/$S61</f>
         <v/>
       </c>
       <c r="P62" s="13">
-        <f>P22/$S62</f>
+        <f>P21/$S61</f>
         <v/>
       </c>
       <c r="Q62" s="13">
-        <f>Q22/$S62</f>
+        <f>Q21/$S61</f>
         <v/>
       </c>
       <c r="R62" s="15" t="n"/>
@@ -3977,66 +3912,65 @@
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="B63" s="11">
-        <f>B23</f>
+        <f>B22</f>
         <v/>
       </c>
       <c r="C63" s="13">
-        <f>C23/$S63</f>
+        <f>C22/$S62</f>
         <v/>
       </c>
       <c r="D63" s="13">
-        <f>D23/$S63</f>
+        <f>D22/$S62</f>
         <v/>
       </c>
       <c r="E63" s="13">
-        <f>E23/$S63</f>
+        <f>E22/$S62</f>
         <v/>
       </c>
       <c r="G63" s="13">
-        <f>G23/$S63</f>
+        <f>G22/$S62</f>
         <v/>
       </c>
       <c r="H63" s="13">
-        <f>H23/$S63</f>
+        <f>H22/$S62</f>
         <v/>
       </c>
       <c r="I63" s="13">
-        <f>I23/$S63</f>
+        <f>I22/$S62</f>
         <v/>
       </c>
       <c r="K63" s="13">
-        <f>K23/$S63</f>
+        <f>K22/$S62</f>
         <v/>
       </c>
       <c r="L63" s="13">
-        <f>L23/$S63</f>
+        <f>L22/$S62</f>
         <v/>
       </c>
       <c r="M63" s="13">
-        <f>M23/$S63</f>
+        <f>M22/$S62</f>
         <v/>
       </c>
       <c r="O63" s="13">
-        <f>O23/$S63</f>
+        <f>O22/$S62</f>
         <v/>
       </c>
       <c r="P63" s="13">
-        <f>P23/$S63</f>
+        <f>P22/$S62</f>
         <v/>
       </c>
       <c r="Q63" s="13">
-        <f>Q23/$S63</f>
+        <f>Q22/$S62</f>
         <v/>
       </c>
       <c r="R63" s="15" t="n"/>
       <c r="S63" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V63" s="24" t="n"/>
       <c r="W63" s="12" t="n"/>
       <c r="X63" s="12" t="n"/>
       <c r="Y63" s="12" t="n"/>
-      <c r="Z63" s="12" t="n"/>
       <c r="AA63" s="12" t="n"/>
       <c r="AB63" s="14" t="n"/>
       <c r="AE63" s="12" t="n"/>
@@ -4044,60 +3978,60 @@
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="B64" s="11">
-        <f>B24</f>
+        <f>B23</f>
         <v/>
       </c>
       <c r="C64" s="13">
-        <f>C24/$S64</f>
+        <f>C23/$S63</f>
         <v/>
       </c>
       <c r="D64" s="13">
-        <f>D24/$S64</f>
+        <f>D23/$S63</f>
         <v/>
       </c>
       <c r="E64" s="13">
-        <f>E24/$S64</f>
+        <f>E23/$S63</f>
         <v/>
       </c>
       <c r="G64" s="13">
-        <f>G24/$S64</f>
+        <f>G23/$S63</f>
         <v/>
       </c>
       <c r="H64" s="13">
-        <f>H24/$S64</f>
+        <f>H23/$S63</f>
         <v/>
       </c>
       <c r="I64" s="13">
-        <f>I24/$S64</f>
+        <f>I23/$S63</f>
         <v/>
       </c>
       <c r="K64" s="13">
-        <f>K24/$S64</f>
+        <f>K23/$S63</f>
         <v/>
       </c>
       <c r="L64" s="13">
-        <f>L24/$S64</f>
+        <f>L23/$S63</f>
         <v/>
       </c>
       <c r="M64" s="13">
-        <f>M24/$S64</f>
+        <f>M23/$S63</f>
         <v/>
       </c>
       <c r="O64" s="13">
-        <f>O24/$S64</f>
+        <f>O23/$S63</f>
         <v/>
       </c>
       <c r="P64" s="13">
-        <f>P24/$S64</f>
+        <f>P23/$S63</f>
         <v/>
       </c>
       <c r="Q64" s="13">
-        <f>Q24/$S64</f>
+        <f>Q23/$S63</f>
         <v/>
       </c>
       <c r="R64" s="15" t="n"/>
       <c r="S64" s="27" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V64" s="24" t="n"/>
       <c r="W64" s="12" t="n"/>
@@ -4111,60 +4045,60 @@
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="B65" s="11">
-        <f>B25</f>
+        <f>B24</f>
         <v/>
       </c>
       <c r="C65" s="13">
-        <f>C25/$S65</f>
+        <f>C24/$S64</f>
         <v/>
       </c>
       <c r="D65" s="13">
-        <f>D25/$S65</f>
+        <f>D24/$S64</f>
         <v/>
       </c>
       <c r="E65" s="13">
-        <f>E25/$S65</f>
+        <f>E24/$S64</f>
         <v/>
       </c>
       <c r="G65" s="13">
-        <f>G25/$S65</f>
+        <f>G24/$S64</f>
         <v/>
       </c>
       <c r="H65" s="13">
-        <f>H25/$S65</f>
+        <f>H24/$S64</f>
         <v/>
       </c>
       <c r="I65" s="13">
-        <f>I25/$S65</f>
+        <f>I24/$S64</f>
         <v/>
       </c>
       <c r="K65" s="13">
-        <f>K25/$S65</f>
+        <f>K24/$S64</f>
         <v/>
       </c>
       <c r="L65" s="13">
-        <f>L25/$S65</f>
+        <f>L24/$S64</f>
         <v/>
       </c>
       <c r="M65" s="13">
-        <f>M25/$S65</f>
+        <f>M24/$S64</f>
         <v/>
       </c>
       <c r="O65" s="13">
-        <f>O25/$S65</f>
+        <f>O24/$S64</f>
         <v/>
       </c>
       <c r="P65" s="13">
-        <f>P25/$S65</f>
+        <f>P24/$S64</f>
         <v/>
       </c>
       <c r="Q65" s="13">
-        <f>Q25/$S65</f>
+        <f>Q24/$S64</f>
         <v/>
       </c>
       <c r="R65" s="15" t="n"/>
       <c r="S65" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V65" s="24" t="n"/>
       <c r="W65" s="12" t="n"/>
@@ -4178,60 +4112,60 @@
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="B66" s="11">
-        <f>B26</f>
+        <f>B25</f>
         <v/>
       </c>
       <c r="C66" s="13">
-        <f>C26/$S66</f>
+        <f>C25/$S65</f>
         <v/>
       </c>
       <c r="D66" s="13">
-        <f>D26/$S66</f>
+        <f>D25/$S65</f>
         <v/>
       </c>
       <c r="E66" s="13">
-        <f>E26/$S66</f>
+        <f>E25/$S65</f>
         <v/>
       </c>
       <c r="G66" s="13">
-        <f>G26/$S66</f>
+        <f>G25/$S65</f>
         <v/>
       </c>
       <c r="H66" s="13">
-        <f>H26/$S66</f>
+        <f>H25/$S65</f>
         <v/>
       </c>
       <c r="I66" s="13">
-        <f>I26/$S66</f>
+        <f>I25/$S65</f>
         <v/>
       </c>
       <c r="K66" s="13">
-        <f>K26/$S66</f>
+        <f>K25/$S65</f>
         <v/>
       </c>
       <c r="L66" s="13">
-        <f>L26/$S66</f>
+        <f>L25/$S65</f>
         <v/>
       </c>
       <c r="M66" s="13">
-        <f>M26/$S66</f>
+        <f>M25/$S65</f>
         <v/>
       </c>
       <c r="O66" s="13">
-        <f>O26/$S66</f>
+        <f>O25/$S65</f>
         <v/>
       </c>
       <c r="P66" s="13">
-        <f>P26/$S66</f>
+        <f>P25/$S65</f>
         <v/>
       </c>
       <c r="Q66" s="13">
-        <f>Q26/$S66</f>
+        <f>Q25/$S65</f>
         <v/>
       </c>
       <c r="R66" s="15" t="n"/>
       <c r="S66" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V66" s="24" t="n"/>
       <c r="W66" s="12" t="n"/>
@@ -4245,60 +4179,60 @@
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="B67" s="11">
-        <f>B27</f>
+        <f>B26</f>
         <v/>
       </c>
       <c r="C67" s="13">
-        <f>C27/$S67</f>
+        <f>C26/$S66</f>
         <v/>
       </c>
       <c r="D67" s="13">
-        <f>D27/$S67</f>
+        <f>D26/$S66</f>
         <v/>
       </c>
       <c r="E67" s="13">
-        <f>E27/$S67</f>
+        <f>E26/$S66</f>
         <v/>
       </c>
       <c r="G67" s="13">
-        <f>G27/$S67</f>
+        <f>G26/$S66</f>
         <v/>
       </c>
       <c r="H67" s="13">
-        <f>H27/$S67</f>
+        <f>H26/$S66</f>
         <v/>
       </c>
       <c r="I67" s="13">
-        <f>I27/$S67</f>
+        <f>I26/$S66</f>
         <v/>
       </c>
       <c r="K67" s="13">
-        <f>K27/$S67</f>
+        <f>K26/$S66</f>
         <v/>
       </c>
       <c r="L67" s="13">
-        <f>L27/$S67</f>
+        <f>L26/$S66</f>
         <v/>
       </c>
       <c r="M67" s="13">
-        <f>M27/$S67</f>
+        <f>M26/$S66</f>
         <v/>
       </c>
       <c r="O67" s="13">
-        <f>O27/$S67</f>
+        <f>O26/$S66</f>
         <v/>
       </c>
       <c r="P67" s="13">
-        <f>P27/$S67</f>
+        <f>P26/$S66</f>
         <v/>
       </c>
       <c r="Q67" s="13">
-        <f>Q27/$S67</f>
+        <f>Q26/$S66</f>
         <v/>
       </c>
       <c r="R67" s="15" t="n"/>
       <c r="S67" s="27" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V67" s="24" t="n"/>
       <c r="W67" s="12" t="n"/>
@@ -4312,60 +4246,60 @@
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="B68" s="11">
-        <f>B28</f>
+        <f>B27</f>
         <v/>
       </c>
       <c r="C68" s="13">
-        <f>C28/$S68</f>
+        <f>C27/$S67</f>
         <v/>
       </c>
       <c r="D68" s="13">
-        <f>D28/$S68</f>
+        <f>D27/$S67</f>
         <v/>
       </c>
       <c r="E68" s="13">
-        <f>E28/$S68</f>
+        <f>E27/$S67</f>
         <v/>
       </c>
       <c r="G68" s="13">
-        <f>G28/$S68</f>
+        <f>G27/$S67</f>
         <v/>
       </c>
       <c r="H68" s="13">
-        <f>H28/$S68</f>
+        <f>H27/$S67</f>
         <v/>
       </c>
       <c r="I68" s="13">
-        <f>I28/$S68</f>
+        <f>I27/$S67</f>
         <v/>
       </c>
       <c r="K68" s="13">
-        <f>K28/$S68</f>
+        <f>K27/$S67</f>
         <v/>
       </c>
       <c r="L68" s="13">
-        <f>L28/$S68</f>
+        <f>L27/$S67</f>
         <v/>
       </c>
       <c r="M68" s="13">
-        <f>M28/$S68</f>
+        <f>M27/$S67</f>
         <v/>
       </c>
       <c r="O68" s="13">
-        <f>O28/$S68</f>
+        <f>O27/$S67</f>
         <v/>
       </c>
       <c r="P68" s="13">
-        <f>P28/$S68</f>
+        <f>P27/$S67</f>
         <v/>
       </c>
       <c r="Q68" s="13">
-        <f>Q28/$S68</f>
+        <f>Q27/$S67</f>
         <v/>
       </c>
       <c r="R68" s="15" t="n"/>
       <c r="S68" s="27" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="V68" s="24" t="n"/>
       <c r="W68" s="12" t="n"/>
@@ -4374,65 +4308,65 @@
       <c r="Z68" s="12" t="n"/>
       <c r="AA68" s="12" t="n"/>
       <c r="AB68" s="14" t="n"/>
-      <c r="AE68" s="16" t="n"/>
+      <c r="AE68" s="12" t="n"/>
       <c r="AF68" s="14" t="n"/>
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="B69" s="11">
-        <f>B29</f>
+        <f>B28</f>
         <v/>
       </c>
       <c r="C69" s="13">
-        <f>C29/$S69</f>
+        <f>C28/$S68</f>
         <v/>
       </c>
       <c r="D69" s="13">
-        <f>D29/$S69</f>
+        <f>D28/$S68</f>
         <v/>
       </c>
       <c r="E69" s="13">
-        <f>E29/$S69</f>
+        <f>E28/$S68</f>
         <v/>
       </c>
       <c r="G69" s="13">
-        <f>G29/$S69</f>
+        <f>G28/$S68</f>
         <v/>
       </c>
       <c r="H69" s="13">
-        <f>H29/$S69</f>
+        <f>H28/$S68</f>
         <v/>
       </c>
       <c r="I69" s="13">
-        <f>I29/$S69</f>
+        <f>I28/$S68</f>
         <v/>
       </c>
       <c r="K69" s="13">
-        <f>K29/$S69</f>
+        <f>K28/$S68</f>
         <v/>
       </c>
       <c r="L69" s="13">
-        <f>L29/$S69</f>
+        <f>L28/$S68</f>
         <v/>
       </c>
       <c r="M69" s="13">
-        <f>M29/$S69</f>
+        <f>M28/$S68</f>
         <v/>
       </c>
       <c r="O69" s="13">
-        <f>O29/$S69</f>
+        <f>O28/$S68</f>
         <v/>
       </c>
       <c r="P69" s="13">
-        <f>P29/$S69</f>
+        <f>P28/$S68</f>
         <v/>
       </c>
       <c r="Q69" s="13">
-        <f>Q29/$S69</f>
+        <f>Q28/$S68</f>
         <v/>
       </c>
       <c r="R69" s="15" t="n"/>
       <c r="S69" s="27" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="V69" s="24" t="n"/>
       <c r="W69" s="12" t="n"/>
@@ -4446,60 +4380,60 @@
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="B70" s="11">
-        <f>B30</f>
+        <f>B29</f>
         <v/>
       </c>
       <c r="C70" s="13">
-        <f>C30/$S70</f>
+        <f>C29/$S69</f>
         <v/>
       </c>
       <c r="D70" s="13">
-        <f>D30/$S70</f>
+        <f>D29/$S69</f>
         <v/>
       </c>
       <c r="E70" s="13">
-        <f>E30/$S70</f>
+        <f>E29/$S69</f>
         <v/>
       </c>
       <c r="G70" s="13">
-        <f>G30/$S70</f>
+        <f>G29/$S69</f>
         <v/>
       </c>
       <c r="H70" s="13">
-        <f>H30/$S70</f>
+        <f>H29/$S69</f>
         <v/>
       </c>
       <c r="I70" s="13">
-        <f>I30/$S70</f>
+        <f>I29/$S69</f>
         <v/>
       </c>
       <c r="K70" s="13">
-        <f>K30/$S70</f>
+        <f>K29/$S69</f>
         <v/>
       </c>
       <c r="L70" s="13">
-        <f>L30/$S70</f>
+        <f>L29/$S69</f>
         <v/>
       </c>
       <c r="M70" s="13">
-        <f>M30/$S70</f>
+        <f>M29/$S69</f>
         <v/>
       </c>
       <c r="O70" s="13">
-        <f>O30/$S70</f>
+        <f>O29/$S69</f>
         <v/>
       </c>
       <c r="P70" s="13">
-        <f>P30/$S70</f>
+        <f>P29/$S69</f>
         <v/>
       </c>
       <c r="Q70" s="13">
-        <f>Q30/$S70</f>
+        <f>Q29/$S69</f>
         <v/>
       </c>
       <c r="R70" s="15" t="n"/>
       <c r="S70" s="27" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V70" s="24" t="n"/>
       <c r="W70" s="12" t="n"/>
@@ -4513,60 +4447,60 @@
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="B71" s="11">
-        <f>B31</f>
+        <f>B30</f>
         <v/>
       </c>
       <c r="C71" s="13">
-        <f>C31/$S71</f>
+        <f>C30/$S70</f>
         <v/>
       </c>
       <c r="D71" s="13">
-        <f>D31/$S71</f>
+        <f>D30/$S70</f>
         <v/>
       </c>
       <c r="E71" s="13">
-        <f>E31/$S71</f>
+        <f>E30/$S70</f>
         <v/>
       </c>
       <c r="G71" s="13">
-        <f>G31/$S71</f>
+        <f>G30/$S70</f>
         <v/>
       </c>
       <c r="H71" s="13">
-        <f>H31/$S71</f>
+        <f>H30/$S70</f>
         <v/>
       </c>
       <c r="I71" s="13">
-        <f>I31/$S71</f>
+        <f>I30/$S70</f>
         <v/>
       </c>
       <c r="K71" s="13">
-        <f>K31/$S71</f>
+        <f>K30/$S70</f>
         <v/>
       </c>
       <c r="L71" s="13">
-        <f>L31/$S71</f>
+        <f>L30/$S70</f>
         <v/>
       </c>
       <c r="M71" s="13">
-        <f>M31/$S71</f>
+        <f>M30/$S70</f>
         <v/>
       </c>
       <c r="O71" s="13">
-        <f>O31/$S71</f>
+        <f>O30/$S70</f>
         <v/>
       </c>
       <c r="P71" s="13">
-        <f>P31/$S71</f>
+        <f>P30/$S70</f>
         <v/>
       </c>
       <c r="Q71" s="13">
-        <f>Q31/$S71</f>
+        <f>Q30/$S70</f>
         <v/>
       </c>
       <c r="R71" s="15" t="n"/>
       <c r="S71" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V71" s="24" t="n"/>
       <c r="W71" s="12" t="n"/>
@@ -4580,60 +4514,60 @@
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="B72" s="11">
-        <f>B32</f>
+        <f>B31</f>
         <v/>
       </c>
       <c r="C72" s="13">
-        <f>C32/$S72</f>
+        <f>C31/$S71</f>
         <v/>
       </c>
       <c r="D72" s="13">
-        <f>D32/$S72</f>
+        <f>D31/$S71</f>
         <v/>
       </c>
       <c r="E72" s="13">
-        <f>E32/$S72</f>
+        <f>E31/$S71</f>
         <v/>
       </c>
       <c r="G72" s="13">
-        <f>G32/$S72</f>
+        <f>G31/$S71</f>
         <v/>
       </c>
       <c r="H72" s="13">
-        <f>H32/$S72</f>
+        <f>H31/$S71</f>
         <v/>
       </c>
       <c r="I72" s="13">
-        <f>I32/$S72</f>
+        <f>I31/$S71</f>
         <v/>
       </c>
       <c r="K72" s="13">
-        <f>K32/$S72</f>
+        <f>K31/$S71</f>
         <v/>
       </c>
       <c r="L72" s="13">
-        <f>L32/$S72</f>
+        <f>L31/$S71</f>
         <v/>
       </c>
       <c r="M72" s="13">
-        <f>M32/$S72</f>
+        <f>M31/$S71</f>
         <v/>
       </c>
       <c r="O72" s="13">
-        <f>O32/$S72</f>
+        <f>O31/$S71</f>
         <v/>
       </c>
       <c r="P72" s="13">
-        <f>P32/$S72</f>
+        <f>P31/$S71</f>
         <v/>
       </c>
       <c r="Q72" s="13">
-        <f>Q32/$S72</f>
+        <f>Q31/$S71</f>
         <v/>
       </c>
       <c r="R72" s="15" t="n"/>
       <c r="S72" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V72" s="24" t="n"/>
       <c r="W72" s="12" t="n"/>
@@ -4647,60 +4581,60 @@
     </row>
     <row r="73">
       <c r="B73" s="11">
-        <f>B33</f>
+        <f>B32</f>
         <v/>
       </c>
       <c r="C73" s="13">
-        <f>C33/$S73</f>
+        <f>C32/$S72</f>
         <v/>
       </c>
       <c r="D73" s="13">
-        <f>D33/$S73</f>
+        <f>D32/$S72</f>
         <v/>
       </c>
       <c r="E73" s="13">
-        <f>E33/$S73</f>
+        <f>E32/$S72</f>
         <v/>
       </c>
       <c r="G73" s="13">
-        <f>G33/$S73</f>
+        <f>G32/$S72</f>
         <v/>
       </c>
       <c r="H73" s="13">
-        <f>H33/$S73</f>
+        <f>H32/$S72</f>
         <v/>
       </c>
       <c r="I73" s="13">
-        <f>I33/$S73</f>
+        <f>I32/$S72</f>
         <v/>
       </c>
       <c r="K73" s="13">
-        <f>K33/$S73</f>
+        <f>K32/$S72</f>
         <v/>
       </c>
       <c r="L73" s="13">
-        <f>L33/$S73</f>
+        <f>L32/$S72</f>
         <v/>
       </c>
       <c r="M73" s="13">
-        <f>M33/$S73</f>
+        <f>M32/$S72</f>
         <v/>
       </c>
       <c r="O73" s="13">
-        <f>O33/$S73</f>
+        <f>O32/$S72</f>
         <v/>
       </c>
       <c r="P73" s="13">
-        <f>P33/$S73</f>
+        <f>P32/$S72</f>
         <v/>
       </c>
       <c r="Q73" s="13">
-        <f>Q33/$S73</f>
-        <v/>
-      </c>
-      <c r="R73" s="12" t="n"/>
+        <f>Q32/$S72</f>
+        <v/>
+      </c>
+      <c r="R73" s="15" t="n"/>
       <c r="S73" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V73" s="24" t="n"/>
       <c r="W73" s="12" t="n"/>
@@ -4714,60 +4648,60 @@
     </row>
     <row r="74">
       <c r="B74" s="11">
-        <f>B34</f>
+        <f>B33</f>
         <v/>
       </c>
       <c r="C74" s="13">
-        <f>C34/$S74</f>
+        <f>C33/$S73</f>
         <v/>
       </c>
       <c r="D74" s="13">
-        <f>D34/$S74</f>
+        <f>D33/$S73</f>
         <v/>
       </c>
       <c r="E74" s="13">
-        <f>E34/$S74</f>
+        <f>E33/$S73</f>
         <v/>
       </c>
       <c r="G74" s="13">
-        <f>G34/$S74</f>
+        <f>G33/$S73</f>
         <v/>
       </c>
       <c r="H74" s="13">
-        <f>H34/$S74</f>
+        <f>H33/$S73</f>
         <v/>
       </c>
       <c r="I74" s="13">
-        <f>I34/$S74</f>
+        <f>I33/$S73</f>
         <v/>
       </c>
       <c r="K74" s="13">
-        <f>K34/$S74</f>
+        <f>K33/$S73</f>
         <v/>
       </c>
       <c r="L74" s="13">
-        <f>L34/$S74</f>
+        <f>L33/$S73</f>
         <v/>
       </c>
       <c r="M74" s="13">
-        <f>M34/$S74</f>
+        <f>M33/$S73</f>
         <v/>
       </c>
       <c r="O74" s="13">
-        <f>O34/$S74</f>
+        <f>O33/$S73</f>
         <v/>
       </c>
       <c r="P74" s="13">
-        <f>P34/$S74</f>
+        <f>P33/$S73</f>
         <v/>
       </c>
       <c r="Q74" s="13">
-        <f>Q34/$S74</f>
+        <f>Q33/$S73</f>
         <v/>
       </c>
       <c r="R74" s="12" t="n"/>
       <c r="S74" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V74" s="24" t="n"/>
       <c r="W74" s="12" t="n"/>
@@ -4781,55 +4715,55 @@
     </row>
     <row r="75">
       <c r="B75" s="11">
-        <f>B35</f>
+        <f>B34</f>
         <v/>
       </c>
       <c r="C75" s="13">
-        <f>C35/$S75</f>
+        <f>C34/$S74</f>
         <v/>
       </c>
       <c r="D75" s="13">
-        <f>D35/$S75</f>
+        <f>D34/$S74</f>
         <v/>
       </c>
       <c r="E75" s="13">
-        <f>E35/$S75</f>
+        <f>E34/$S74</f>
         <v/>
       </c>
       <c r="G75" s="13">
-        <f>G35/$S75</f>
+        <f>G34/$S74</f>
         <v/>
       </c>
       <c r="H75" s="13">
-        <f>H35/$S75</f>
+        <f>H34/$S74</f>
         <v/>
       </c>
       <c r="I75" s="13">
-        <f>I35/$S75</f>
+        <f>I34/$S74</f>
         <v/>
       </c>
       <c r="K75" s="13">
-        <f>K35/$S75</f>
+        <f>K34/$S74</f>
         <v/>
       </c>
       <c r="L75" s="13">
-        <f>L35/$S75</f>
+        <f>L34/$S74</f>
         <v/>
       </c>
       <c r="M75" s="13">
-        <f>M35/$S75</f>
+        <f>M34/$S74</f>
         <v/>
       </c>
       <c r="O75" s="13">
-        <f>O35/$S75</f>
+        <f>O34/$S74</f>
         <v/>
       </c>
       <c r="P75" s="13">
-        <f>P35/$S75</f>
+        <f>P34/$S74</f>
         <v/>
       </c>
       <c r="Q75" s="13">
-        <f>Q35/$S75</f>
+        <f>Q34/$S74</f>
         <v/>
       </c>
       <c r="R75" s="12" t="n"/>
@@ -4848,60 +4782,60 @@
     </row>
     <row r="76">
       <c r="B76" s="11">
-        <f>B36</f>
+        <f>B35</f>
         <v/>
       </c>
       <c r="C76" s="13">
-        <f>C36/$S76</f>
+        <f>C35/$S75</f>
         <v/>
       </c>
       <c r="D76" s="13">
-        <f>D36/$S76</f>
+        <f>D35/$S75</f>
         <v/>
       </c>
       <c r="E76" s="13">
-        <f>E36/$S76</f>
+        <f>E35/$S75</f>
         <v/>
       </c>
       <c r="G76" s="13">
-        <f>G36/$S76</f>
+        <f>G35/$S75</f>
         <v/>
       </c>
       <c r="H76" s="13">
-        <f>H36/$S76</f>
+        <f>H35/$S75</f>
         <v/>
       </c>
       <c r="I76" s="13">
-        <f>I36/$S76</f>
+        <f>I35/$S75</f>
         <v/>
       </c>
       <c r="K76" s="13">
-        <f>K36/$S76</f>
+        <f>K35/$S75</f>
         <v/>
       </c>
       <c r="L76" s="13">
-        <f>L36/$S76</f>
+        <f>L35/$S75</f>
         <v/>
       </c>
       <c r="M76" s="13">
-        <f>M36/$S76</f>
+        <f>M35/$S75</f>
         <v/>
       </c>
       <c r="O76" s="13">
-        <f>O36/$S76</f>
+        <f>O35/$S75</f>
         <v/>
       </c>
       <c r="P76" s="13">
-        <f>P36/$S76</f>
+        <f>P35/$S75</f>
         <v/>
       </c>
       <c r="Q76" s="13">
-        <f>Q36/$S76</f>
+        <f>Q35/$S75</f>
         <v/>
       </c>
       <c r="R76" s="12" t="n"/>
       <c r="S76" s="27" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="V76" s="24" t="n"/>
       <c r="W76" s="12" t="n"/>
@@ -4915,60 +4849,60 @@
     </row>
     <row r="77">
       <c r="B77" s="11">
-        <f>B37</f>
+        <f>B36</f>
         <v/>
       </c>
       <c r="C77" s="13">
-        <f>C37/$S77</f>
+        <f>C36/$S76</f>
         <v/>
       </c>
       <c r="D77" s="13">
-        <f>D37/$S77</f>
+        <f>D36/$S76</f>
         <v/>
       </c>
       <c r="E77" s="13">
-        <f>E37/$S77</f>
+        <f>E36/$S76</f>
         <v/>
       </c>
       <c r="G77" s="13">
-        <f>G37/$S77</f>
+        <f>G36/$S76</f>
         <v/>
       </c>
       <c r="H77" s="13">
-        <f>H37/$S77</f>
+        <f>H36/$S76</f>
         <v/>
       </c>
       <c r="I77" s="13">
-        <f>I37/$S77</f>
+        <f>I36/$S76</f>
         <v/>
       </c>
       <c r="K77" s="13">
-        <f>K37/$S77</f>
+        <f>K36/$S76</f>
         <v/>
       </c>
       <c r="L77" s="13">
-        <f>L37/$S77</f>
+        <f>L36/$S76</f>
         <v/>
       </c>
       <c r="M77" s="13">
-        <f>M37/$S77</f>
+        <f>M36/$S76</f>
         <v/>
       </c>
       <c r="O77" s="13">
-        <f>O37/$S77</f>
+        <f>O36/$S76</f>
         <v/>
       </c>
       <c r="P77" s="13">
-        <f>P37/$S77</f>
+        <f>P36/$S76</f>
         <v/>
       </c>
       <c r="Q77" s="13">
-        <f>Q37/$S77</f>
+        <f>Q36/$S76</f>
         <v/>
       </c>
       <c r="R77" s="12" t="n"/>
       <c r="S77" s="27" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="V77" s="24" t="n"/>
       <c r="W77" s="12" t="n"/>
@@ -4982,60 +4916,60 @@
     </row>
     <row r="78">
       <c r="B78" s="11">
-        <f>B38</f>
+        <f>B37</f>
         <v/>
       </c>
       <c r="C78" s="13">
-        <f>C38/$S78</f>
+        <f>C37/$S77</f>
         <v/>
       </c>
       <c r="D78" s="13">
-        <f>D38/$S78</f>
+        <f>D37/$S77</f>
         <v/>
       </c>
       <c r="E78" s="13">
-        <f>E38/$S78</f>
+        <f>E37/$S77</f>
         <v/>
       </c>
       <c r="G78" s="13">
-        <f>G38/$S78</f>
+        <f>G37/$S77</f>
         <v/>
       </c>
       <c r="H78" s="13">
-        <f>H38/$S78</f>
+        <f>H37/$S77</f>
         <v/>
       </c>
       <c r="I78" s="13">
-        <f>I38/$S78</f>
+        <f>I37/$S77</f>
         <v/>
       </c>
       <c r="K78" s="13">
-        <f>K38/$S78</f>
+        <f>K37/$S77</f>
         <v/>
       </c>
       <c r="L78" s="13">
-        <f>L38/$S78</f>
+        <f>L37/$S77</f>
         <v/>
       </c>
       <c r="M78" s="13">
-        <f>M38/$S78</f>
+        <f>M37/$S77</f>
         <v/>
       </c>
       <c r="O78" s="13">
-        <f>O38/$S78</f>
+        <f>O37/$S77</f>
         <v/>
       </c>
       <c r="P78" s="13">
-        <f>P38/$S78</f>
+        <f>P37/$S77</f>
         <v/>
       </c>
       <c r="Q78" s="13">
-        <f>Q38/$S78</f>
+        <f>Q37/$S77</f>
         <v/>
       </c>
       <c r="R78" s="12" t="n"/>
       <c r="S78" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V78" s="24" t="n"/>
       <c r="W78" s="12" t="n"/>
@@ -5049,60 +4983,60 @@
     </row>
     <row r="79">
       <c r="B79" s="11">
-        <f>B39</f>
+        <f>B38</f>
         <v/>
       </c>
       <c r="C79" s="13">
-        <f>C39/$S79</f>
+        <f>C38/$S78</f>
         <v/>
       </c>
       <c r="D79" s="13">
-        <f>D39/$S79</f>
+        <f>D38/$S78</f>
         <v/>
       </c>
       <c r="E79" s="13">
-        <f>E39/$S79</f>
+        <f>E38/$S78</f>
         <v/>
       </c>
       <c r="G79" s="13">
-        <f>G39/$S79</f>
+        <f>G38/$S78</f>
         <v/>
       </c>
       <c r="H79" s="13">
-        <f>H39/$S79</f>
+        <f>H38/$S78</f>
         <v/>
       </c>
       <c r="I79" s="13">
-        <f>I39/$S79</f>
+        <f>I38/$S78</f>
         <v/>
       </c>
       <c r="K79" s="13">
-        <f>K39/$S79</f>
+        <f>K38/$S78</f>
         <v/>
       </c>
       <c r="L79" s="13">
-        <f>L39/$S79</f>
+        <f>L38/$S78</f>
         <v/>
       </c>
       <c r="M79" s="13">
-        <f>M39/$S79</f>
+        <f>M38/$S78</f>
         <v/>
       </c>
       <c r="O79" s="13">
-        <f>O39/$S79</f>
+        <f>O38/$S78</f>
         <v/>
       </c>
       <c r="P79" s="13">
-        <f>P39/$S79</f>
+        <f>P38/$S78</f>
         <v/>
       </c>
       <c r="Q79" s="13">
-        <f>Q39/$S79</f>
+        <f>Q38/$S78</f>
         <v/>
       </c>
       <c r="R79" s="12" t="n"/>
       <c r="S79" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V79" s="24" t="n"/>
       <c r="W79" s="12" t="n"/>
@@ -5116,60 +5050,60 @@
     </row>
     <row r="80">
       <c r="B80" s="11">
-        <f>B40</f>
+        <f>B39</f>
         <v/>
       </c>
       <c r="C80" s="13">
-        <f>C40/$S80</f>
+        <f>C39/$S79</f>
         <v/>
       </c>
       <c r="D80" s="13">
-        <f>D40/$S80</f>
+        <f>D39/$S79</f>
         <v/>
       </c>
       <c r="E80" s="13">
-        <f>E40/$S80</f>
+        <f>E39/$S79</f>
         <v/>
       </c>
       <c r="G80" s="13">
-        <f>G40/$S80</f>
+        <f>G39/$S79</f>
         <v/>
       </c>
       <c r="H80" s="13">
-        <f>H40/$S80</f>
+        <f>H39/$S79</f>
         <v/>
       </c>
       <c r="I80" s="13">
-        <f>I40/$S80</f>
+        <f>I39/$S79</f>
         <v/>
       </c>
       <c r="K80" s="13">
-        <f>K40/$S80</f>
+        <f>K39/$S79</f>
         <v/>
       </c>
       <c r="L80" s="13">
-        <f>L40/$S80</f>
+        <f>L39/$S79</f>
         <v/>
       </c>
       <c r="M80" s="13">
-        <f>M40/$S80</f>
+        <f>M39/$S79</f>
         <v/>
       </c>
       <c r="O80" s="13">
-        <f>O40/$S80</f>
+        <f>O39/$S79</f>
         <v/>
       </c>
       <c r="P80" s="13">
-        <f>P40/$S80</f>
+        <f>P39/$S79</f>
         <v/>
       </c>
       <c r="Q80" s="13">
-        <f>Q40/$S80</f>
+        <f>Q39/$S79</f>
         <v/>
       </c>
       <c r="R80" s="12" t="n"/>
       <c r="S80" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V80" s="24" t="n"/>
       <c r="W80" s="12" t="n"/>
@@ -5183,55 +5117,55 @@
     </row>
     <row r="81">
       <c r="B81" s="11">
-        <f>B41</f>
+        <f>B40</f>
         <v/>
       </c>
       <c r="C81" s="13">
-        <f>C41/$S81</f>
+        <f>C40/$S80</f>
         <v/>
       </c>
       <c r="D81" s="13">
-        <f>D41/$S81</f>
+        <f>D40/$S80</f>
         <v/>
       </c>
       <c r="E81" s="13">
-        <f>E41/$S81</f>
+        <f>E40/$S80</f>
         <v/>
       </c>
       <c r="G81" s="13">
-        <f>G41/$S81</f>
+        <f>G40/$S80</f>
         <v/>
       </c>
       <c r="H81" s="13">
-        <f>H41/$S81</f>
+        <f>H40/$S80</f>
         <v/>
       </c>
       <c r="I81" s="13">
-        <f>I41/$S81</f>
+        <f>I40/$S80</f>
         <v/>
       </c>
       <c r="K81" s="13">
-        <f>K41/$S81</f>
+        <f>K40/$S80</f>
         <v/>
       </c>
       <c r="L81" s="13">
-        <f>L41/$S81</f>
+        <f>L40/$S80</f>
         <v/>
       </c>
       <c r="M81" s="13">
-        <f>M41/$S81</f>
+        <f>M40/$S80</f>
         <v/>
       </c>
       <c r="O81" s="13">
-        <f>O41/$S81</f>
+        <f>O40/$S80</f>
         <v/>
       </c>
       <c r="P81" s="13">
-        <f>P41/$S81</f>
+        <f>P40/$S80</f>
         <v/>
       </c>
       <c r="Q81" s="13">
-        <f>Q41/$S81</f>
+        <f>Q40/$S80</f>
         <v/>
       </c>
       <c r="R81" s="12" t="n"/>
@@ -5250,60 +5184,60 @@
     </row>
     <row r="82">
       <c r="B82" s="11">
-        <f>B42</f>
+        <f>B41</f>
         <v/>
       </c>
       <c r="C82" s="13">
-        <f>C42/$S82</f>
+        <f>C41/$S81</f>
         <v/>
       </c>
       <c r="D82" s="13">
-        <f>D42/$S82</f>
+        <f>D41/$S81</f>
         <v/>
       </c>
       <c r="E82" s="13">
-        <f>E42/$S82</f>
+        <f>E41/$S81</f>
         <v/>
       </c>
       <c r="G82" s="13">
-        <f>G42/$S82</f>
+        <f>G41/$S81</f>
         <v/>
       </c>
       <c r="H82" s="13">
-        <f>H42/$S82</f>
+        <f>H41/$S81</f>
         <v/>
       </c>
       <c r="I82" s="13">
-        <f>I42/$S82</f>
+        <f>I41/$S81</f>
         <v/>
       </c>
       <c r="K82" s="13">
-        <f>K42/$S82</f>
+        <f>K41/$S81</f>
         <v/>
       </c>
       <c r="L82" s="13">
-        <f>L42/$S82</f>
+        <f>L41/$S81</f>
         <v/>
       </c>
       <c r="M82" s="13">
-        <f>M42/$S82</f>
+        <f>M41/$S81</f>
         <v/>
       </c>
       <c r="O82" s="13">
-        <f>O42/$S82</f>
+        <f>O41/$S81</f>
         <v/>
       </c>
       <c r="P82" s="13">
-        <f>P42/$S82</f>
+        <f>P41/$S81</f>
         <v/>
       </c>
       <c r="Q82" s="13">
-        <f>Q42/$S82</f>
+        <f>Q41/$S81</f>
         <v/>
       </c>
       <c r="R82" s="12" t="n"/>
       <c r="S82" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V82" s="24" t="n"/>
       <c r="W82" s="12" t="n"/>
@@ -5317,60 +5251,60 @@
     </row>
     <row r="83">
       <c r="B83" s="11">
-        <f>B43</f>
+        <f>B42</f>
         <v/>
       </c>
       <c r="C83" s="13">
-        <f>C43/$S83</f>
+        <f>C42/$S82</f>
         <v/>
       </c>
       <c r="D83" s="13">
-        <f>D43/$S83</f>
+        <f>D42/$S82</f>
         <v/>
       </c>
       <c r="E83" s="13">
-        <f>E43/$S83</f>
+        <f>E42/$S82</f>
         <v/>
       </c>
       <c r="G83" s="13">
-        <f>G43/$S83</f>
+        <f>G42/$S82</f>
         <v/>
       </c>
       <c r="H83" s="13">
-        <f>H43/$S83</f>
+        <f>H42/$S82</f>
         <v/>
       </c>
       <c r="I83" s="13">
-        <f>I43/$S83</f>
+        <f>I42/$S82</f>
         <v/>
       </c>
       <c r="K83" s="13">
-        <f>K43/$S83</f>
+        <f>K42/$S82</f>
         <v/>
       </c>
       <c r="L83" s="13">
-        <f>L43/$S83</f>
+        <f>L42/$S82</f>
         <v/>
       </c>
       <c r="M83" s="13">
-        <f>M43/$S83</f>
+        <f>M42/$S82</f>
         <v/>
       </c>
       <c r="O83" s="13">
-        <f>O43/$S83</f>
+        <f>O42/$S82</f>
         <v/>
       </c>
       <c r="P83" s="13">
-        <f>P43/$S83</f>
+        <f>P42/$S82</f>
         <v/>
       </c>
       <c r="Q83" s="13">
-        <f>Q43/$S83</f>
+        <f>Q42/$S82</f>
         <v/>
       </c>
       <c r="R83" s="12" t="n"/>
       <c r="S83" s="27" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V83" s="24" t="n"/>
       <c r="W83" s="12" t="n"/>
@@ -5384,60 +5318,60 @@
     </row>
     <row r="84">
       <c r="B84" s="11">
-        <f>B44</f>
+        <f>B43</f>
         <v/>
       </c>
       <c r="C84" s="13">
-        <f>C44/$S84</f>
+        <f>C43/$S83</f>
         <v/>
       </c>
       <c r="D84" s="13">
-        <f>D44/$S84</f>
+        <f>D43/$S83</f>
         <v/>
       </c>
       <c r="E84" s="13">
-        <f>E44/$S84</f>
+        <f>E43/$S83</f>
         <v/>
       </c>
       <c r="G84" s="13">
-        <f>G44/$S84</f>
+        <f>G43/$S83</f>
         <v/>
       </c>
       <c r="H84" s="13">
-        <f>H44/$S84</f>
+        <f>H43/$S83</f>
         <v/>
       </c>
       <c r="I84" s="13">
-        <f>I44/$S84</f>
+        <f>I43/$S83</f>
         <v/>
       </c>
       <c r="K84" s="13">
-        <f>K44/$S84</f>
+        <f>K43/$S83</f>
         <v/>
       </c>
       <c r="L84" s="13">
-        <f>L44/$S84</f>
+        <f>L43/$S83</f>
         <v/>
       </c>
       <c r="M84" s="13">
-        <f>M44/$S84</f>
+        <f>M43/$S83</f>
         <v/>
       </c>
       <c r="O84" s="13">
-        <f>O44/$S84</f>
+        <f>O43/$S83</f>
         <v/>
       </c>
       <c r="P84" s="13">
-        <f>P44/$S84</f>
+        <f>P43/$S83</f>
         <v/>
       </c>
       <c r="Q84" s="13">
-        <f>Q44/$S84</f>
+        <f>Q43/$S83</f>
         <v/>
       </c>
       <c r="R84" s="12" t="n"/>
       <c r="S84" s="27" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="V84" s="24" t="n"/>
       <c r="W84" s="12" t="n"/>
@@ -5451,120 +5385,126 @@
     </row>
     <row r="85">
       <c r="B85" s="11">
-        <f>B45</f>
+        <f>B44</f>
         <v/>
       </c>
       <c r="C85" s="13">
-        <f>C45/$S85</f>
+        <f>C44/$S84</f>
         <v/>
       </c>
       <c r="D85" s="13">
-        <f>D45/$S85</f>
+        <f>D44/$S84</f>
         <v/>
       </c>
       <c r="E85" s="13">
-        <f>E45/$S85</f>
+        <f>E44/$S84</f>
         <v/>
       </c>
       <c r="G85" s="13">
-        <f>G45/$S85</f>
+        <f>G44/$S84</f>
         <v/>
       </c>
       <c r="H85" s="13">
-        <f>H45/$S85</f>
+        <f>H44/$S84</f>
         <v/>
       </c>
       <c r="I85" s="13">
-        <f>I45/$S85</f>
+        <f>I44/$S84</f>
         <v/>
       </c>
       <c r="K85" s="13">
-        <f>K45/$S85</f>
+        <f>K44/$S84</f>
         <v/>
       </c>
       <c r="L85" s="13">
-        <f>L45/$S85</f>
+        <f>L44/$S84</f>
         <v/>
       </c>
       <c r="M85" s="13">
-        <f>M45/$S85</f>
+        <f>M44/$S84</f>
         <v/>
       </c>
       <c r="O85" s="13">
-        <f>O45/$S85</f>
+        <f>O44/$S84</f>
         <v/>
       </c>
       <c r="P85" s="13">
-        <f>P45/$S85</f>
+        <f>P44/$S84</f>
         <v/>
       </c>
       <c r="Q85" s="13">
-        <f>Q45/$S85</f>
-        <v/>
-      </c>
+        <f>Q44/$S84</f>
+        <v/>
+      </c>
+      <c r="R85" s="12" t="n"/>
       <c r="S85" s="27" t="n">
         <v>21</v>
       </c>
+      <c r="V85" s="24" t="n"/>
       <c r="W85" s="12" t="n"/>
       <c r="X85" s="12" t="n"/>
       <c r="Y85" s="12" t="n"/>
       <c r="Z85" s="12" t="n"/>
+      <c r="AA85" s="12" t="n"/>
+      <c r="AB85" s="14" t="n"/>
+      <c r="AE85" s="16" t="n"/>
+      <c r="AF85" s="14" t="n"/>
     </row>
     <row r="86">
       <c r="B86" s="11">
-        <f>B46</f>
+        <f>B45</f>
         <v/>
       </c>
       <c r="C86" s="13">
-        <f>C46/$S86</f>
+        <f>C45/$S85</f>
         <v/>
       </c>
       <c r="D86" s="13">
-        <f>D46/$S86</f>
+        <f>D45/$S85</f>
         <v/>
       </c>
       <c r="E86" s="13">
-        <f>E46/$S86</f>
+        <f>E45/$S85</f>
         <v/>
       </c>
       <c r="G86" s="13">
-        <f>G46/$S86</f>
+        <f>G45/$S85</f>
         <v/>
       </c>
       <c r="H86" s="13">
-        <f>H46/$S86</f>
+        <f>H45/$S85</f>
         <v/>
       </c>
       <c r="I86" s="13">
-        <f>I46/$S86</f>
+        <f>I45/$S85</f>
         <v/>
       </c>
       <c r="K86" s="13">
-        <f>K46/$S86</f>
+        <f>K45/$S85</f>
         <v/>
       </c>
       <c r="L86" s="13">
-        <f>L46/$S86</f>
+        <f>L45/$S85</f>
         <v/>
       </c>
       <c r="M86" s="13">
-        <f>M46/$S86</f>
+        <f>M45/$S85</f>
         <v/>
       </c>
       <c r="O86" s="13">
-        <f>O46/$S86</f>
+        <f>O45/$S85</f>
         <v/>
       </c>
       <c r="P86" s="13">
-        <f>P46/$S86</f>
+        <f>P45/$S85</f>
         <v/>
       </c>
       <c r="Q86" s="13">
-        <f>Q46/$S86</f>
+        <f>Q45/$S85</f>
         <v/>
       </c>
       <c r="S86" s="27" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W86" s="12" t="n"/>
       <c r="X86" s="12" t="n"/>
@@ -5573,248 +5513,294 @@
     </row>
     <row r="87">
       <c r="B87" s="11">
-        <f>B47</f>
+        <f>B46</f>
         <v/>
       </c>
       <c r="C87" s="13">
-        <f>C47/$S87</f>
+        <f>C46/$S86</f>
         <v/>
       </c>
       <c r="D87" s="13">
-        <f>D47/$S87</f>
+        <f>D46/$S86</f>
         <v/>
       </c>
       <c r="E87" s="13">
-        <f>E47/$S87</f>
+        <f>E46/$S86</f>
         <v/>
       </c>
       <c r="G87" s="13">
-        <f>G47/$S87</f>
+        <f>G46/$S86</f>
         <v/>
       </c>
       <c r="H87" s="13">
-        <f>H47/$S87</f>
+        <f>H46/$S86</f>
         <v/>
       </c>
       <c r="I87" s="13">
-        <f>I47/$S87</f>
+        <f>I46/$S86</f>
         <v/>
       </c>
       <c r="K87" s="13">
-        <f>K47/$S87</f>
+        <f>K46/$S86</f>
         <v/>
       </c>
       <c r="L87" s="13">
-        <f>L47/$S87</f>
+        <f>L46/$S86</f>
         <v/>
       </c>
       <c r="M87" s="13">
-        <f>M47/$S87</f>
+        <f>M46/$S86</f>
         <v/>
       </c>
       <c r="O87" s="13">
-        <f>O47/$S87</f>
+        <f>O46/$S86</f>
         <v/>
       </c>
       <c r="P87" s="13">
-        <f>P47/$S87</f>
+        <f>P46/$S86</f>
         <v/>
       </c>
       <c r="Q87" s="13">
-        <f>Q47/$S87</f>
+        <f>Q46/$S86</f>
         <v/>
       </c>
       <c r="S87" s="27" t="n">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="W87" s="12" t="n"/>
+      <c r="X87" s="12" t="n"/>
+      <c r="Y87" s="12" t="n"/>
+      <c r="Z87" s="12" t="n"/>
     </row>
     <row r="88">
       <c r="B88" s="11">
-        <f>B48</f>
+        <f>B47</f>
         <v/>
       </c>
       <c r="C88" s="13">
-        <f>C48/$S88</f>
+        <f>C47/$S87</f>
         <v/>
       </c>
       <c r="D88" s="13">
-        <f>D48/$S88</f>
+        <f>D47/$S87</f>
         <v/>
       </c>
       <c r="E88" s="13">
-        <f>E48/$S88</f>
+        <f>E47/$S87</f>
         <v/>
       </c>
       <c r="G88" s="13">
-        <f>G48/$S88</f>
+        <f>G47/$S87</f>
         <v/>
       </c>
       <c r="H88" s="13">
-        <f>H48/$S88</f>
+        <f>H47/$S87</f>
         <v/>
       </c>
       <c r="I88" s="13">
-        <f>I48/$S88</f>
+        <f>I47/$S87</f>
         <v/>
       </c>
       <c r="K88" s="13">
-        <f>K48/$S88</f>
+        <f>K47/$S87</f>
         <v/>
       </c>
       <c r="L88" s="13">
-        <f>L48/$S88</f>
+        <f>L47/$S87</f>
         <v/>
       </c>
       <c r="M88" s="13">
-        <f>M48/$S88</f>
+        <f>M47/$S87</f>
         <v/>
       </c>
       <c r="O88" s="13">
-        <f>O48/$S88</f>
+        <f>O47/$S87</f>
         <v/>
       </c>
       <c r="P88" s="13">
-        <f>P48/$S88</f>
+        <f>P47/$S87</f>
         <v/>
       </c>
       <c r="Q88" s="13">
-        <f>Q48/$S88</f>
+        <f>Q47/$S87</f>
         <v/>
       </c>
       <c r="S88" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" s="11">
-        <f>B49</f>
+        <f>B48</f>
         <v/>
       </c>
       <c r="C89" s="13">
-        <f>C49/$S89</f>
+        <f>C48/$S88</f>
         <v/>
       </c>
       <c r="D89" s="13">
-        <f>D49/$S89</f>
+        <f>D48/$S88</f>
         <v/>
       </c>
       <c r="E89" s="13">
-        <f>E49/$S89</f>
+        <f>E48/$S88</f>
         <v/>
       </c>
       <c r="G89" s="13">
-        <f>G49/$S89</f>
+        <f>G48/$S88</f>
         <v/>
       </c>
       <c r="H89" s="13">
-        <f>H49/$S89</f>
+        <f>H48/$S88</f>
         <v/>
       </c>
       <c r="I89" s="13">
-        <f>I49/$S89</f>
+        <f>I48/$S88</f>
         <v/>
       </c>
       <c r="K89" s="13">
-        <f>K49/$S89</f>
+        <f>K48/$S88</f>
         <v/>
       </c>
       <c r="L89" s="13">
-        <f>L49/$S89</f>
+        <f>L48/$S88</f>
         <v/>
       </c>
       <c r="M89" s="13">
-        <f>M49/$S89</f>
+        <f>M48/$S88</f>
         <v/>
       </c>
       <c r="O89" s="13">
-        <f>O49/$S89</f>
+        <f>O48/$S88</f>
         <v/>
       </c>
       <c r="P89" s="13">
-        <f>P49/$S89</f>
+        <f>P48/$S88</f>
         <v/>
       </c>
       <c r="Q89" s="13">
-        <f>Q49/$S89</f>
+        <f>Q48/$S88</f>
         <v/>
       </c>
       <c r="S89" s="27" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" s="11">
+        <f>B49</f>
+        <v/>
+      </c>
+      <c r="C90" s="13">
+        <f>C49/$S89</f>
+        <v/>
+      </c>
+      <c r="D90" s="13">
+        <f>D49/$S89</f>
+        <v/>
+      </c>
+      <c r="E90" s="13">
+        <f>E49/$S89</f>
+        <v/>
+      </c>
+      <c r="G90" s="13">
+        <f>G49/$S89</f>
+        <v/>
+      </c>
+      <c r="H90" s="13">
+        <f>H49/$S89</f>
+        <v/>
+      </c>
+      <c r="I90" s="13">
+        <f>I49/$S89</f>
+        <v/>
+      </c>
+      <c r="K90" s="13">
+        <f>K49/$S89</f>
+        <v/>
+      </c>
+      <c r="L90" s="13">
+        <f>L49/$S89</f>
+        <v/>
+      </c>
+      <c r="M90" s="13">
+        <f>M49/$S89</f>
+        <v/>
+      </c>
+      <c r="O90" s="13">
+        <f>O49/$S89</f>
+        <v/>
+      </c>
+      <c r="P90" s="13">
+        <f>P49/$S89</f>
+        <v/>
+      </c>
+      <c r="Q90" s="13">
+        <f>Q49/$S89</f>
+        <v/>
+      </c>
+      <c r="S90" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" s="11">
         <f>B50</f>
         <v/>
       </c>
-      <c r="C90" s="13">
+      <c r="C91" s="13">
         <f>C50/$S90</f>
         <v/>
       </c>
-      <c r="D90" s="13">
+      <c r="D91" s="13">
         <f>D50/$S90</f>
         <v/>
       </c>
-      <c r="E90" s="13">
+      <c r="E91" s="13">
         <f>E50/$S90</f>
         <v/>
       </c>
-      <c r="G90" s="13">
+      <c r="G91" s="13">
         <f>G50/$S90</f>
         <v/>
       </c>
-      <c r="H90" s="13">
+      <c r="H91" s="13">
         <f>H50/$S90</f>
         <v/>
       </c>
-      <c r="I90" s="13">
+      <c r="I91" s="13">
         <f>I50/$S90</f>
         <v/>
       </c>
-      <c r="K90" s="13">
+      <c r="K91" s="13">
         <f>K50/$S90</f>
         <v/>
       </c>
-      <c r="L90" s="13">
+      <c r="L91" s="13">
         <f>L50/$S90</f>
         <v/>
       </c>
-      <c r="M90" s="13">
+      <c r="M91" s="13">
         <f>M50/$S90</f>
         <v/>
       </c>
-      <c r="O90" s="13">
+      <c r="O91" s="13">
         <f>O50/$S90</f>
         <v/>
       </c>
-      <c r="P90" s="13">
+      <c r="P91" s="13">
         <f>P50/$S90</f>
         <v/>
       </c>
-      <c r="Q90" s="13">
+      <c r="Q91" s="13">
         <f>Q50/$S90</f>
         <v/>
       </c>
-      <c r="S90" s="27" t="n">
+      <c r="S91" s="27" t="n">
         <v>20</v>
       </c>
-      <c r="T90" s="12" t="n"/>
-      <c r="U90" s="68" t="n"/>
-    </row>
-    <row r="91">
-      <c r="B91" s="25" t="n"/>
-      <c r="C91" s="12" t="n"/>
-      <c r="D91" s="14" t="n"/>
-      <c r="E91" s="12" t="n"/>
-      <c r="G91" s="12" t="n"/>
-      <c r="H91" s="14" t="n"/>
-      <c r="I91" s="12" t="n"/>
-      <c r="K91" s="14" t="n"/>
-      <c r="L91" s="14" t="n"/>
-      <c r="M91" s="12" t="n"/>
-      <c r="O91" s="12" t="n"/>
-      <c r="P91" s="12" t="n"/>
-      <c r="Q91" s="12" t="n"/>
+      <c r="T91" s="12" t="n"/>
+      <c r="U91" s="68" t="n"/>
     </row>
     <row r="92">
       <c r="B92" s="25" t="n"/>
@@ -6042,14 +6028,15 @@
       <c r="Q106" s="12" t="n"/>
     </row>
     <row r="107">
+      <c r="B107" s="25" t="n"/>
       <c r="C107" s="12" t="n"/>
-      <c r="D107" s="12" t="n"/>
+      <c r="D107" s="14" t="n"/>
       <c r="E107" s="12" t="n"/>
       <c r="G107" s="12" t="n"/>
       <c r="H107" s="14" t="n"/>
       <c r="I107" s="12" t="n"/>
-      <c r="K107" s="12" t="n"/>
-      <c r="L107" s="12" t="n"/>
+      <c r="K107" s="14" t="n"/>
+      <c r="L107" s="14" t="n"/>
       <c r="M107" s="12" t="n"/>
       <c r="O107" s="12" t="n"/>
       <c r="P107" s="12" t="n"/>
@@ -6060,7 +6047,7 @@
       <c r="D108" s="12" t="n"/>
       <c r="E108" s="12" t="n"/>
       <c r="G108" s="12" t="n"/>
-      <c r="H108" s="12" t="n"/>
+      <c r="H108" s="14" t="n"/>
       <c r="I108" s="12" t="n"/>
       <c r="K108" s="12" t="n"/>
       <c r="L108" s="12" t="n"/>
@@ -6199,6 +6186,15 @@
       <c r="C118" s="12" t="n"/>
       <c r="D118" s="12" t="n"/>
       <c r="E118" s="12" t="n"/>
+      <c r="G118" s="12" t="n"/>
+      <c r="H118" s="12" t="n"/>
+      <c r="I118" s="12" t="n"/>
+      <c r="K118" s="12" t="n"/>
+      <c r="L118" s="12" t="n"/>
+      <c r="M118" s="12" t="n"/>
+      <c r="O118" s="12" t="n"/>
+      <c r="P118" s="12" t="n"/>
+      <c r="Q118" s="12" t="n"/>
     </row>
     <row r="119">
       <c r="C119" s="12" t="n"/>
@@ -6220,8 +6216,13 @@
       <c r="D122" s="12" t="n"/>
       <c r="E122" s="12" t="n"/>
     </row>
+    <row r="123">
+      <c r="C123" s="12" t="n"/>
+      <c r="D123" s="12" t="n"/>
+      <c r="E123" s="12" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="G54:I54"/>
     <mergeCell ref="O14:Q14"/>
@@ -6229,6 +6230,7 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="C10:Q10"/>
     <mergeCell ref="O54:Q54"/>
+    <mergeCell ref="C55:E55"/>
     <mergeCell ref="K54:M54"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="C11:Q11"/>

</xml_diff>

<commit_message>
Began creating csv outputs
</commit_message>
<xml_diff>
--- a/Outputs/SA_MI.xlsx
+++ b/Outputs/SA_MI.xlsx
@@ -294,7 +294,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -442,9 +442,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,7 +835,7 @@
       <selection activeCell="B23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="9.140625" customWidth="1" style="2" min="1" max="1"/>
     <col width="11.140625" customWidth="1" style="3" min="2" max="3"/>
@@ -1163,13 +1160,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AF124"/>
+  <dimension ref="A2:AF123"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
   <cols>
     <col width="3.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="26.7109375" customWidth="1" style="1" min="2" max="2"/>
@@ -3394,262 +3391,323 @@
       <c r="W51" s="12" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1"/>
-    <row r="53"/>
+    <row r="53">
+      <c r="B53" s="29" t="inlineStr">
+        <is>
+          <t>Specialist Advice Activity by measure, per working day</t>
+        </is>
+      </c>
+      <c r="G53" s="16" t="n"/>
+      <c r="T53" s="12" t="n"/>
+      <c r="U53" s="12" t="n"/>
+      <c r="V53" s="12" t="n"/>
+      <c r="W53" s="12" t="n"/>
+      <c r="X53" s="26" t="n"/>
+      <c r="Y53" s="12" t="n"/>
+    </row>
     <row r="54" ht="30" customHeight="1">
-      <c r="B54" s="29" t="inlineStr">
-        <is>
-          <t>Specialist Advice Activity by measure, per working day</t>
-        </is>
-      </c>
-      <c r="G54" s="16" t="n"/>
-      <c r="T54" s="12" t="n"/>
-      <c r="U54" s="12" t="n"/>
-      <c r="V54" s="12" t="n"/>
-      <c r="W54" s="12" t="n"/>
+      <c r="W54" s="25" t="n"/>
       <c r="X54" s="26" t="n"/>
       <c r="Y54" s="12" t="n"/>
     </row>
     <row r="55" ht="73.5" customHeight="1">
-      <c r="C55" s="71" t="n"/>
-      <c r="G55" s="71" t="n"/>
-      <c r="K55" s="71" t="n"/>
-      <c r="O55" s="71" t="n"/>
+      <c r="C55" s="68" t="inlineStr">
+        <is>
+          <t>All types of Specialist Advice</t>
+        </is>
+      </c>
+      <c r="F55" s="21" t="n"/>
+      <c r="G55" s="69" t="inlineStr">
+        <is>
+          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
+        </is>
+      </c>
+      <c r="H55" s="61" t="n"/>
+      <c r="I55" s="62" t="n"/>
+      <c r="J55" s="21" t="n"/>
+      <c r="K55" s="69" t="inlineStr">
+        <is>
+          <t>Post Referral Specialist Advice</t>
+        </is>
+      </c>
+      <c r="L55" s="61" t="n"/>
+      <c r="M55" s="62" t="n"/>
+      <c r="N55" s="21" t="n"/>
+      <c r="O55" s="69" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="P55" s="61" t="n"/>
+      <c r="Q55" s="62" t="n"/>
       <c r="W55" s="25" t="n"/>
       <c r="X55" s="26" t="n"/>
       <c r="Y55" s="12" t="n"/>
     </row>
     <row r="56">
-      <c r="C56" s="68" t="inlineStr">
-        <is>
-          <t>All types of Specialist Advice</t>
-        </is>
-      </c>
-      <c r="F56" s="21" t="n"/>
-      <c r="G56" s="69" t="inlineStr">
-        <is>
-          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
-        </is>
-      </c>
-      <c r="H56" s="61" t="n"/>
-      <c r="I56" s="62" t="n"/>
-      <c r="J56" s="21" t="n"/>
-      <c r="K56" s="69" t="inlineStr">
-        <is>
-          <t>Post Referral Specialist Advice</t>
-        </is>
-      </c>
-      <c r="L56" s="61" t="n"/>
-      <c r="M56" s="62" t="n"/>
-      <c r="N56" s="21" t="n"/>
-      <c r="O56" s="69" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="P56" s="61" t="n"/>
-      <c r="Q56" s="62" t="n"/>
-      <c r="W56" s="25" t="n"/>
-      <c r="X56" s="26" t="n"/>
-      <c r="Y56" s="12" t="n"/>
-    </row>
-    <row r="57">
-      <c r="B57" s="9" t="inlineStr">
+      <c r="B56" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">Month </t>
         </is>
       </c>
-      <c r="C57" s="9" t="inlineStr">
+      <c r="C56" s="9" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="D57" s="9" t="inlineStr">
+      <c r="D56" s="9" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="E57" s="9" t="inlineStr">
+      <c r="E56" s="9" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="F57" s="22" t="n"/>
-      <c r="G57" s="10" t="inlineStr">
+      <c r="F56" s="22" t="n"/>
+      <c r="G56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="H57" s="10" t="inlineStr">
+      <c r="H56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="I57" s="10" t="inlineStr">
+      <c r="I56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="J57" s="22" t="n"/>
-      <c r="K57" s="10" t="inlineStr">
+      <c r="J56" s="22" t="n"/>
+      <c r="K56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="L57" s="10" t="inlineStr">
+      <c r="L56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="M57" s="10" t="inlineStr">
+      <c r="M56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="N57" s="22" t="n"/>
-      <c r="O57" s="10" t="inlineStr">
+      <c r="N56" s="22" t="n"/>
+      <c r="O56" s="10" t="inlineStr">
         <is>
           <t>Total Requests 
 per working day</t>
         </is>
       </c>
-      <c r="P57" s="10" t="inlineStr">
+      <c r="P56" s="10" t="inlineStr">
         <is>
           <t>Processed Requests per working day</t>
         </is>
       </c>
-      <c r="Q57" s="10" t="inlineStr">
+      <c r="Q56" s="10" t="inlineStr">
         <is>
           <t>Diverted Requests per working day</t>
         </is>
       </c>
-      <c r="S57" s="28" t="inlineStr">
+      <c r="S56" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">No. of working days </t>
         </is>
       </c>
-      <c r="W57" s="25" t="n"/>
+      <c r="W56" s="25" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="11">
+        <f>B16</f>
+        <v/>
+      </c>
+      <c r="C57" s="13">
+        <f>C16/$S56</f>
+        <v/>
+      </c>
+      <c r="D57" s="13">
+        <f>D16/$S56</f>
+        <v/>
+      </c>
+      <c r="E57" s="13">
+        <f>E16/$S56</f>
+        <v/>
+      </c>
+      <c r="G57" s="13">
+        <f>G16/$S56</f>
+        <v/>
+      </c>
+      <c r="H57" s="13">
+        <f>H16/$S56</f>
+        <v/>
+      </c>
+      <c r="I57" s="13">
+        <f>I16/$S56</f>
+        <v/>
+      </c>
+      <c r="K57" s="13">
+        <f>K16/$S56</f>
+        <v/>
+      </c>
+      <c r="L57" s="13">
+        <f>L16/$S56</f>
+        <v/>
+      </c>
+      <c r="M57" s="13">
+        <f>M16/$S56</f>
+        <v/>
+      </c>
+      <c r="O57" s="13">
+        <f>O16/$S56</f>
+        <v/>
+      </c>
+      <c r="P57" s="13">
+        <f>P16/$S56</f>
+        <v/>
+      </c>
+      <c r="Q57" s="13">
+        <f>Q16/$S56</f>
+        <v/>
+      </c>
+      <c r="R57" s="12" t="n"/>
+      <c r="S57" s="27" t="n">
+        <v>19</v>
+      </c>
+      <c r="V57" s="24" t="n"/>
+      <c r="W57" s="12" t="n"/>
+      <c r="X57" s="12" t="n"/>
+      <c r="Y57" s="12" t="n"/>
     </row>
     <row r="58">
       <c r="B58" s="11">
-        <f>B16</f>
+        <f>B17</f>
         <v/>
       </c>
       <c r="C58" s="13">
-        <f>C16/$S56</f>
+        <f>C17/$S57</f>
         <v/>
       </c>
       <c r="D58" s="13">
-        <f>D16/$S56</f>
+        <f>D17/$S57</f>
         <v/>
       </c>
       <c r="E58" s="13">
-        <f>E16/$S56</f>
+        <f>E17/$S57</f>
         <v/>
       </c>
       <c r="G58" s="13">
-        <f>G16/$S56</f>
+        <f>G17/$S57</f>
         <v/>
       </c>
       <c r="H58" s="13">
-        <f>H16/$S56</f>
+        <f>H17/$S57</f>
         <v/>
       </c>
       <c r="I58" s="13">
-        <f>I16/$S56</f>
+        <f>I17/$S57</f>
         <v/>
       </c>
       <c r="K58" s="13">
-        <f>K16/$S56</f>
+        <f>K17/$S57</f>
         <v/>
       </c>
       <c r="L58" s="13">
-        <f>L16/$S56</f>
+        <f>L17/$S57</f>
         <v/>
       </c>
       <c r="M58" s="13">
-        <f>M16/$S56</f>
+        <f>M17/$S57</f>
         <v/>
       </c>
       <c r="O58" s="13">
-        <f>O16/$S56</f>
+        <f>O17/$S57</f>
         <v/>
       </c>
       <c r="P58" s="13">
-        <f>P16/$S56</f>
+        <f>P17/$S57</f>
         <v/>
       </c>
       <c r="Q58" s="13">
-        <f>Q16/$S56</f>
+        <f>Q17/$S57</f>
         <v/>
       </c>
       <c r="R58" s="12" t="n"/>
       <c r="S58" s="27" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V58" s="24" t="n"/>
       <c r="W58" s="12" t="n"/>
       <c r="X58" s="12" t="n"/>
       <c r="Y58" s="12" t="n"/>
+      <c r="AA58" s="12" t="n"/>
+      <c r="AB58" s="14" t="n"/>
+      <c r="AE58" s="12" t="n"/>
+      <c r="AF58" s="14" t="n"/>
     </row>
     <row r="59">
       <c r="B59" s="11">
-        <f>B17</f>
+        <f>B18</f>
         <v/>
       </c>
       <c r="C59" s="13">
-        <f>C17/$S57</f>
+        <f>C18/$S58</f>
         <v/>
       </c>
       <c r="D59" s="13">
-        <f>D17/$S57</f>
+        <f>D18/$S58</f>
         <v/>
       </c>
       <c r="E59" s="13">
-        <f>E17/$S57</f>
+        <f>E18/$S58</f>
         <v/>
       </c>
       <c r="G59" s="13">
-        <f>G17/$S57</f>
+        <f>G18/$S58</f>
         <v/>
       </c>
       <c r="H59" s="13">
-        <f>H17/$S57</f>
+        <f>H18/$S58</f>
         <v/>
       </c>
       <c r="I59" s="13">
-        <f>I17/$S57</f>
+        <f>I18/$S58</f>
         <v/>
       </c>
       <c r="K59" s="13">
-        <f>K17/$S57</f>
+        <f>K18/$S58</f>
         <v/>
       </c>
       <c r="L59" s="13">
-        <f>L17/$S57</f>
+        <f>L18/$S58</f>
         <v/>
       </c>
       <c r="M59" s="13">
-        <f>M17/$S57</f>
+        <f>M18/$S58</f>
         <v/>
       </c>
       <c r="O59" s="13">
-        <f>O17/$S57</f>
+        <f>O18/$S58</f>
         <v/>
       </c>
       <c r="P59" s="13">
-        <f>P17/$S57</f>
+        <f>P18/$S58</f>
         <v/>
       </c>
       <c r="Q59" s="13">
-        <f>Q17/$S57</f>
+        <f>Q18/$S58</f>
         <v/>
       </c>
       <c r="R59" s="12" t="n"/>
       <c r="S59" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V59" s="24" t="n"/>
       <c r="W59" s="12" t="n"/>
@@ -3662,60 +3720,60 @@
     </row>
     <row r="60">
       <c r="B60" s="11">
-        <f>B18</f>
+        <f>B19</f>
         <v/>
       </c>
       <c r="C60" s="13">
-        <f>C18/$S58</f>
+        <f>C19/$S59</f>
         <v/>
       </c>
       <c r="D60" s="13">
-        <f>D18/$S58</f>
+        <f>D19/$S59</f>
         <v/>
       </c>
       <c r="E60" s="13">
-        <f>E18/$S58</f>
+        <f>E19/$S59</f>
         <v/>
       </c>
       <c r="G60" s="13">
-        <f>G18/$S58</f>
+        <f>G19/$S59</f>
         <v/>
       </c>
       <c r="H60" s="13">
-        <f>H18/$S58</f>
+        <f>H19/$S59</f>
         <v/>
       </c>
       <c r="I60" s="13">
-        <f>I18/$S58</f>
+        <f>I19/$S59</f>
         <v/>
       </c>
       <c r="K60" s="13">
-        <f>K18/$S58</f>
+        <f>K19/$S59</f>
         <v/>
       </c>
       <c r="L60" s="13">
-        <f>L18/$S58</f>
+        <f>L19/$S59</f>
         <v/>
       </c>
       <c r="M60" s="13">
-        <f>M18/$S58</f>
+        <f>M19/$S59</f>
         <v/>
       </c>
       <c r="O60" s="13">
-        <f>O18/$S58</f>
+        <f>O19/$S59</f>
         <v/>
       </c>
       <c r="P60" s="13">
-        <f>P18/$S58</f>
+        <f>P19/$S59</f>
         <v/>
       </c>
       <c r="Q60" s="13">
-        <f>Q18/$S58</f>
+        <f>Q19/$S59</f>
         <v/>
       </c>
       <c r="R60" s="12" t="n"/>
       <c r="S60" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V60" s="24" t="n"/>
       <c r="W60" s="12" t="n"/>
@@ -3728,60 +3786,60 @@
     </row>
     <row r="61" ht="15" customHeight="1">
       <c r="B61" s="11">
-        <f>B19</f>
+        <f>B20</f>
         <v/>
       </c>
       <c r="C61" s="13">
-        <f>C19/$S59</f>
+        <f>C20/$S60</f>
         <v/>
       </c>
       <c r="D61" s="13">
-        <f>D19/$S59</f>
+        <f>D20/$S60</f>
         <v/>
       </c>
       <c r="E61" s="13">
-        <f>E19/$S59</f>
+        <f>E20/$S60</f>
         <v/>
       </c>
       <c r="G61" s="13">
-        <f>G19/$S59</f>
+        <f>G20/$S60</f>
         <v/>
       </c>
       <c r="H61" s="13">
-        <f>H19/$S59</f>
+        <f>H20/$S60</f>
         <v/>
       </c>
       <c r="I61" s="13">
-        <f>I19/$S59</f>
+        <f>I20/$S60</f>
         <v/>
       </c>
       <c r="K61" s="13">
-        <f>K19/$S59</f>
+        <f>K20/$S60</f>
         <v/>
       </c>
       <c r="L61" s="13">
-        <f>L19/$S59</f>
+        <f>L20/$S60</f>
         <v/>
       </c>
       <c r="M61" s="13">
-        <f>M19/$S59</f>
+        <f>M20/$S60</f>
         <v/>
       </c>
       <c r="O61" s="13">
-        <f>O19/$S59</f>
+        <f>O20/$S60</f>
         <v/>
       </c>
       <c r="P61" s="13">
-        <f>P19/$S59</f>
+        <f>P20/$S60</f>
         <v/>
       </c>
       <c r="Q61" s="13">
-        <f>Q19/$S59</f>
+        <f>Q20/$S60</f>
         <v/>
       </c>
       <c r="R61" s="12" t="n"/>
       <c r="S61" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V61" s="24" t="n"/>
       <c r="W61" s="12" t="n"/>
@@ -3794,60 +3852,60 @@
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="B62" s="11">
-        <f>B20</f>
+        <f>B21</f>
         <v/>
       </c>
       <c r="C62" s="13">
-        <f>C20/$S60</f>
+        <f>C21/$S61</f>
         <v/>
       </c>
       <c r="D62" s="13">
-        <f>D20/$S60</f>
+        <f>D21/$S61</f>
         <v/>
       </c>
       <c r="E62" s="13">
-        <f>E20/$S60</f>
+        <f>E21/$S61</f>
         <v/>
       </c>
       <c r="G62" s="13">
-        <f>G20/$S60</f>
+        <f>G21/$S61</f>
         <v/>
       </c>
       <c r="H62" s="13">
-        <f>H20/$S60</f>
+        <f>H21/$S61</f>
         <v/>
       </c>
       <c r="I62" s="13">
-        <f>I20/$S60</f>
+        <f>I21/$S61</f>
         <v/>
       </c>
       <c r="K62" s="13">
-        <f>K20/$S60</f>
+        <f>K21/$S61</f>
         <v/>
       </c>
       <c r="L62" s="13">
-        <f>L20/$S60</f>
+        <f>L21/$S61</f>
         <v/>
       </c>
       <c r="M62" s="13">
-        <f>M20/$S60</f>
+        <f>M21/$S61</f>
         <v/>
       </c>
       <c r="O62" s="13">
-        <f>O20/$S60</f>
+        <f>O21/$S61</f>
         <v/>
       </c>
       <c r="P62" s="13">
-        <f>P20/$S60</f>
+        <f>P21/$S61</f>
         <v/>
       </c>
       <c r="Q62" s="13">
-        <f>Q20/$S60</f>
-        <v/>
-      </c>
-      <c r="R62" s="12" t="n"/>
+        <f>Q21/$S61</f>
+        <v/>
+      </c>
+      <c r="R62" s="15" t="n"/>
       <c r="S62" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V62" s="24" t="n"/>
       <c r="W62" s="12" t="n"/>
@@ -3860,55 +3918,55 @@
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="B63" s="11">
-        <f>B21</f>
+        <f>B22</f>
         <v/>
       </c>
       <c r="C63" s="13">
-        <f>C21/$S61</f>
+        <f>C22/$S62</f>
         <v/>
       </c>
       <c r="D63" s="13">
-        <f>D21/$S61</f>
+        <f>D22/$S62</f>
         <v/>
       </c>
       <c r="E63" s="13">
-        <f>E21/$S61</f>
+        <f>E22/$S62</f>
         <v/>
       </c>
       <c r="G63" s="13">
-        <f>G21/$S61</f>
+        <f>G22/$S62</f>
         <v/>
       </c>
       <c r="H63" s="13">
-        <f>H21/$S61</f>
+        <f>H22/$S62</f>
         <v/>
       </c>
       <c r="I63" s="13">
-        <f>I21/$S61</f>
+        <f>I22/$S62</f>
         <v/>
       </c>
       <c r="K63" s="13">
-        <f>K21/$S61</f>
+        <f>K22/$S62</f>
         <v/>
       </c>
       <c r="L63" s="13">
-        <f>L21/$S61</f>
+        <f>L22/$S62</f>
         <v/>
       </c>
       <c r="M63" s="13">
-        <f>M21/$S61</f>
+        <f>M22/$S62</f>
         <v/>
       </c>
       <c r="O63" s="13">
-        <f>O21/$S61</f>
+        <f>O22/$S62</f>
         <v/>
       </c>
       <c r="P63" s="13">
-        <f>P21/$S61</f>
+        <f>P22/$S62</f>
         <v/>
       </c>
       <c r="Q63" s="13">
-        <f>Q21/$S61</f>
+        <f>Q22/$S62</f>
         <v/>
       </c>
       <c r="R63" s="15" t="n"/>
@@ -3926,65 +3984,66 @@
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="B64" s="11">
-        <f>B22</f>
+        <f>B23</f>
         <v/>
       </c>
       <c r="C64" s="13">
-        <f>C22/$S62</f>
+        <f>C23/$S63</f>
         <v/>
       </c>
       <c r="D64" s="13">
-        <f>D22/$S62</f>
+        <f>D23/$S63</f>
         <v/>
       </c>
       <c r="E64" s="13">
-        <f>E22/$S62</f>
+        <f>E23/$S63</f>
         <v/>
       </c>
       <c r="G64" s="13">
-        <f>G22/$S62</f>
+        <f>G23/$S63</f>
         <v/>
       </c>
       <c r="H64" s="13">
-        <f>H22/$S62</f>
+        <f>H23/$S63</f>
         <v/>
       </c>
       <c r="I64" s="13">
-        <f>I22/$S62</f>
+        <f>I23/$S63</f>
         <v/>
       </c>
       <c r="K64" s="13">
-        <f>K22/$S62</f>
+        <f>K23/$S63</f>
         <v/>
       </c>
       <c r="L64" s="13">
-        <f>L22/$S62</f>
+        <f>L23/$S63</f>
         <v/>
       </c>
       <c r="M64" s="13">
-        <f>M22/$S62</f>
+        <f>M23/$S63</f>
         <v/>
       </c>
       <c r="O64" s="13">
-        <f>O22/$S62</f>
+        <f>O23/$S63</f>
         <v/>
       </c>
       <c r="P64" s="13">
-        <f>P22/$S62</f>
+        <f>P23/$S63</f>
         <v/>
       </c>
       <c r="Q64" s="13">
-        <f>Q22/$S62</f>
+        <f>Q23/$S63</f>
         <v/>
       </c>
       <c r="R64" s="15" t="n"/>
       <c r="S64" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V64" s="24" t="n"/>
       <c r="W64" s="12" t="n"/>
       <c r="X64" s="12" t="n"/>
       <c r="Y64" s="12" t="n"/>
+      <c r="Z64" s="12" t="n"/>
       <c r="AA64" s="12" t="n"/>
       <c r="AB64" s="14" t="n"/>
       <c r="AE64" s="12" t="n"/>
@@ -3992,60 +4051,60 @@
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="B65" s="11">
-        <f>B23</f>
+        <f>B24</f>
         <v/>
       </c>
       <c r="C65" s="13">
-        <f>C23/$S63</f>
+        <f>C24/$S64</f>
         <v/>
       </c>
       <c r="D65" s="13">
-        <f>D23/$S63</f>
+        <f>D24/$S64</f>
         <v/>
       </c>
       <c r="E65" s="13">
-        <f>E23/$S63</f>
+        <f>E24/$S64</f>
         <v/>
       </c>
       <c r="G65" s="13">
-        <f>G23/$S63</f>
+        <f>G24/$S64</f>
         <v/>
       </c>
       <c r="H65" s="13">
-        <f>H23/$S63</f>
+        <f>H24/$S64</f>
         <v/>
       </c>
       <c r="I65" s="13">
-        <f>I23/$S63</f>
+        <f>I24/$S64</f>
         <v/>
       </c>
       <c r="K65" s="13">
-        <f>K23/$S63</f>
+        <f>K24/$S64</f>
         <v/>
       </c>
       <c r="L65" s="13">
-        <f>L23/$S63</f>
+        <f>L24/$S64</f>
         <v/>
       </c>
       <c r="M65" s="13">
-        <f>M23/$S63</f>
+        <f>M24/$S64</f>
         <v/>
       </c>
       <c r="O65" s="13">
-        <f>O23/$S63</f>
+        <f>O24/$S64</f>
         <v/>
       </c>
       <c r="P65" s="13">
-        <f>P23/$S63</f>
+        <f>P24/$S64</f>
         <v/>
       </c>
       <c r="Q65" s="13">
-        <f>Q23/$S63</f>
+        <f>Q24/$S64</f>
         <v/>
       </c>
       <c r="R65" s="15" t="n"/>
       <c r="S65" s="27" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V65" s="24" t="n"/>
       <c r="W65" s="12" t="n"/>
@@ -4059,60 +4118,60 @@
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="B66" s="11">
-        <f>B24</f>
+        <f>B25</f>
         <v/>
       </c>
       <c r="C66" s="13">
-        <f>C24/$S64</f>
+        <f>C25/$S65</f>
         <v/>
       </c>
       <c r="D66" s="13">
-        <f>D24/$S64</f>
+        <f>D25/$S65</f>
         <v/>
       </c>
       <c r="E66" s="13">
-        <f>E24/$S64</f>
+        <f>E25/$S65</f>
         <v/>
       </c>
       <c r="G66" s="13">
-        <f>G24/$S64</f>
+        <f>G25/$S65</f>
         <v/>
       </c>
       <c r="H66" s="13">
-        <f>H24/$S64</f>
+        <f>H25/$S65</f>
         <v/>
       </c>
       <c r="I66" s="13">
-        <f>I24/$S64</f>
+        <f>I25/$S65</f>
         <v/>
       </c>
       <c r="K66" s="13">
-        <f>K24/$S64</f>
+        <f>K25/$S65</f>
         <v/>
       </c>
       <c r="L66" s="13">
-        <f>L24/$S64</f>
+        <f>L25/$S65</f>
         <v/>
       </c>
       <c r="M66" s="13">
-        <f>M24/$S64</f>
+        <f>M25/$S65</f>
         <v/>
       </c>
       <c r="O66" s="13">
-        <f>O24/$S64</f>
+        <f>O25/$S65</f>
         <v/>
       </c>
       <c r="P66" s="13">
-        <f>P24/$S64</f>
+        <f>P25/$S65</f>
         <v/>
       </c>
       <c r="Q66" s="13">
-        <f>Q24/$S64</f>
+        <f>Q25/$S65</f>
         <v/>
       </c>
       <c r="R66" s="15" t="n"/>
       <c r="S66" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V66" s="24" t="n"/>
       <c r="W66" s="12" t="n"/>
@@ -4126,60 +4185,60 @@
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="B67" s="11">
-        <f>B25</f>
+        <f>B26</f>
         <v/>
       </c>
       <c r="C67" s="13">
-        <f>C25/$S65</f>
+        <f>C26/$S66</f>
         <v/>
       </c>
       <c r="D67" s="13">
-        <f>D25/$S65</f>
+        <f>D26/$S66</f>
         <v/>
       </c>
       <c r="E67" s="13">
-        <f>E25/$S65</f>
+        <f>E26/$S66</f>
         <v/>
       </c>
       <c r="G67" s="13">
-        <f>G25/$S65</f>
+        <f>G26/$S66</f>
         <v/>
       </c>
       <c r="H67" s="13">
-        <f>H25/$S65</f>
+        <f>H26/$S66</f>
         <v/>
       </c>
       <c r="I67" s="13">
-        <f>I25/$S65</f>
+        <f>I26/$S66</f>
         <v/>
       </c>
       <c r="K67" s="13">
-        <f>K25/$S65</f>
+        <f>K26/$S66</f>
         <v/>
       </c>
       <c r="L67" s="13">
-        <f>L25/$S65</f>
+        <f>L26/$S66</f>
         <v/>
       </c>
       <c r="M67" s="13">
-        <f>M25/$S65</f>
+        <f>M26/$S66</f>
         <v/>
       </c>
       <c r="O67" s="13">
-        <f>O25/$S65</f>
+        <f>O26/$S66</f>
         <v/>
       </c>
       <c r="P67" s="13">
-        <f>P25/$S65</f>
+        <f>P26/$S66</f>
         <v/>
       </c>
       <c r="Q67" s="13">
-        <f>Q25/$S65</f>
+        <f>Q26/$S66</f>
         <v/>
       </c>
       <c r="R67" s="15" t="n"/>
       <c r="S67" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V67" s="24" t="n"/>
       <c r="W67" s="12" t="n"/>
@@ -4193,60 +4252,60 @@
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="B68" s="11">
-        <f>B26</f>
+        <f>B27</f>
         <v/>
       </c>
       <c r="C68" s="13">
-        <f>C26/$S66</f>
+        <f>C27/$S67</f>
         <v/>
       </c>
       <c r="D68" s="13">
-        <f>D26/$S66</f>
+        <f>D27/$S67</f>
         <v/>
       </c>
       <c r="E68" s="13">
-        <f>E26/$S66</f>
+        <f>E27/$S67</f>
         <v/>
       </c>
       <c r="G68" s="13">
-        <f>G26/$S66</f>
+        <f>G27/$S67</f>
         <v/>
       </c>
       <c r="H68" s="13">
-        <f>H26/$S66</f>
+        <f>H27/$S67</f>
         <v/>
       </c>
       <c r="I68" s="13">
-        <f>I26/$S66</f>
+        <f>I27/$S67</f>
         <v/>
       </c>
       <c r="K68" s="13">
-        <f>K26/$S66</f>
+        <f>K27/$S67</f>
         <v/>
       </c>
       <c r="L68" s="13">
-        <f>L26/$S66</f>
+        <f>L27/$S67</f>
         <v/>
       </c>
       <c r="M68" s="13">
-        <f>M26/$S66</f>
+        <f>M27/$S67</f>
         <v/>
       </c>
       <c r="O68" s="13">
-        <f>O26/$S66</f>
+        <f>O27/$S67</f>
         <v/>
       </c>
       <c r="P68" s="13">
-        <f>P26/$S66</f>
+        <f>P27/$S67</f>
         <v/>
       </c>
       <c r="Q68" s="13">
-        <f>Q26/$S66</f>
+        <f>Q27/$S67</f>
         <v/>
       </c>
       <c r="R68" s="15" t="n"/>
       <c r="S68" s="27" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="V68" s="24" t="n"/>
       <c r="W68" s="12" t="n"/>
@@ -4260,60 +4319,60 @@
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="B69" s="11">
-        <f>B27</f>
+        <f>B28</f>
         <v/>
       </c>
       <c r="C69" s="13">
-        <f>C27/$S67</f>
+        <f>C28/$S68</f>
         <v/>
       </c>
       <c r="D69" s="13">
-        <f>D27/$S67</f>
+        <f>D28/$S68</f>
         <v/>
       </c>
       <c r="E69" s="13">
-        <f>E27/$S67</f>
+        <f>E28/$S68</f>
         <v/>
       </c>
       <c r="G69" s="13">
-        <f>G27/$S67</f>
+        <f>G28/$S68</f>
         <v/>
       </c>
       <c r="H69" s="13">
-        <f>H27/$S67</f>
+        <f>H28/$S68</f>
         <v/>
       </c>
       <c r="I69" s="13">
-        <f>I27/$S67</f>
+        <f>I28/$S68</f>
         <v/>
       </c>
       <c r="K69" s="13">
-        <f>K27/$S67</f>
+        <f>K28/$S68</f>
         <v/>
       </c>
       <c r="L69" s="13">
-        <f>L27/$S67</f>
+        <f>L28/$S68</f>
         <v/>
       </c>
       <c r="M69" s="13">
-        <f>M27/$S67</f>
+        <f>M28/$S68</f>
         <v/>
       </c>
       <c r="O69" s="13">
-        <f>O27/$S67</f>
+        <f>O28/$S68</f>
         <v/>
       </c>
       <c r="P69" s="13">
-        <f>P27/$S67</f>
+        <f>P28/$S68</f>
         <v/>
       </c>
       <c r="Q69" s="13">
-        <f>Q27/$S67</f>
+        <f>Q28/$S68</f>
         <v/>
       </c>
       <c r="R69" s="15" t="n"/>
       <c r="S69" s="27" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="V69" s="24" t="n"/>
       <c r="W69" s="12" t="n"/>
@@ -4322,65 +4381,65 @@
       <c r="Z69" s="12" t="n"/>
       <c r="AA69" s="12" t="n"/>
       <c r="AB69" s="14" t="n"/>
-      <c r="AE69" s="12" t="n"/>
+      <c r="AE69" s="16" t="n"/>
       <c r="AF69" s="14" t="n"/>
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="B70" s="11">
-        <f>B28</f>
+        <f>B29</f>
         <v/>
       </c>
       <c r="C70" s="13">
-        <f>C28/$S68</f>
+        <f>C29/$S69</f>
         <v/>
       </c>
       <c r="D70" s="13">
-        <f>D28/$S68</f>
+        <f>D29/$S69</f>
         <v/>
       </c>
       <c r="E70" s="13">
-        <f>E28/$S68</f>
+        <f>E29/$S69</f>
         <v/>
       </c>
       <c r="G70" s="13">
-        <f>G28/$S68</f>
+        <f>G29/$S69</f>
         <v/>
       </c>
       <c r="H70" s="13">
-        <f>H28/$S68</f>
+        <f>H29/$S69</f>
         <v/>
       </c>
       <c r="I70" s="13">
-        <f>I28/$S68</f>
+        <f>I29/$S69</f>
         <v/>
       </c>
       <c r="K70" s="13">
-        <f>K28/$S68</f>
+        <f>K29/$S69</f>
         <v/>
       </c>
       <c r="L70" s="13">
-        <f>L28/$S68</f>
+        <f>L29/$S69</f>
         <v/>
       </c>
       <c r="M70" s="13">
-        <f>M28/$S68</f>
+        <f>M29/$S69</f>
         <v/>
       </c>
       <c r="O70" s="13">
-        <f>O28/$S68</f>
+        <f>O29/$S69</f>
         <v/>
       </c>
       <c r="P70" s="13">
-        <f>P28/$S68</f>
+        <f>P29/$S69</f>
         <v/>
       </c>
       <c r="Q70" s="13">
-        <f>Q28/$S68</f>
+        <f>Q29/$S69</f>
         <v/>
       </c>
       <c r="R70" s="15" t="n"/>
       <c r="S70" s="27" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="V70" s="24" t="n"/>
       <c r="W70" s="12" t="n"/>
@@ -4394,60 +4453,60 @@
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="B71" s="11">
-        <f>B29</f>
+        <f>B30</f>
         <v/>
       </c>
       <c r="C71" s="13">
-        <f>C29/$S69</f>
+        <f>C30/$S70</f>
         <v/>
       </c>
       <c r="D71" s="13">
-        <f>D29/$S69</f>
+        <f>D30/$S70</f>
         <v/>
       </c>
       <c r="E71" s="13">
-        <f>E29/$S69</f>
+        <f>E30/$S70</f>
         <v/>
       </c>
       <c r="G71" s="13">
-        <f>G29/$S69</f>
+        <f>G30/$S70</f>
         <v/>
       </c>
       <c r="H71" s="13">
-        <f>H29/$S69</f>
+        <f>H30/$S70</f>
         <v/>
       </c>
       <c r="I71" s="13">
-        <f>I29/$S69</f>
+        <f>I30/$S70</f>
         <v/>
       </c>
       <c r="K71" s="13">
-        <f>K29/$S69</f>
+        <f>K30/$S70</f>
         <v/>
       </c>
       <c r="L71" s="13">
-        <f>L29/$S69</f>
+        <f>L30/$S70</f>
         <v/>
       </c>
       <c r="M71" s="13">
-        <f>M29/$S69</f>
+        <f>M30/$S70</f>
         <v/>
       </c>
       <c r="O71" s="13">
-        <f>O29/$S69</f>
+        <f>O30/$S70</f>
         <v/>
       </c>
       <c r="P71" s="13">
-        <f>P29/$S69</f>
+        <f>P30/$S70</f>
         <v/>
       </c>
       <c r="Q71" s="13">
-        <f>Q29/$S69</f>
+        <f>Q30/$S70</f>
         <v/>
       </c>
       <c r="R71" s="15" t="n"/>
       <c r="S71" s="27" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V71" s="24" t="n"/>
       <c r="W71" s="12" t="n"/>
@@ -4461,60 +4520,60 @@
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="B72" s="11">
-        <f>B30</f>
+        <f>B31</f>
         <v/>
       </c>
       <c r="C72" s="13">
-        <f>C30/$S70</f>
+        <f>C31/$S71</f>
         <v/>
       </c>
       <c r="D72" s="13">
-        <f>D30/$S70</f>
+        <f>D31/$S71</f>
         <v/>
       </c>
       <c r="E72" s="13">
-        <f>E30/$S70</f>
+        <f>E31/$S71</f>
         <v/>
       </c>
       <c r="G72" s="13">
-        <f>G30/$S70</f>
+        <f>G31/$S71</f>
         <v/>
       </c>
       <c r="H72" s="13">
-        <f>H30/$S70</f>
+        <f>H31/$S71</f>
         <v/>
       </c>
       <c r="I72" s="13">
-        <f>I30/$S70</f>
+        <f>I31/$S71</f>
         <v/>
       </c>
       <c r="K72" s="13">
-        <f>K30/$S70</f>
+        <f>K31/$S71</f>
         <v/>
       </c>
       <c r="L72" s="13">
-        <f>L30/$S70</f>
+        <f>L31/$S71</f>
         <v/>
       </c>
       <c r="M72" s="13">
-        <f>M30/$S70</f>
+        <f>M31/$S71</f>
         <v/>
       </c>
       <c r="O72" s="13">
-        <f>O30/$S70</f>
+        <f>O31/$S71</f>
         <v/>
       </c>
       <c r="P72" s="13">
-        <f>P30/$S70</f>
+        <f>P31/$S71</f>
         <v/>
       </c>
       <c r="Q72" s="13">
-        <f>Q30/$S70</f>
+        <f>Q31/$S71</f>
         <v/>
       </c>
       <c r="R72" s="15" t="n"/>
       <c r="S72" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V72" s="24" t="n"/>
       <c r="W72" s="12" t="n"/>
@@ -4528,60 +4587,60 @@
     </row>
     <row r="73">
       <c r="B73" s="11">
-        <f>B31</f>
+        <f>B32</f>
         <v/>
       </c>
       <c r="C73" s="13">
-        <f>C31/$S71</f>
+        <f>C32/$S72</f>
         <v/>
       </c>
       <c r="D73" s="13">
-        <f>D31/$S71</f>
+        <f>D32/$S72</f>
         <v/>
       </c>
       <c r="E73" s="13">
-        <f>E31/$S71</f>
+        <f>E32/$S72</f>
         <v/>
       </c>
       <c r="G73" s="13">
-        <f>G31/$S71</f>
+        <f>G32/$S72</f>
         <v/>
       </c>
       <c r="H73" s="13">
-        <f>H31/$S71</f>
+        <f>H32/$S72</f>
         <v/>
       </c>
       <c r="I73" s="13">
-        <f>I31/$S71</f>
+        <f>I32/$S72</f>
         <v/>
       </c>
       <c r="K73" s="13">
-        <f>K31/$S71</f>
+        <f>K32/$S72</f>
         <v/>
       </c>
       <c r="L73" s="13">
-        <f>L31/$S71</f>
+        <f>L32/$S72</f>
         <v/>
       </c>
       <c r="M73" s="13">
-        <f>M31/$S71</f>
+        <f>M32/$S72</f>
         <v/>
       </c>
       <c r="O73" s="13">
-        <f>O31/$S71</f>
+        <f>O32/$S72</f>
         <v/>
       </c>
       <c r="P73" s="13">
-        <f>P31/$S71</f>
+        <f>P32/$S72</f>
         <v/>
       </c>
       <c r="Q73" s="13">
-        <f>Q31/$S71</f>
+        <f>Q32/$S72</f>
         <v/>
       </c>
       <c r="R73" s="15" t="n"/>
       <c r="S73" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V73" s="24" t="n"/>
       <c r="W73" s="12" t="n"/>
@@ -4595,60 +4654,60 @@
     </row>
     <row r="74">
       <c r="B74" s="11">
-        <f>B32</f>
+        <f>B33</f>
         <v/>
       </c>
       <c r="C74" s="13">
-        <f>C32/$S72</f>
+        <f>C33/$S73</f>
         <v/>
       </c>
       <c r="D74" s="13">
-        <f>D32/$S72</f>
+        <f>D33/$S73</f>
         <v/>
       </c>
       <c r="E74" s="13">
-        <f>E32/$S72</f>
+        <f>E33/$S73</f>
         <v/>
       </c>
       <c r="G74" s="13">
-        <f>G32/$S72</f>
+        <f>G33/$S73</f>
         <v/>
       </c>
       <c r="H74" s="13">
-        <f>H32/$S72</f>
+        <f>H33/$S73</f>
         <v/>
       </c>
       <c r="I74" s="13">
-        <f>I32/$S72</f>
+        <f>I33/$S73</f>
         <v/>
       </c>
       <c r="K74" s="13">
-        <f>K32/$S72</f>
+        <f>K33/$S73</f>
         <v/>
       </c>
       <c r="L74" s="13">
-        <f>L32/$S72</f>
+        <f>L33/$S73</f>
         <v/>
       </c>
       <c r="M74" s="13">
-        <f>M32/$S72</f>
+        <f>M33/$S73</f>
         <v/>
       </c>
       <c r="O74" s="13">
-        <f>O32/$S72</f>
+        <f>O33/$S73</f>
         <v/>
       </c>
       <c r="P74" s="13">
-        <f>P32/$S72</f>
+        <f>P33/$S73</f>
         <v/>
       </c>
       <c r="Q74" s="13">
-        <f>Q32/$S72</f>
-        <v/>
-      </c>
-      <c r="R74" s="15" t="n"/>
+        <f>Q33/$S73</f>
+        <v/>
+      </c>
+      <c r="R74" s="12" t="n"/>
       <c r="S74" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V74" s="24" t="n"/>
       <c r="W74" s="12" t="n"/>
@@ -4662,60 +4721,60 @@
     </row>
     <row r="75">
       <c r="B75" s="11">
-        <f>B33</f>
+        <f>B34</f>
         <v/>
       </c>
       <c r="C75" s="13">
-        <f>C33/$S73</f>
+        <f>C34/$S74</f>
         <v/>
       </c>
       <c r="D75" s="13">
-        <f>D33/$S73</f>
+        <f>D34/$S74</f>
         <v/>
       </c>
       <c r="E75" s="13">
-        <f>E33/$S73</f>
+        <f>E34/$S74</f>
         <v/>
       </c>
       <c r="G75" s="13">
-        <f>G33/$S73</f>
+        <f>G34/$S74</f>
         <v/>
       </c>
       <c r="H75" s="13">
-        <f>H33/$S73</f>
+        <f>H34/$S74</f>
         <v/>
       </c>
       <c r="I75" s="13">
-        <f>I33/$S73</f>
+        <f>I34/$S74</f>
         <v/>
       </c>
       <c r="K75" s="13">
-        <f>K33/$S73</f>
+        <f>K34/$S74</f>
         <v/>
       </c>
       <c r="L75" s="13">
-        <f>L33/$S73</f>
+        <f>L34/$S74</f>
         <v/>
       </c>
       <c r="M75" s="13">
-        <f>M33/$S73</f>
+        <f>M34/$S74</f>
         <v/>
       </c>
       <c r="O75" s="13">
-        <f>O33/$S73</f>
+        <f>O34/$S74</f>
         <v/>
       </c>
       <c r="P75" s="13">
-        <f>P33/$S73</f>
+        <f>P34/$S74</f>
         <v/>
       </c>
       <c r="Q75" s="13">
-        <f>Q33/$S73</f>
+        <f>Q34/$S74</f>
         <v/>
       </c>
       <c r="R75" s="12" t="n"/>
       <c r="S75" s="27" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V75" s="24" t="n"/>
       <c r="W75" s="12" t="n"/>
@@ -4729,55 +4788,55 @@
     </row>
     <row r="76">
       <c r="B76" s="11">
-        <f>B34</f>
+        <f>B35</f>
         <v/>
       </c>
       <c r="C76" s="13">
-        <f>C34/$S74</f>
+        <f>C35/$S75</f>
         <v/>
       </c>
       <c r="D76" s="13">
-        <f>D34/$S74</f>
+        <f>D35/$S75</f>
         <v/>
       </c>
       <c r="E76" s="13">
-        <f>E34/$S74</f>
+        <f>E35/$S75</f>
         <v/>
       </c>
       <c r="G76" s="13">
-        <f>G34/$S74</f>
+        <f>G35/$S75</f>
         <v/>
       </c>
       <c r="H76" s="13">
-        <f>H34/$S74</f>
+        <f>H35/$S75</f>
         <v/>
       </c>
       <c r="I76" s="13">
-        <f>I34/$S74</f>
+        <f>I35/$S75</f>
         <v/>
       </c>
       <c r="K76" s="13">
-        <f>K34/$S74</f>
+        <f>K35/$S75</f>
         <v/>
       </c>
       <c r="L76" s="13">
-        <f>L34/$S74</f>
+        <f>L35/$S75</f>
         <v/>
       </c>
       <c r="M76" s="13">
-        <f>M34/$S74</f>
+        <f>M35/$S75</f>
         <v/>
       </c>
       <c r="O76" s="13">
-        <f>O34/$S74</f>
+        <f>O35/$S75</f>
         <v/>
       </c>
       <c r="P76" s="13">
-        <f>P34/$S74</f>
+        <f>P35/$S75</f>
         <v/>
       </c>
       <c r="Q76" s="13">
-        <f>Q34/$S74</f>
+        <f>Q35/$S75</f>
         <v/>
       </c>
       <c r="R76" s="12" t="n"/>
@@ -4796,60 +4855,60 @@
     </row>
     <row r="77">
       <c r="B77" s="11">
-        <f>B35</f>
+        <f>B36</f>
         <v/>
       </c>
       <c r="C77" s="13">
-        <f>C35/$S75</f>
+        <f>C36/$S76</f>
         <v/>
       </c>
       <c r="D77" s="13">
-        <f>D35/$S75</f>
+        <f>D36/$S76</f>
         <v/>
       </c>
       <c r="E77" s="13">
-        <f>E35/$S75</f>
+        <f>E36/$S76</f>
         <v/>
       </c>
       <c r="G77" s="13">
-        <f>G35/$S75</f>
+        <f>G36/$S76</f>
         <v/>
       </c>
       <c r="H77" s="13">
-        <f>H35/$S75</f>
+        <f>H36/$S76</f>
         <v/>
       </c>
       <c r="I77" s="13">
-        <f>I35/$S75</f>
+        <f>I36/$S76</f>
         <v/>
       </c>
       <c r="K77" s="13">
-        <f>K35/$S75</f>
+        <f>K36/$S76</f>
         <v/>
       </c>
       <c r="L77" s="13">
-        <f>L35/$S75</f>
+        <f>L36/$S76</f>
         <v/>
       </c>
       <c r="M77" s="13">
-        <f>M35/$S75</f>
+        <f>M36/$S76</f>
         <v/>
       </c>
       <c r="O77" s="13">
-        <f>O35/$S75</f>
+        <f>O36/$S76</f>
         <v/>
       </c>
       <c r="P77" s="13">
-        <f>P35/$S75</f>
+        <f>P36/$S76</f>
         <v/>
       </c>
       <c r="Q77" s="13">
-        <f>Q35/$S75</f>
+        <f>Q36/$S76</f>
         <v/>
       </c>
       <c r="R77" s="12" t="n"/>
       <c r="S77" s="27" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="V77" s="24" t="n"/>
       <c r="W77" s="12" t="n"/>
@@ -4863,60 +4922,60 @@
     </row>
     <row r="78">
       <c r="B78" s="11">
-        <f>B36</f>
+        <f>B37</f>
         <v/>
       </c>
       <c r="C78" s="13">
-        <f>C36/$S76</f>
+        <f>C37/$S77</f>
         <v/>
       </c>
       <c r="D78" s="13">
-        <f>D36/$S76</f>
+        <f>D37/$S77</f>
         <v/>
       </c>
       <c r="E78" s="13">
-        <f>E36/$S76</f>
+        <f>E37/$S77</f>
         <v/>
       </c>
       <c r="G78" s="13">
-        <f>G36/$S76</f>
+        <f>G37/$S77</f>
         <v/>
       </c>
       <c r="H78" s="13">
-        <f>H36/$S76</f>
+        <f>H37/$S77</f>
         <v/>
       </c>
       <c r="I78" s="13">
-        <f>I36/$S76</f>
+        <f>I37/$S77</f>
         <v/>
       </c>
       <c r="K78" s="13">
-        <f>K36/$S76</f>
+        <f>K37/$S77</f>
         <v/>
       </c>
       <c r="L78" s="13">
-        <f>L36/$S76</f>
+        <f>L37/$S77</f>
         <v/>
       </c>
       <c r="M78" s="13">
-        <f>M36/$S76</f>
+        <f>M37/$S77</f>
         <v/>
       </c>
       <c r="O78" s="13">
-        <f>O36/$S76</f>
+        <f>O37/$S77</f>
         <v/>
       </c>
       <c r="P78" s="13">
-        <f>P36/$S76</f>
+        <f>P37/$S77</f>
         <v/>
       </c>
       <c r="Q78" s="13">
-        <f>Q36/$S76</f>
+        <f>Q37/$S77</f>
         <v/>
       </c>
       <c r="R78" s="12" t="n"/>
       <c r="S78" s="27" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="V78" s="24" t="n"/>
       <c r="W78" s="12" t="n"/>
@@ -4930,60 +4989,60 @@
     </row>
     <row r="79">
       <c r="B79" s="11">
-        <f>B37</f>
+        <f>B38</f>
         <v/>
       </c>
       <c r="C79" s="13">
-        <f>C37/$S77</f>
+        <f>C38/$S78</f>
         <v/>
       </c>
       <c r="D79" s="13">
-        <f>D37/$S77</f>
+        <f>D38/$S78</f>
         <v/>
       </c>
       <c r="E79" s="13">
-        <f>E37/$S77</f>
+        <f>E38/$S78</f>
         <v/>
       </c>
       <c r="G79" s="13">
-        <f>G37/$S77</f>
+        <f>G38/$S78</f>
         <v/>
       </c>
       <c r="H79" s="13">
-        <f>H37/$S77</f>
+        <f>H38/$S78</f>
         <v/>
       </c>
       <c r="I79" s="13">
-        <f>I37/$S77</f>
+        <f>I38/$S78</f>
         <v/>
       </c>
       <c r="K79" s="13">
-        <f>K37/$S77</f>
+        <f>K38/$S78</f>
         <v/>
       </c>
       <c r="L79" s="13">
-        <f>L37/$S77</f>
+        <f>L38/$S78</f>
         <v/>
       </c>
       <c r="M79" s="13">
-        <f>M37/$S77</f>
+        <f>M38/$S78</f>
         <v/>
       </c>
       <c r="O79" s="13">
-        <f>O37/$S77</f>
+        <f>O38/$S78</f>
         <v/>
       </c>
       <c r="P79" s="13">
-        <f>P37/$S77</f>
+        <f>P38/$S78</f>
         <v/>
       </c>
       <c r="Q79" s="13">
-        <f>Q37/$S77</f>
+        <f>Q38/$S78</f>
         <v/>
       </c>
       <c r="R79" s="12" t="n"/>
       <c r="S79" s="27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V79" s="24" t="n"/>
       <c r="W79" s="12" t="n"/>
@@ -4997,60 +5056,60 @@
     </row>
     <row r="80">
       <c r="B80" s="11">
-        <f>B38</f>
+        <f>B39</f>
         <v/>
       </c>
       <c r="C80" s="13">
-        <f>C38/$S78</f>
+        <f>C39/$S79</f>
         <v/>
       </c>
       <c r="D80" s="13">
-        <f>D38/$S78</f>
+        <f>D39/$S79</f>
         <v/>
       </c>
       <c r="E80" s="13">
-        <f>E38/$S78</f>
+        <f>E39/$S79</f>
         <v/>
       </c>
       <c r="G80" s="13">
-        <f>G38/$S78</f>
+        <f>G39/$S79</f>
         <v/>
       </c>
       <c r="H80" s="13">
-        <f>H38/$S78</f>
+        <f>H39/$S79</f>
         <v/>
       </c>
       <c r="I80" s="13">
-        <f>I38/$S78</f>
+        <f>I39/$S79</f>
         <v/>
       </c>
       <c r="K80" s="13">
-        <f>K38/$S78</f>
+        <f>K39/$S79</f>
         <v/>
       </c>
       <c r="L80" s="13">
-        <f>L38/$S78</f>
+        <f>L39/$S79</f>
         <v/>
       </c>
       <c r="M80" s="13">
-        <f>M38/$S78</f>
+        <f>M39/$S79</f>
         <v/>
       </c>
       <c r="O80" s="13">
-        <f>O38/$S78</f>
+        <f>O39/$S79</f>
         <v/>
       </c>
       <c r="P80" s="13">
-        <f>P38/$S78</f>
+        <f>P39/$S79</f>
         <v/>
       </c>
       <c r="Q80" s="13">
-        <f>Q38/$S78</f>
+        <f>Q39/$S79</f>
         <v/>
       </c>
       <c r="R80" s="12" t="n"/>
       <c r="S80" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V80" s="24" t="n"/>
       <c r="W80" s="12" t="n"/>
@@ -5064,60 +5123,60 @@
     </row>
     <row r="81">
       <c r="B81" s="11">
-        <f>B39</f>
+        <f>B40</f>
         <v/>
       </c>
       <c r="C81" s="13">
-        <f>C39/$S79</f>
+        <f>C40/$S80</f>
         <v/>
       </c>
       <c r="D81" s="13">
-        <f>D39/$S79</f>
+        <f>D40/$S80</f>
         <v/>
       </c>
       <c r="E81" s="13">
-        <f>E39/$S79</f>
+        <f>E40/$S80</f>
         <v/>
       </c>
       <c r="G81" s="13">
-        <f>G39/$S79</f>
+        <f>G40/$S80</f>
         <v/>
       </c>
       <c r="H81" s="13">
-        <f>H39/$S79</f>
+        <f>H40/$S80</f>
         <v/>
       </c>
       <c r="I81" s="13">
-        <f>I39/$S79</f>
+        <f>I40/$S80</f>
         <v/>
       </c>
       <c r="K81" s="13">
-        <f>K39/$S79</f>
+        <f>K40/$S80</f>
         <v/>
       </c>
       <c r="L81" s="13">
-        <f>L39/$S79</f>
+        <f>L40/$S80</f>
         <v/>
       </c>
       <c r="M81" s="13">
-        <f>M39/$S79</f>
+        <f>M40/$S80</f>
         <v/>
       </c>
       <c r="O81" s="13">
-        <f>O39/$S79</f>
+        <f>O40/$S80</f>
         <v/>
       </c>
       <c r="P81" s="13">
-        <f>P39/$S79</f>
+        <f>P40/$S80</f>
         <v/>
       </c>
       <c r="Q81" s="13">
-        <f>Q39/$S79</f>
+        <f>Q40/$S80</f>
         <v/>
       </c>
       <c r="R81" s="12" t="n"/>
       <c r="S81" s="27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V81" s="24" t="n"/>
       <c r="W81" s="12" t="n"/>
@@ -5131,55 +5190,55 @@
     </row>
     <row r="82">
       <c r="B82" s="11">
-        <f>B40</f>
+        <f>B41</f>
         <v/>
       </c>
       <c r="C82" s="13">
-        <f>C40/$S80</f>
+        <f>C41/$S81</f>
         <v/>
       </c>
       <c r="D82" s="13">
-        <f>D40/$S80</f>
+        <f>D41/$S81</f>
         <v/>
       </c>
       <c r="E82" s="13">
-        <f>E40/$S80</f>
+        <f>E41/$S81</f>
         <v/>
       </c>
       <c r="G82" s="13">
-        <f>G40/$S80</f>
+        <f>G41/$S81</f>
         <v/>
       </c>
       <c r="H82" s="13">
-        <f>H40/$S80</f>
+        <f>H41/$S81</f>
         <v/>
       </c>
       <c r="I82" s="13">
-        <f>I40/$S80</f>
+        <f>I41/$S81</f>
         <v/>
       </c>
       <c r="K82" s="13">
-        <f>K40/$S80</f>
+        <f>K41/$S81</f>
         <v/>
       </c>
       <c r="L82" s="13">
-        <f>L40/$S80</f>
+        <f>L41/$S81</f>
         <v/>
       </c>
       <c r="M82" s="13">
-        <f>M40/$S80</f>
+        <f>M41/$S81</f>
         <v/>
       </c>
       <c r="O82" s="13">
-        <f>O40/$S80</f>
+        <f>O41/$S81</f>
         <v/>
       </c>
       <c r="P82" s="13">
-        <f>P40/$S80</f>
+        <f>P41/$S81</f>
         <v/>
       </c>
       <c r="Q82" s="13">
-        <f>Q40/$S80</f>
+        <f>Q41/$S81</f>
         <v/>
       </c>
       <c r="R82" s="12" t="n"/>
@@ -5198,60 +5257,60 @@
     </row>
     <row r="83">
       <c r="B83" s="11">
-        <f>B41</f>
+        <f>B42</f>
         <v/>
       </c>
       <c r="C83" s="13">
-        <f>C41/$S81</f>
+        <f>C42/$S82</f>
         <v/>
       </c>
       <c r="D83" s="13">
-        <f>D41/$S81</f>
+        <f>D42/$S82</f>
         <v/>
       </c>
       <c r="E83" s="13">
-        <f>E41/$S81</f>
+        <f>E42/$S82</f>
         <v/>
       </c>
       <c r="G83" s="13">
-        <f>G41/$S81</f>
+        <f>G42/$S82</f>
         <v/>
       </c>
       <c r="H83" s="13">
-        <f>H41/$S81</f>
+        <f>H42/$S82</f>
         <v/>
       </c>
       <c r="I83" s="13">
-        <f>I41/$S81</f>
+        <f>I42/$S82</f>
         <v/>
       </c>
       <c r="K83" s="13">
-        <f>K41/$S81</f>
+        <f>K42/$S82</f>
         <v/>
       </c>
       <c r="L83" s="13">
-        <f>L41/$S81</f>
+        <f>L42/$S82</f>
         <v/>
       </c>
       <c r="M83" s="13">
-        <f>M41/$S81</f>
+        <f>M42/$S82</f>
         <v/>
       </c>
       <c r="O83" s="13">
-        <f>O41/$S81</f>
+        <f>O42/$S82</f>
         <v/>
       </c>
       <c r="P83" s="13">
-        <f>P41/$S81</f>
+        <f>P42/$S82</f>
         <v/>
       </c>
       <c r="Q83" s="13">
-        <f>Q41/$S81</f>
+        <f>Q42/$S82</f>
         <v/>
       </c>
       <c r="R83" s="12" t="n"/>
       <c r="S83" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V83" s="24" t="n"/>
       <c r="W83" s="12" t="n"/>
@@ -5265,60 +5324,60 @@
     </row>
     <row r="84">
       <c r="B84" s="11">
-        <f>B42</f>
+        <f>B43</f>
         <v/>
       </c>
       <c r="C84" s="13">
-        <f>C42/$S82</f>
+        <f>C43/$S83</f>
         <v/>
       </c>
       <c r="D84" s="13">
-        <f>D42/$S82</f>
+        <f>D43/$S83</f>
         <v/>
       </c>
       <c r="E84" s="13">
-        <f>E42/$S82</f>
+        <f>E43/$S83</f>
         <v/>
       </c>
       <c r="G84" s="13">
-        <f>G42/$S82</f>
+        <f>G43/$S83</f>
         <v/>
       </c>
       <c r="H84" s="13">
-        <f>H42/$S82</f>
+        <f>H43/$S83</f>
         <v/>
       </c>
       <c r="I84" s="13">
-        <f>I42/$S82</f>
+        <f>I43/$S83</f>
         <v/>
       </c>
       <c r="K84" s="13">
-        <f>K42/$S82</f>
+        <f>K43/$S83</f>
         <v/>
       </c>
       <c r="L84" s="13">
-        <f>L42/$S82</f>
+        <f>L43/$S83</f>
         <v/>
       </c>
       <c r="M84" s="13">
-        <f>M42/$S82</f>
+        <f>M43/$S83</f>
         <v/>
       </c>
       <c r="O84" s="13">
-        <f>O42/$S82</f>
+        <f>O43/$S83</f>
         <v/>
       </c>
       <c r="P84" s="13">
-        <f>P42/$S82</f>
+        <f>P43/$S83</f>
         <v/>
       </c>
       <c r="Q84" s="13">
-        <f>Q42/$S82</f>
+        <f>Q43/$S83</f>
         <v/>
       </c>
       <c r="R84" s="12" t="n"/>
       <c r="S84" s="27" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="V84" s="24" t="n"/>
       <c r="W84" s="12" t="n"/>
@@ -5332,60 +5391,60 @@
     </row>
     <row r="85">
       <c r="B85" s="11">
-        <f>B43</f>
+        <f>B44</f>
         <v/>
       </c>
       <c r="C85" s="13">
-        <f>C43/$S83</f>
+        <f>C44/$S84</f>
         <v/>
       </c>
       <c r="D85" s="13">
-        <f>D43/$S83</f>
+        <f>D44/$S84</f>
         <v/>
       </c>
       <c r="E85" s="13">
-        <f>E43/$S83</f>
+        <f>E44/$S84</f>
         <v/>
       </c>
       <c r="G85" s="13">
-        <f>G43/$S83</f>
+        <f>G44/$S84</f>
         <v/>
       </c>
       <c r="H85" s="13">
-        <f>H43/$S83</f>
+        <f>H44/$S84</f>
         <v/>
       </c>
       <c r="I85" s="13">
-        <f>I43/$S83</f>
+        <f>I44/$S84</f>
         <v/>
       </c>
       <c r="K85" s="13">
-        <f>K43/$S83</f>
+        <f>K44/$S84</f>
         <v/>
       </c>
       <c r="L85" s="13">
-        <f>L43/$S83</f>
+        <f>L44/$S84</f>
         <v/>
       </c>
       <c r="M85" s="13">
-        <f>M43/$S83</f>
+        <f>M44/$S84</f>
         <v/>
       </c>
       <c r="O85" s="13">
-        <f>O43/$S83</f>
+        <f>O44/$S84</f>
         <v/>
       </c>
       <c r="P85" s="13">
-        <f>P43/$S83</f>
+        <f>P44/$S84</f>
         <v/>
       </c>
       <c r="Q85" s="13">
-        <f>Q43/$S83</f>
+        <f>Q44/$S84</f>
         <v/>
       </c>
       <c r="R85" s="12" t="n"/>
       <c r="S85" s="27" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="V85" s="24" t="n"/>
       <c r="W85" s="12" t="n"/>
@@ -5399,126 +5458,120 @@
     </row>
     <row r="86">
       <c r="B86" s="11">
-        <f>B44</f>
+        <f>B45</f>
         <v/>
       </c>
       <c r="C86" s="13">
-        <f>C44/$S84</f>
+        <f>C45/$S85</f>
         <v/>
       </c>
       <c r="D86" s="13">
-        <f>D44/$S84</f>
+        <f>D45/$S85</f>
         <v/>
       </c>
       <c r="E86" s="13">
-        <f>E44/$S84</f>
+        <f>E45/$S85</f>
         <v/>
       </c>
       <c r="G86" s="13">
-        <f>G44/$S84</f>
+        <f>G45/$S85</f>
         <v/>
       </c>
       <c r="H86" s="13">
-        <f>H44/$S84</f>
+        <f>H45/$S85</f>
         <v/>
       </c>
       <c r="I86" s="13">
-        <f>I44/$S84</f>
+        <f>I45/$S85</f>
         <v/>
       </c>
       <c r="K86" s="13">
-        <f>K44/$S84</f>
+        <f>K45/$S85</f>
         <v/>
       </c>
       <c r="L86" s="13">
-        <f>L44/$S84</f>
+        <f>L45/$S85</f>
         <v/>
       </c>
       <c r="M86" s="13">
-        <f>M44/$S84</f>
+        <f>M45/$S85</f>
         <v/>
       </c>
       <c r="O86" s="13">
-        <f>O44/$S84</f>
+        <f>O45/$S85</f>
         <v/>
       </c>
       <c r="P86" s="13">
-        <f>P44/$S84</f>
+        <f>P45/$S85</f>
         <v/>
       </c>
       <c r="Q86" s="13">
-        <f>Q44/$S84</f>
-        <v/>
-      </c>
-      <c r="R86" s="12" t="n"/>
+        <f>Q45/$S85</f>
+        <v/>
+      </c>
       <c r="S86" s="27" t="n">
         <v>21</v>
       </c>
-      <c r="V86" s="24" t="n"/>
       <c r="W86" s="12" t="n"/>
       <c r="X86" s="12" t="n"/>
       <c r="Y86" s="12" t="n"/>
       <c r="Z86" s="12" t="n"/>
-      <c r="AA86" s="12" t="n"/>
-      <c r="AB86" s="14" t="n"/>
-      <c r="AE86" s="16" t="n"/>
-      <c r="AF86" s="14" t="n"/>
     </row>
     <row r="87">
       <c r="B87" s="11">
-        <f>B45</f>
+        <f>B46</f>
         <v/>
       </c>
       <c r="C87" s="13">
-        <f>C45/$S85</f>
+        <f>C46/$S86</f>
         <v/>
       </c>
       <c r="D87" s="13">
-        <f>D45/$S85</f>
+        <f>D46/$S86</f>
         <v/>
       </c>
       <c r="E87" s="13">
-        <f>E45/$S85</f>
+        <f>E46/$S86</f>
         <v/>
       </c>
       <c r="G87" s="13">
-        <f>G45/$S85</f>
+        <f>G46/$S86</f>
         <v/>
       </c>
       <c r="H87" s="13">
-        <f>H45/$S85</f>
+        <f>H46/$S86</f>
         <v/>
       </c>
       <c r="I87" s="13">
-        <f>I45/$S85</f>
+        <f>I46/$S86</f>
         <v/>
       </c>
       <c r="K87" s="13">
-        <f>K45/$S85</f>
+        <f>K46/$S86</f>
         <v/>
       </c>
       <c r="L87" s="13">
-        <f>L45/$S85</f>
+        <f>L46/$S86</f>
         <v/>
       </c>
       <c r="M87" s="13">
-        <f>M45/$S85</f>
+        <f>M46/$S86</f>
         <v/>
       </c>
       <c r="O87" s="13">
-        <f>O45/$S85</f>
+        <f>O46/$S86</f>
         <v/>
       </c>
       <c r="P87" s="13">
-        <f>P45/$S85</f>
+        <f>P46/$S86</f>
         <v/>
       </c>
       <c r="Q87" s="13">
-        <f>Q45/$S85</f>
+        <f>Q46/$S86</f>
         <v/>
       </c>
       <c r="S87" s="27" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="W87" s="12" t="n"/>
       <c r="X87" s="12" t="n"/>
@@ -5527,294 +5580,248 @@
     </row>
     <row r="88">
       <c r="B88" s="11">
-        <f>B46</f>
+        <f>B47</f>
         <v/>
       </c>
       <c r="C88" s="13">
-        <f>C46/$S86</f>
+        <f>C47/$S87</f>
         <v/>
       </c>
       <c r="D88" s="13">
-        <f>D46/$S86</f>
+        <f>D47/$S87</f>
         <v/>
       </c>
       <c r="E88" s="13">
-        <f>E46/$S86</f>
+        <f>E47/$S87</f>
         <v/>
       </c>
       <c r="G88" s="13">
-        <f>G46/$S86</f>
+        <f>G47/$S87</f>
         <v/>
       </c>
       <c r="H88" s="13">
-        <f>H46/$S86</f>
+        <f>H47/$S87</f>
         <v/>
       </c>
       <c r="I88" s="13">
-        <f>I46/$S86</f>
+        <f>I47/$S87</f>
         <v/>
       </c>
       <c r="K88" s="13">
-        <f>K46/$S86</f>
+        <f>K47/$S87</f>
         <v/>
       </c>
       <c r="L88" s="13">
-        <f>L46/$S86</f>
+        <f>L47/$S87</f>
         <v/>
       </c>
       <c r="M88" s="13">
-        <f>M46/$S86</f>
+        <f>M47/$S87</f>
         <v/>
       </c>
       <c r="O88" s="13">
-        <f>O46/$S86</f>
+        <f>O47/$S87</f>
         <v/>
       </c>
       <c r="P88" s="13">
-        <f>P46/$S86</f>
+        <f>P47/$S87</f>
         <v/>
       </c>
       <c r="Q88" s="13">
-        <f>Q46/$S86</f>
+        <f>Q47/$S87</f>
         <v/>
       </c>
       <c r="S88" s="27" t="n">
-        <v>23</v>
-      </c>
-      <c r="W88" s="12" t="n"/>
-      <c r="X88" s="12" t="n"/>
-      <c r="Y88" s="12" t="n"/>
-      <c r="Z88" s="12" t="n"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" s="11">
-        <f>B47</f>
+        <f>B48</f>
         <v/>
       </c>
       <c r="C89" s="13">
-        <f>C47/$S87</f>
+        <f>C48/$S88</f>
         <v/>
       </c>
       <c r="D89" s="13">
-        <f>D47/$S87</f>
+        <f>D48/$S88</f>
         <v/>
       </c>
       <c r="E89" s="13">
-        <f>E47/$S87</f>
+        <f>E48/$S88</f>
         <v/>
       </c>
       <c r="G89" s="13">
-        <f>G47/$S87</f>
+        <f>G48/$S88</f>
         <v/>
       </c>
       <c r="H89" s="13">
-        <f>H47/$S87</f>
+        <f>H48/$S88</f>
         <v/>
       </c>
       <c r="I89" s="13">
-        <f>I47/$S87</f>
+        <f>I48/$S88</f>
         <v/>
       </c>
       <c r="K89" s="13">
-        <f>K47/$S87</f>
+        <f>K48/$S88</f>
         <v/>
       </c>
       <c r="L89" s="13">
-        <f>L47/$S87</f>
+        <f>L48/$S88</f>
         <v/>
       </c>
       <c r="M89" s="13">
-        <f>M47/$S87</f>
+        <f>M48/$S88</f>
         <v/>
       </c>
       <c r="O89" s="13">
-        <f>O47/$S87</f>
+        <f>O48/$S88</f>
         <v/>
       </c>
       <c r="P89" s="13">
-        <f>P47/$S87</f>
+        <f>P48/$S88</f>
         <v/>
       </c>
       <c r="Q89" s="13">
-        <f>Q47/$S87</f>
+        <f>Q48/$S88</f>
         <v/>
       </c>
       <c r="S89" s="27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" s="11">
-        <f>B48</f>
+        <f>B49</f>
         <v/>
       </c>
       <c r="C90" s="13">
-        <f>C48/$S88</f>
+        <f>C49/$S89</f>
         <v/>
       </c>
       <c r="D90" s="13">
-        <f>D48/$S88</f>
+        <f>D49/$S89</f>
         <v/>
       </c>
       <c r="E90" s="13">
-        <f>E48/$S88</f>
+        <f>E49/$S89</f>
         <v/>
       </c>
       <c r="G90" s="13">
-        <f>G48/$S88</f>
+        <f>G49/$S89</f>
         <v/>
       </c>
       <c r="H90" s="13">
-        <f>H48/$S88</f>
+        <f>H49/$S89</f>
         <v/>
       </c>
       <c r="I90" s="13">
-        <f>I48/$S88</f>
+        <f>I49/$S89</f>
         <v/>
       </c>
       <c r="K90" s="13">
-        <f>K48/$S88</f>
+        <f>K49/$S89</f>
         <v/>
       </c>
       <c r="L90" s="13">
-        <f>L48/$S88</f>
+        <f>L49/$S89</f>
         <v/>
       </c>
       <c r="M90" s="13">
-        <f>M48/$S88</f>
+        <f>M49/$S89</f>
         <v/>
       </c>
       <c r="O90" s="13">
-        <f>O48/$S88</f>
+        <f>O49/$S89</f>
         <v/>
       </c>
       <c r="P90" s="13">
-        <f>P48/$S88</f>
+        <f>P49/$S89</f>
         <v/>
       </c>
       <c r="Q90" s="13">
-        <f>Q48/$S88</f>
+        <f>Q49/$S89</f>
         <v/>
       </c>
       <c r="S90" s="27" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" s="11">
-        <f>B49</f>
+        <f>B50</f>
         <v/>
       </c>
       <c r="C91" s="13">
-        <f>C49/$S89</f>
+        <f>C50/$S90</f>
         <v/>
       </c>
       <c r="D91" s="13">
-        <f>D49/$S89</f>
+        <f>D50/$S90</f>
         <v/>
       </c>
       <c r="E91" s="13">
-        <f>E49/$S89</f>
+        <f>E50/$S90</f>
         <v/>
       </c>
       <c r="G91" s="13">
-        <f>G49/$S89</f>
+        <f>G50/$S90</f>
         <v/>
       </c>
       <c r="H91" s="13">
-        <f>H49/$S89</f>
+        <f>H50/$S90</f>
         <v/>
       </c>
       <c r="I91" s="13">
-        <f>I49/$S89</f>
+        <f>I50/$S90</f>
         <v/>
       </c>
       <c r="K91" s="13">
-        <f>K49/$S89</f>
+        <f>K50/$S90</f>
         <v/>
       </c>
       <c r="L91" s="13">
-        <f>L49/$S89</f>
+        <f>L50/$S90</f>
         <v/>
       </c>
       <c r="M91" s="13">
-        <f>M49/$S89</f>
+        <f>M50/$S90</f>
         <v/>
       </c>
       <c r="O91" s="13">
-        <f>O49/$S89</f>
+        <f>O50/$S90</f>
         <v/>
       </c>
       <c r="P91" s="13">
-        <f>P49/$S89</f>
+        <f>P50/$S90</f>
         <v/>
       </c>
       <c r="Q91" s="13">
-        <f>Q49/$S89</f>
+        <f>Q50/$S90</f>
         <v/>
       </c>
       <c r="S91" s="27" t="n">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="T91" s="12" t="n"/>
+      <c r="U91" s="70" t="n"/>
     </row>
     <row r="92">
-      <c r="B92" s="11">
-        <f>B50</f>
-        <v/>
-      </c>
-      <c r="C92" s="13">
-        <f>C50/$S90</f>
-        <v/>
-      </c>
-      <c r="D92" s="13">
-        <f>D50/$S90</f>
-        <v/>
-      </c>
-      <c r="E92" s="13">
-        <f>E50/$S90</f>
-        <v/>
-      </c>
-      <c r="G92" s="13">
-        <f>G50/$S90</f>
-        <v/>
-      </c>
-      <c r="H92" s="13">
-        <f>H50/$S90</f>
-        <v/>
-      </c>
-      <c r="I92" s="13">
-        <f>I50/$S90</f>
-        <v/>
-      </c>
-      <c r="K92" s="13">
-        <f>K50/$S90</f>
-        <v/>
-      </c>
-      <c r="L92" s="13">
-        <f>L50/$S90</f>
-        <v/>
-      </c>
-      <c r="M92" s="13">
-        <f>M50/$S90</f>
-        <v/>
-      </c>
-      <c r="O92" s="13">
-        <f>O50/$S90</f>
-        <v/>
-      </c>
-      <c r="P92" s="13">
-        <f>P50/$S90</f>
-        <v/>
-      </c>
-      <c r="Q92" s="13">
-        <f>Q50/$S90</f>
-        <v/>
-      </c>
-      <c r="S92" s="27" t="n">
-        <v>20</v>
-      </c>
-      <c r="T92" s="12" t="n"/>
-      <c r="U92" s="70" t="n"/>
+      <c r="B92" s="25" t="n"/>
+      <c r="C92" s="12" t="n"/>
+      <c r="D92" s="14" t="n"/>
+      <c r="E92" s="12" t="n"/>
+      <c r="G92" s="12" t="n"/>
+      <c r="H92" s="14" t="n"/>
+      <c r="I92" s="12" t="n"/>
+      <c r="K92" s="14" t="n"/>
+      <c r="L92" s="14" t="n"/>
+      <c r="M92" s="12" t="n"/>
+      <c r="O92" s="12" t="n"/>
+      <c r="P92" s="12" t="n"/>
+      <c r="Q92" s="12" t="n"/>
     </row>
     <row r="93">
       <c r="B93" s="25" t="n"/>
@@ -6042,15 +6049,14 @@
       <c r="Q107" s="12" t="n"/>
     </row>
     <row r="108">
-      <c r="B108" s="25" t="n"/>
       <c r="C108" s="12" t="n"/>
-      <c r="D108" s="14" t="n"/>
+      <c r="D108" s="12" t="n"/>
       <c r="E108" s="12" t="n"/>
       <c r="G108" s="12" t="n"/>
       <c r="H108" s="14" t="n"/>
       <c r="I108" s="12" t="n"/>
-      <c r="K108" s="14" t="n"/>
-      <c r="L108" s="14" t="n"/>
+      <c r="K108" s="12" t="n"/>
+      <c r="L108" s="12" t="n"/>
       <c r="M108" s="12" t="n"/>
       <c r="O108" s="12" t="n"/>
       <c r="P108" s="12" t="n"/>
@@ -6061,7 +6067,7 @@
       <c r="D109" s="12" t="n"/>
       <c r="E109" s="12" t="n"/>
       <c r="G109" s="12" t="n"/>
-      <c r="H109" s="14" t="n"/>
+      <c r="H109" s="12" t="n"/>
       <c r="I109" s="12" t="n"/>
       <c r="K109" s="12" t="n"/>
       <c r="L109" s="12" t="n"/>
@@ -6200,15 +6206,6 @@
       <c r="C119" s="12" t="n"/>
       <c r="D119" s="12" t="n"/>
       <c r="E119" s="12" t="n"/>
-      <c r="G119" s="12" t="n"/>
-      <c r="H119" s="12" t="n"/>
-      <c r="I119" s="12" t="n"/>
-      <c r="K119" s="12" t="n"/>
-      <c r="L119" s="12" t="n"/>
-      <c r="M119" s="12" t="n"/>
-      <c r="O119" s="12" t="n"/>
-      <c r="P119" s="12" t="n"/>
-      <c r="Q119" s="12" t="n"/>
     </row>
     <row r="120">
       <c r="C120" s="12" t="n"/>
@@ -6229,11 +6226,6 @@
       <c r="C123" s="12" t="n"/>
       <c r="D123" s="12" t="n"/>
       <c r="E123" s="12" t="n"/>
-    </row>
-    <row r="124">
-      <c r="C124" s="12" t="n"/>
-      <c r="D124" s="12" t="n"/>
-      <c r="E124" s="12" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Created all dfs for each sa type with pivots
</commit_message>
<xml_diff>
--- a/Outputs/SA_MI.xlsx
+++ b/Outputs/SA_MI.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Source Data &amp; Defintions" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="England | Specialist Advice" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="England | Working days" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -392,27 +393,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -422,7 +402,28 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -847,7 +848,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="B1" s="56" t="n"/>
+      <c r="B1" s="49" t="n"/>
       <c r="F1" s="37" t="n"/>
       <c r="G1" s="37" t="n"/>
       <c r="H1" s="37" t="n"/>
@@ -855,7 +856,7 @@
       <c r="J1" s="37" t="n"/>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="B2" s="57" t="inlineStr">
+      <c r="B2" s="50" t="inlineStr">
         <is>
           <t>Source Data &amp; Defintions</t>
         </is>
@@ -867,7 +868,7 @@
       <c r="J2" s="37" t="n"/>
     </row>
     <row r="3" ht="388.5" customHeight="1">
-      <c r="B3" s="53" t="inlineStr">
+      <c r="B3" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">Data source 
 Monthly specialist advice activity returns are collected from Integrated Care Boards (ICBs) as part of the System Elective Recovery Outpatient Collection (System EROC). 
@@ -890,7 +891,7 @@
       <c r="J3" s="5" t="n"/>
     </row>
     <row r="4" ht="6.6" customHeight="1">
-      <c r="B4" s="53" t="n"/>
+      <c r="B4" s="51" t="n"/>
       <c r="F4" s="37" t="n"/>
       <c r="G4" s="37" t="n"/>
       <c r="H4" s="37" t="n"/>
@@ -910,7 +911,7 @@
       <c r="J5" s="37" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="58" t="inlineStr">
+      <c r="B6" s="53" t="inlineStr">
         <is>
           <t>The data are also available by ‘type of specialist advice’, and defines the different types as:</t>
         </is>
@@ -922,7 +923,7 @@
       <c r="J6" s="37" t="n"/>
     </row>
     <row r="7" ht="36.75" customHeight="1">
-      <c r="B7" s="55" t="inlineStr">
+      <c r="B7" s="48" t="inlineStr">
         <is>
           <t>Pre Referral specialist advice (e.g. Advice &amp; Guidance)</t>
         </is>
@@ -934,7 +935,7 @@
       <c r="J7" s="37" t="n"/>
     </row>
     <row r="8" ht="70.5" customFormat="1" customHeight="1" s="3">
-      <c r="B8" s="49" t="inlineStr">
+      <c r="B8" s="54" t="inlineStr">
         <is>
           <t>Specialist advice to support a clinical dialogue, enabling a referring clinician to seek advice from a specialist prior to, or instead of referral about a named patient. This can be synchronous, for example, a telephone call; or  asynchronous, enabled electronically through the NHS e-Referral Service (e-RS) Advice &amp; Guidance channel or other IT platforms / dedicated email addresses where there is agreement from all stakeholders that these will be used to leverage Advice &amp; Guidance</t>
         </is>
@@ -946,7 +947,7 @@
       <c r="J8" s="39" t="n"/>
     </row>
     <row r="9" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B9" s="49" t="inlineStr">
+      <c r="B9" s="54" t="inlineStr">
         <is>
           <t>Pre Referral Specialist advice may be provided by appropriately trained and commissioned specialists including both consultant and non-consultant led services in secondary care community or primary care providers, interface or intermediate services, and referral management systems.</t>
         </is>
@@ -958,7 +959,7 @@
       <c r="J9" s="39" t="n"/>
     </row>
     <row r="10" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B10" s="49" t="inlineStr">
+      <c r="B10" s="54" t="inlineStr">
         <is>
           <t>This will typically be accessed via a digital communication channel and facilitate a two-way dialogue and sharing of relevant clinical information in relation to the management of a named patient where at the outset of the interaction there is no clear intention to refer to secondary care.</t>
         </is>
@@ -970,7 +971,7 @@
       <c r="J10" s="39" t="n"/>
     </row>
     <row r="11" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B11" s="50" t="inlineStr">
+      <c r="B11" s="55" t="inlineStr">
         <is>
           <t>This is non face to face activity, with no referral or booking having yet been made, and as such there has been no RTT Clock Start.</t>
         </is>
@@ -993,7 +994,7 @@
       <c r="J12" s="37" t="n"/>
     </row>
     <row r="13" ht="36.75" customHeight="1">
-      <c r="B13" s="55" t="inlineStr">
+      <c r="B13" s="48" t="inlineStr">
         <is>
           <t>Post Referral Specialist advice (e.g. Referral Triage models that offer Specialist advice)</t>
         </is>
@@ -1005,7 +1006,7 @@
       <c r="J13" s="37" t="n"/>
     </row>
     <row r="14" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B14" s="49" t="inlineStr">
+      <c r="B14" s="54" t="inlineStr">
         <is>
           <t>Specialist-led assessment of a patient’s clinical referral Information to support a decision on primary care management or the most appropriate onward clinical pathway.</t>
         </is>
@@ -1017,7 +1018,7 @@
       <c r="J14" s="39" t="n"/>
     </row>
     <row r="15" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B15" s="49" t="inlineStr">
+      <c r="B15" s="54" t="inlineStr">
         <is>
           <t>Referrals may be returned to the original referrer with advice to continue to manage in the community, similar to specialist advice, but differ as a referral will have been created with the implicit expectation that onward care would be managed by the service receiving the referral.</t>
         </is>
@@ -1029,7 +1030,7 @@
       <c r="J15" s="39" t="n"/>
     </row>
     <row r="16" ht="59.25" customFormat="1" customHeight="1" s="3">
-      <c r="B16" s="49" t="inlineStr">
+      <c r="B16" s="54" t="inlineStr">
         <is>
           <t>Referral triage can be undertaken by secondary care providers through Referral Assessment Services (RAS) via e-RS, Clinical assessment and triage services (CATS) and referral management centres (RMCs) providing intermediary levels of clinical triage, assessment and treatment between traditional primary and secondary care, or within primary care providers.</t>
         </is>
@@ -1041,21 +1042,21 @@
       <c r="J16" s="39" t="n"/>
     </row>
     <row r="17" ht="36.75" customFormat="1" customHeight="1" s="3">
-      <c r="B17" s="50" t="inlineStr">
+      <c r="B17" s="55" t="inlineStr">
         <is>
           <t>This is non-Face to Face activity, but as a referral has been made there has been an RTT Clock Start. However, no booking, or ASI in lieu of a booking, will have been made, and the episode / patient is not automatically registered on provider PTL.</t>
         </is>
       </c>
     </row>
     <row r="18" ht="36.75" customFormat="1" customHeight="1" s="4">
-      <c r="B18" s="51" t="inlineStr">
+      <c r="B18" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve">Other types of specialist advice </t>
         </is>
       </c>
     </row>
     <row r="19" ht="50.1" customFormat="1" customHeight="1" s="3">
-      <c r="B19" s="49" t="inlineStr">
+      <c r="B19" s="54" t="inlineStr">
         <is>
           <t>Other recorded clinical dialogue that facilitates the seeking and/or provision of specialist advice to support a referrer, enabling more patients to be managed without the need for an onward booking and thereby avoiding unnecessary first attendances where these do not add clinical value.</t>
         </is>
@@ -1064,8 +1065,8 @@
     <row r="20">
       <c r="B20" s="42" t="n"/>
       <c r="C20" s="42" t="n"/>
-      <c r="D20" s="58" t="n"/>
-      <c r="E20" s="58" t="n"/>
+      <c r="D20" s="53" t="n"/>
+      <c r="E20" s="53" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="52" t="inlineStr">
@@ -1075,14 +1076,14 @@
       </c>
     </row>
     <row r="22" ht="44.45" customFormat="1" customHeight="1" s="3">
-      <c r="B22" s="53" t="inlineStr">
+      <c r="B22" s="51" t="inlineStr">
         <is>
           <t>The data collection launched in August 2021, making this a relatively new data collection. Please use caution when interpreting this data as we continue to work with ICBs to improve data quality.</t>
         </is>
       </c>
     </row>
     <row r="23" ht="81.95" customFormat="1" customHeight="1" s="3">
-      <c r="B23" s="54" t="inlineStr">
+      <c r="B23" s="58" t="inlineStr">
         <is>
           <t>Data are included from April 2022 to the latest available reporting period. The England level data is an aggregation of the latest available data as reported by ICBs. This means that the latest position is subject to change as we receive more detail relating to the outcome and status of the specialist advice requests. This is particularly relevant when viewing activity data for 'Processed' and 'Diverted' requests, due to a lag in the reporting of outcomes and status' for requests that are raised toward the end of the reporting period. This lag in the underlying data means that there is an expected general downward trend for these measures in the most recent months, this reporting gap should reduce over time as the data is refreshed each month.</t>
         </is>
@@ -1102,7 +1103,7 @@
       </c>
     </row>
     <row r="26" ht="58.5" customHeight="1">
-      <c r="B26" s="53" t="inlineStr">
+      <c r="B26" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">For further information about the published management information relating to outpatient recovery and transformation, please contact us at england.outpatient-transformation@nhs.net.  </t>
         </is>
@@ -1121,7 +1122,7 @@
       <c r="E28" s="37" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="48" t="n"/>
+      <c r="B29" s="56" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -1162,10 +1163,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AK122"/>
+  <dimension ref="A2:AF122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
@@ -1385,12 +1386,6 @@
           <t>Specialist Advice Activity, by measure and month</t>
         </is>
       </c>
-      <c r="T12" s="46" t="inlineStr">
-        <is>
-          <t>Specialist Advice Activity by measure, per working day</t>
-        </is>
-      </c>
-      <c r="Y12" s="47" t="n"/>
     </row>
     <row r="14" ht="32.25" customFormat="1" customHeight="1" s="6">
       <c r="B14" s="1" t="n"/>
@@ -1423,38 +1418,6 @@
       </c>
       <c r="P14" s="63" t="n"/>
       <c r="Q14" s="64" t="n"/>
-      <c r="T14" s="1" t="n"/>
-      <c r="U14" s="59" t="inlineStr">
-        <is>
-          <t>All types of Specialist Advice</t>
-        </is>
-      </c>
-      <c r="X14" s="21" t="n"/>
-      <c r="Y14" s="60" t="inlineStr">
-        <is>
-          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
-        </is>
-      </c>
-      <c r="Z14" s="63" t="n"/>
-      <c r="AA14" s="64" t="n"/>
-      <c r="AB14" s="21" t="n"/>
-      <c r="AC14" s="61" t="inlineStr">
-        <is>
-          <t>Post Referral Specialist Advice</t>
-        </is>
-      </c>
-      <c r="AD14" s="63" t="n"/>
-      <c r="AE14" s="64" t="n"/>
-      <c r="AF14" s="21" t="n"/>
-      <c r="AG14" s="61" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="AH14" s="63" t="n"/>
-      <c r="AI14" s="64" t="n"/>
-      <c r="AJ14" s="1" t="n"/>
-      <c r="AK14" s="1" t="n"/>
     </row>
     <row r="15" ht="60.95" customFormat="1" customHeight="1" s="8">
       <c r="B15" s="7" t="inlineStr">
@@ -1523,84 +1486,6 @@
       <c r="Q15" s="61" t="inlineStr">
         <is>
           <t>Diverted Requests</t>
-        </is>
-      </c>
-      <c r="T15" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Month </t>
-        </is>
-      </c>
-      <c r="U15" s="9" t="inlineStr">
-        <is>
-          <t>Total Requests 
-per working day</t>
-        </is>
-      </c>
-      <c r="V15" s="9" t="inlineStr">
-        <is>
-          <t>Processed Requests per working day</t>
-        </is>
-      </c>
-      <c r="W15" s="9" t="inlineStr">
-        <is>
-          <t>Diverted Requests per working day</t>
-        </is>
-      </c>
-      <c r="X15" s="22" t="n"/>
-      <c r="Y15" s="61" t="inlineStr">
-        <is>
-          <t>Total Requests 
-per working day</t>
-        </is>
-      </c>
-      <c r="Z15" s="61" t="inlineStr">
-        <is>
-          <t>Processed Requests per working day</t>
-        </is>
-      </c>
-      <c r="AA15" s="61" t="inlineStr">
-        <is>
-          <t>Diverted Requests per working day</t>
-        </is>
-      </c>
-      <c r="AB15" s="22" t="n"/>
-      <c r="AC15" s="61" t="inlineStr">
-        <is>
-          <t>Total Requests 
-per working day</t>
-        </is>
-      </c>
-      <c r="AD15" s="61" t="inlineStr">
-        <is>
-          <t>Processed Requests per working day</t>
-        </is>
-      </c>
-      <c r="AE15" s="61" t="inlineStr">
-        <is>
-          <t>Diverted Requests per working day</t>
-        </is>
-      </c>
-      <c r="AF15" s="22" t="n"/>
-      <c r="AG15" s="61" t="inlineStr">
-        <is>
-          <t>Total Requests 
-per working day</t>
-        </is>
-      </c>
-      <c r="AH15" s="61" t="inlineStr">
-        <is>
-          <t>Processed Requests per working day</t>
-        </is>
-      </c>
-      <c r="AI15" s="61" t="inlineStr">
-        <is>
-          <t>Diverted Requests per working day</t>
-        </is>
-      </c>
-      <c r="AJ15" s="1" t="n"/>
-      <c r="AK15" s="28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">No. of working days </t>
         </is>
       </c>
     </row>
@@ -1650,62 +1535,6 @@
         <v>560</v>
       </c>
       <c r="S16" s="12" t="n"/>
-      <c r="T16" s="11">
-        <f>B16</f>
-        <v/>
-      </c>
-      <c r="U16" s="13">
-        <f>C16/$AK16</f>
-        <v/>
-      </c>
-      <c r="V16" s="13">
-        <f>D16/$AK16</f>
-        <v/>
-      </c>
-      <c r="W16" s="13">
-        <f>E16/$AK16</f>
-        <v/>
-      </c>
-      <c r="Y16" s="13">
-        <f>G16/$AK16</f>
-        <v/>
-      </c>
-      <c r="Z16" s="13">
-        <f>H16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AA16" s="13">
-        <f>I16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AC16" s="13">
-        <f>K16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AD16" s="13">
-        <f>L16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AE16" s="13">
-        <f>M16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AG16" s="13">
-        <f>O16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AH16" s="13">
-        <f>P16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AI16" s="13">
-        <f>Q16/$AK16</f>
-        <v/>
-      </c>
-      <c r="AJ16" s="12" t="n"/>
-      <c r="AK16" s="27" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="B17" s="11" t="inlineStr">
@@ -1753,62 +1582,6 @@
         <v>685</v>
       </c>
       <c r="S17" s="12" t="n"/>
-      <c r="T17" s="11">
-        <f>B17</f>
-        <v/>
-      </c>
-      <c r="U17" s="13">
-        <f>C17/$AK17</f>
-        <v/>
-      </c>
-      <c r="V17" s="13">
-        <f>D17/$AK17</f>
-        <v/>
-      </c>
-      <c r="W17" s="13">
-        <f>E17/$AK17</f>
-        <v/>
-      </c>
-      <c r="Y17" s="13">
-        <f>G17/$AK17</f>
-        <v/>
-      </c>
-      <c r="Z17" s="13">
-        <f>H17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AA17" s="13">
-        <f>I17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AC17" s="13">
-        <f>K17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AD17" s="13">
-        <f>L17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AE17" s="13">
-        <f>M17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AG17" s="13">
-        <f>O17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AH17" s="13">
-        <f>P17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AI17" s="13">
-        <f>Q17/$AK17</f>
-        <v/>
-      </c>
-      <c r="AJ17" s="12" t="n"/>
-      <c r="AK17" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="B18" s="11" t="inlineStr">
@@ -1856,62 +1629,6 @@
         <v>239</v>
       </c>
       <c r="S18" s="12" t="n"/>
-      <c r="T18" s="11">
-        <f>B18</f>
-        <v/>
-      </c>
-      <c r="U18" s="13">
-        <f>C18/$AK18</f>
-        <v/>
-      </c>
-      <c r="V18" s="13">
-        <f>D18/$AK18</f>
-        <v/>
-      </c>
-      <c r="W18" s="13">
-        <f>E18/$AK18</f>
-        <v/>
-      </c>
-      <c r="Y18" s="13">
-        <f>G18/$AK18</f>
-        <v/>
-      </c>
-      <c r="Z18" s="13">
-        <f>H18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AA18" s="13">
-        <f>I18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AC18" s="13">
-        <f>K18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AD18" s="13">
-        <f>L18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AE18" s="13">
-        <f>M18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AG18" s="13">
-        <f>O18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AH18" s="13">
-        <f>P18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AI18" s="13">
-        <f>Q18/$AK18</f>
-        <v/>
-      </c>
-      <c r="AJ18" s="12" t="n"/>
-      <c r="AK18" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="B19" s="11" t="inlineStr">
@@ -1959,62 +1676,6 @@
         <v>33</v>
       </c>
       <c r="S19" s="12" t="n"/>
-      <c r="T19" s="11">
-        <f>B19</f>
-        <v/>
-      </c>
-      <c r="U19" s="13">
-        <f>C19/$AK19</f>
-        <v/>
-      </c>
-      <c r="V19" s="13">
-        <f>D19/$AK19</f>
-        <v/>
-      </c>
-      <c r="W19" s="13">
-        <f>E19/$AK19</f>
-        <v/>
-      </c>
-      <c r="Y19" s="13">
-        <f>G19/$AK19</f>
-        <v/>
-      </c>
-      <c r="Z19" s="13">
-        <f>H19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AA19" s="13">
-        <f>I19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AC19" s="13">
-        <f>K19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AD19" s="13">
-        <f>L19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AE19" s="13">
-        <f>M19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AG19" s="13">
-        <f>O19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AH19" s="13">
-        <f>P19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AI19" s="13">
-        <f>Q19/$AK19</f>
-        <v/>
-      </c>
-      <c r="AJ19" s="12" t="n"/>
-      <c r="AK19" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="B20" s="11" t="inlineStr">
@@ -2062,62 +1723,6 @@
         <v>4</v>
       </c>
       <c r="S20" s="12" t="n"/>
-      <c r="T20" s="11">
-        <f>B20</f>
-        <v/>
-      </c>
-      <c r="U20" s="13">
-        <f>C20/$AK20</f>
-        <v/>
-      </c>
-      <c r="V20" s="13">
-        <f>D20/$AK20</f>
-        <v/>
-      </c>
-      <c r="W20" s="13">
-        <f>E20/$AK20</f>
-        <v/>
-      </c>
-      <c r="Y20" s="13">
-        <f>G20/$AK20</f>
-        <v/>
-      </c>
-      <c r="Z20" s="13">
-        <f>H20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AA20" s="13">
-        <f>I20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AC20" s="13">
-        <f>K20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AD20" s="13">
-        <f>L20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AE20" s="13">
-        <f>M20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AG20" s="13">
-        <f>O20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AH20" s="13">
-        <f>P20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AI20" s="13">
-        <f>Q20/$AK20</f>
-        <v/>
-      </c>
-      <c r="AJ20" s="12" t="n"/>
-      <c r="AK20" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="B21" s="11" t="inlineStr">
@@ -2165,62 +1770,6 @@
         <v>1</v>
       </c>
       <c r="S21" s="12" t="n"/>
-      <c r="T21" s="11">
-        <f>B21</f>
-        <v/>
-      </c>
-      <c r="U21" s="13">
-        <f>C21/$AK21</f>
-        <v/>
-      </c>
-      <c r="V21" s="13">
-        <f>D21/$AK21</f>
-        <v/>
-      </c>
-      <c r="W21" s="13">
-        <f>E21/$AK21</f>
-        <v/>
-      </c>
-      <c r="Y21" s="13">
-        <f>G21/$AK21</f>
-        <v/>
-      </c>
-      <c r="Z21" s="13">
-        <f>H21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AA21" s="13">
-        <f>I21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AC21" s="13">
-        <f>K21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AD21" s="13">
-        <f>L21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AE21" s="13">
-        <f>M21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AG21" s="13">
-        <f>O21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AH21" s="13">
-        <f>P21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AI21" s="13">
-        <f>Q21/$AK21</f>
-        <v/>
-      </c>
-      <c r="AJ21" s="15" t="n"/>
-      <c r="AK21" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="B22" s="11" t="inlineStr">
@@ -2268,62 +1817,6 @@
         <v/>
       </c>
       <c r="S22" s="12" t="n"/>
-      <c r="T22" s="11">
-        <f>B22</f>
-        <v/>
-      </c>
-      <c r="U22" s="13">
-        <f>C22/$AK22</f>
-        <v/>
-      </c>
-      <c r="V22" s="13">
-        <f>D22/$AK22</f>
-        <v/>
-      </c>
-      <c r="W22" s="13">
-        <f>E22/$AK22</f>
-        <v/>
-      </c>
-      <c r="Y22" s="13">
-        <f>G22/$AK22</f>
-        <v/>
-      </c>
-      <c r="Z22" s="13">
-        <f>H22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AA22" s="13">
-        <f>I22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AC22" s="13">
-        <f>K22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AD22" s="13">
-        <f>L22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AE22" s="13">
-        <f>M22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AG22" s="13">
-        <f>O22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AH22" s="13">
-        <f>P22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AI22" s="13">
-        <f>Q22/$AK22</f>
-        <v/>
-      </c>
-      <c r="AJ22" s="15" t="n"/>
-      <c r="AK22" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="B23" s="11" t="inlineStr">
@@ -2371,62 +1864,6 @@
         <v/>
       </c>
       <c r="S23" s="12" t="n"/>
-      <c r="T23" s="11">
-        <f>B23</f>
-        <v/>
-      </c>
-      <c r="U23" s="13">
-        <f>C23/$AK23</f>
-        <v/>
-      </c>
-      <c r="V23" s="13">
-        <f>D23/$AK23</f>
-        <v/>
-      </c>
-      <c r="W23" s="13">
-        <f>E23/$AK23</f>
-        <v/>
-      </c>
-      <c r="Y23" s="13">
-        <f>G23/$AK23</f>
-        <v/>
-      </c>
-      <c r="Z23" s="13">
-        <f>H23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AA23" s="13">
-        <f>I23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AC23" s="13">
-        <f>K23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AD23" s="13">
-        <f>L23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AE23" s="13">
-        <f>M23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AG23" s="13">
-        <f>O23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AH23" s="13">
-        <f>P23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AI23" s="13">
-        <f>Q23/$AK23</f>
-        <v/>
-      </c>
-      <c r="AJ23" s="15" t="n"/>
-      <c r="AK23" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="B24" s="11" t="inlineStr">
@@ -2474,62 +1911,6 @@
         <v/>
       </c>
       <c r="S24" s="12" t="n"/>
-      <c r="T24" s="11">
-        <f>B24</f>
-        <v/>
-      </c>
-      <c r="U24" s="13">
-        <f>C24/$AK24</f>
-        <v/>
-      </c>
-      <c r="V24" s="13">
-        <f>D24/$AK24</f>
-        <v/>
-      </c>
-      <c r="W24" s="13">
-        <f>E24/$AK24</f>
-        <v/>
-      </c>
-      <c r="Y24" s="13">
-        <f>G24/$AK24</f>
-        <v/>
-      </c>
-      <c r="Z24" s="13">
-        <f>H24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AA24" s="13">
-        <f>I24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AC24" s="13">
-        <f>K24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AD24" s="13">
-        <f>L24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AE24" s="13">
-        <f>M24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AG24" s="13">
-        <f>O24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AH24" s="13">
-        <f>P24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AI24" s="13">
-        <f>Q24/$AK24</f>
-        <v/>
-      </c>
-      <c r="AJ24" s="15" t="n"/>
-      <c r="AK24" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="B25" s="11" t="inlineStr">
@@ -2577,62 +1958,6 @@
         <v>8</v>
       </c>
       <c r="S25" s="12" t="n"/>
-      <c r="T25" s="11">
-        <f>B25</f>
-        <v/>
-      </c>
-      <c r="U25" s="13">
-        <f>C25/$AK25</f>
-        <v/>
-      </c>
-      <c r="V25" s="13">
-        <f>D25/$AK25</f>
-        <v/>
-      </c>
-      <c r="W25" s="13">
-        <f>E25/$AK25</f>
-        <v/>
-      </c>
-      <c r="Y25" s="13">
-        <f>G25/$AK25</f>
-        <v/>
-      </c>
-      <c r="Z25" s="13">
-        <f>H25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AA25" s="13">
-        <f>I25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AC25" s="13">
-        <f>K25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AD25" s="13">
-        <f>L25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AE25" s="13">
-        <f>M25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AG25" s="13">
-        <f>O25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AH25" s="13">
-        <f>P25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AI25" s="13">
-        <f>Q25/$AK25</f>
-        <v/>
-      </c>
-      <c r="AJ25" s="15" t="n"/>
-      <c r="AK25" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="B26" s="11" t="inlineStr">
@@ -2680,62 +2005,6 @@
         <v/>
       </c>
       <c r="S26" s="12" t="n"/>
-      <c r="T26" s="11">
-        <f>B26</f>
-        <v/>
-      </c>
-      <c r="U26" s="13">
-        <f>C26/$AK26</f>
-        <v/>
-      </c>
-      <c r="V26" s="13">
-        <f>D26/$AK26</f>
-        <v/>
-      </c>
-      <c r="W26" s="13">
-        <f>E26/$AK26</f>
-        <v/>
-      </c>
-      <c r="Y26" s="13">
-        <f>G26/$AK26</f>
-        <v/>
-      </c>
-      <c r="Z26" s="13">
-        <f>H26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AA26" s="13">
-        <f>I26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AC26" s="13">
-        <f>K26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AD26" s="13">
-        <f>L26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AE26" s="13">
-        <f>M26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AG26" s="13">
-        <f>O26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AH26" s="13">
-        <f>P26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AI26" s="13">
-        <f>Q26/$AK26</f>
-        <v/>
-      </c>
-      <c r="AJ26" s="15" t="n"/>
-      <c r="AK26" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="27" ht="15" customHeight="1">
       <c r="B27" s="11" t="inlineStr">
@@ -2783,62 +2052,6 @@
         <v/>
       </c>
       <c r="S27" s="12" t="n"/>
-      <c r="T27" s="11">
-        <f>B27</f>
-        <v/>
-      </c>
-      <c r="U27" s="13">
-        <f>C27/$AK27</f>
-        <v/>
-      </c>
-      <c r="V27" s="13">
-        <f>D27/$AK27</f>
-        <v/>
-      </c>
-      <c r="W27" s="13">
-        <f>E27/$AK27</f>
-        <v/>
-      </c>
-      <c r="Y27" s="13">
-        <f>G27/$AK27</f>
-        <v/>
-      </c>
-      <c r="Z27" s="13">
-        <f>H27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AA27" s="13">
-        <f>I27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AC27" s="13">
-        <f>K27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AD27" s="13">
-        <f>L27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AE27" s="13">
-        <f>M27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AG27" s="13">
-        <f>O27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AH27" s="13">
-        <f>P27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AI27" s="13">
-        <f>Q27/$AK27</f>
-        <v/>
-      </c>
-      <c r="AJ27" s="15" t="n"/>
-      <c r="AK27" s="27" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="B28" s="11" t="inlineStr">
@@ -2886,62 +2099,6 @@
         <v>1042</v>
       </c>
       <c r="S28" s="12" t="n"/>
-      <c r="T28" s="11">
-        <f>B28</f>
-        <v/>
-      </c>
-      <c r="U28" s="13">
-        <f>C28/$AK28</f>
-        <v/>
-      </c>
-      <c r="V28" s="13">
-        <f>D28/$AK28</f>
-        <v/>
-      </c>
-      <c r="W28" s="13">
-        <f>E28/$AK28</f>
-        <v/>
-      </c>
-      <c r="Y28" s="13">
-        <f>G28/$AK28</f>
-        <v/>
-      </c>
-      <c r="Z28" s="13">
-        <f>H28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AA28" s="13">
-        <f>I28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AC28" s="13">
-        <f>K28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AD28" s="13">
-        <f>L28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AE28" s="13">
-        <f>M28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AG28" s="13">
-        <f>O28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AH28" s="13">
-        <f>P28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AI28" s="13">
-        <f>Q28/$AK28</f>
-        <v/>
-      </c>
-      <c r="AJ28" s="15" t="n"/>
-      <c r="AK28" s="27" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="29" ht="15" customHeight="1">
       <c r="B29" s="11" t="inlineStr">
@@ -2989,62 +2146,6 @@
         <v>1122</v>
       </c>
       <c r="S29" s="12" t="n"/>
-      <c r="T29" s="11">
-        <f>B29</f>
-        <v/>
-      </c>
-      <c r="U29" s="13">
-        <f>C29/$AK29</f>
-        <v/>
-      </c>
-      <c r="V29" s="13">
-        <f>D29/$AK29</f>
-        <v/>
-      </c>
-      <c r="W29" s="13">
-        <f>E29/$AK29</f>
-        <v/>
-      </c>
-      <c r="Y29" s="13">
-        <f>G29/$AK29</f>
-        <v/>
-      </c>
-      <c r="Z29" s="13">
-        <f>H29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AA29" s="13">
-        <f>I29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AC29" s="13">
-        <f>K29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AD29" s="13">
-        <f>L29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AE29" s="13">
-        <f>M29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AG29" s="13">
-        <f>O29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AH29" s="13">
-        <f>P29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AI29" s="13">
-        <f>Q29/$AK29</f>
-        <v/>
-      </c>
-      <c r="AJ29" s="15" t="n"/>
-      <c r="AK29" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="30" ht="15" customHeight="1">
       <c r="B30" s="11" t="inlineStr">
@@ -3092,62 +2193,6 @@
         <v>1352</v>
       </c>
       <c r="S30" s="12" t="n"/>
-      <c r="T30" s="11">
-        <f>B30</f>
-        <v/>
-      </c>
-      <c r="U30" s="13">
-        <f>C30/$AK30</f>
-        <v/>
-      </c>
-      <c r="V30" s="13">
-        <f>D30/$AK30</f>
-        <v/>
-      </c>
-      <c r="W30" s="13">
-        <f>E30/$AK30</f>
-        <v/>
-      </c>
-      <c r="Y30" s="13">
-        <f>G30/$AK30</f>
-        <v/>
-      </c>
-      <c r="Z30" s="13">
-        <f>H30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AA30" s="13">
-        <f>I30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AC30" s="13">
-        <f>K30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AD30" s="13">
-        <f>L30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AE30" s="13">
-        <f>M30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AG30" s="13">
-        <f>O30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AH30" s="13">
-        <f>P30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AI30" s="13">
-        <f>Q30/$AK30</f>
-        <v/>
-      </c>
-      <c r="AJ30" s="15" t="n"/>
-      <c r="AK30" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="B31" s="11" t="inlineStr">
@@ -3195,62 +2240,6 @@
         <v>1197</v>
       </c>
       <c r="S31" s="12" t="n"/>
-      <c r="T31" s="11">
-        <f>B31</f>
-        <v/>
-      </c>
-      <c r="U31" s="13">
-        <f>C31/$AK31</f>
-        <v/>
-      </c>
-      <c r="V31" s="13">
-        <f>D31/$AK31</f>
-        <v/>
-      </c>
-      <c r="W31" s="13">
-        <f>E31/$AK31</f>
-        <v/>
-      </c>
-      <c r="Y31" s="13">
-        <f>G31/$AK31</f>
-        <v/>
-      </c>
-      <c r="Z31" s="13">
-        <f>H31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AA31" s="13">
-        <f>I31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AC31" s="13">
-        <f>K31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AD31" s="13">
-        <f>L31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AE31" s="13">
-        <f>M31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AG31" s="13">
-        <f>O31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AH31" s="13">
-        <f>P31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AI31" s="13">
-        <f>Q31/$AK31</f>
-        <v/>
-      </c>
-      <c r="AJ31" s="15" t="n"/>
-      <c r="AK31" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="32" ht="15" customHeight="1">
       <c r="B32" s="11" t="inlineStr">
@@ -3298,62 +2287,6 @@
         <v>1220</v>
       </c>
       <c r="S32" s="12" t="n"/>
-      <c r="T32" s="11">
-        <f>B32</f>
-        <v/>
-      </c>
-      <c r="U32" s="13">
-        <f>C32/$AK32</f>
-        <v/>
-      </c>
-      <c r="V32" s="13">
-        <f>D32/$AK32</f>
-        <v/>
-      </c>
-      <c r="W32" s="13">
-        <f>E32/$AK32</f>
-        <v/>
-      </c>
-      <c r="Y32" s="13">
-        <f>G32/$AK32</f>
-        <v/>
-      </c>
-      <c r="Z32" s="13">
-        <f>H32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AA32" s="13">
-        <f>I32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AC32" s="13">
-        <f>K32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AD32" s="13">
-        <f>L32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AE32" s="13">
-        <f>M32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AG32" s="13">
-        <f>O32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AH32" s="13">
-        <f>P32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AI32" s="13">
-        <f>Q32/$AK32</f>
-        <v/>
-      </c>
-      <c r="AJ32" s="15" t="n"/>
-      <c r="AK32" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="33" ht="15" customHeight="1">
       <c r="B33" s="11" t="inlineStr">
@@ -3401,62 +2334,6 @@
         <v>1126</v>
       </c>
       <c r="S33" s="12" t="n"/>
-      <c r="T33" s="11">
-        <f>B33</f>
-        <v/>
-      </c>
-      <c r="U33" s="13">
-        <f>C33/$AK33</f>
-        <v/>
-      </c>
-      <c r="V33" s="13">
-        <f>D33/$AK33</f>
-        <v/>
-      </c>
-      <c r="W33" s="13">
-        <f>E33/$AK33</f>
-        <v/>
-      </c>
-      <c r="Y33" s="13">
-        <f>G33/$AK33</f>
-        <v/>
-      </c>
-      <c r="Z33" s="13">
-        <f>H33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AA33" s="13">
-        <f>I33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AC33" s="13">
-        <f>K33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AD33" s="13">
-        <f>L33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AE33" s="13">
-        <f>M33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AG33" s="13">
-        <f>O33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AH33" s="13">
-        <f>P33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AI33" s="13">
-        <f>Q33/$AK33</f>
-        <v/>
-      </c>
-      <c r="AJ33" s="12" t="n"/>
-      <c r="AK33" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="34" ht="15" customHeight="1">
       <c r="B34" s="11" t="inlineStr">
@@ -3504,62 +2381,6 @@
         <v>1246</v>
       </c>
       <c r="S34" s="12" t="n"/>
-      <c r="T34" s="11">
-        <f>B34</f>
-        <v/>
-      </c>
-      <c r="U34" s="13">
-        <f>C34/$AK34</f>
-        <v/>
-      </c>
-      <c r="V34" s="13">
-        <f>D34/$AK34</f>
-        <v/>
-      </c>
-      <c r="W34" s="13">
-        <f>E34/$AK34</f>
-        <v/>
-      </c>
-      <c r="Y34" s="13">
-        <f>G34/$AK34</f>
-        <v/>
-      </c>
-      <c r="Z34" s="13">
-        <f>H34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AA34" s="13">
-        <f>I34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AC34" s="13">
-        <f>K34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AD34" s="13">
-        <f>L34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AE34" s="13">
-        <f>M34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AG34" s="13">
-        <f>O34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AH34" s="13">
-        <f>P34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AI34" s="13">
-        <f>Q34/$AK34</f>
-        <v/>
-      </c>
-      <c r="AJ34" s="12" t="n"/>
-      <c r="AK34" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="B35" s="11" t="inlineStr">
@@ -3607,62 +2428,6 @@
         <v>1303</v>
       </c>
       <c r="S35" s="12" t="n"/>
-      <c r="T35" s="11">
-        <f>B35</f>
-        <v/>
-      </c>
-      <c r="U35" s="13">
-        <f>C35/$AK35</f>
-        <v/>
-      </c>
-      <c r="V35" s="13">
-        <f>D35/$AK35</f>
-        <v/>
-      </c>
-      <c r="W35" s="13">
-        <f>E35/$AK35</f>
-        <v/>
-      </c>
-      <c r="Y35" s="13">
-        <f>G35/$AK35</f>
-        <v/>
-      </c>
-      <c r="Z35" s="13">
-        <f>H35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AA35" s="13">
-        <f>I35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AC35" s="13">
-        <f>K35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AD35" s="13">
-        <f>L35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AE35" s="13">
-        <f>M35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AG35" s="13">
-        <f>O35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AH35" s="13">
-        <f>P35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AI35" s="13">
-        <f>Q35/$AK35</f>
-        <v/>
-      </c>
-      <c r="AJ35" s="12" t="n"/>
-      <c r="AK35" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="B36" s="11" t="inlineStr">
@@ -3710,62 +2475,6 @@
         <v>1157</v>
       </c>
       <c r="S36" s="12" t="n"/>
-      <c r="T36" s="11">
-        <f>B36</f>
-        <v/>
-      </c>
-      <c r="U36" s="13">
-        <f>C36/$AK36</f>
-        <v/>
-      </c>
-      <c r="V36" s="13">
-        <f>D36/$AK36</f>
-        <v/>
-      </c>
-      <c r="W36" s="13">
-        <f>E36/$AK36</f>
-        <v/>
-      </c>
-      <c r="Y36" s="13">
-        <f>G36/$AK36</f>
-        <v/>
-      </c>
-      <c r="Z36" s="13">
-        <f>H36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AA36" s="13">
-        <f>I36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AC36" s="13">
-        <f>K36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AD36" s="13">
-        <f>L36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AE36" s="13">
-        <f>M36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AG36" s="13">
-        <f>O36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AH36" s="13">
-        <f>P36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AI36" s="13">
-        <f>Q36/$AK36</f>
-        <v/>
-      </c>
-      <c r="AJ36" s="12" t="n"/>
-      <c r="AK36" s="27" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="B37" s="11" t="inlineStr">
@@ -3813,62 +2522,6 @@
         <v>1442</v>
       </c>
       <c r="S37" s="12" t="n"/>
-      <c r="T37" s="11">
-        <f>B37</f>
-        <v/>
-      </c>
-      <c r="U37" s="13">
-        <f>C37/$AK37</f>
-        <v/>
-      </c>
-      <c r="V37" s="13">
-        <f>D37/$AK37</f>
-        <v/>
-      </c>
-      <c r="W37" s="13">
-        <f>E37/$AK37</f>
-        <v/>
-      </c>
-      <c r="Y37" s="13">
-        <f>G37/$AK37</f>
-        <v/>
-      </c>
-      <c r="Z37" s="13">
-        <f>H37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AA37" s="13">
-        <f>I37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AC37" s="13">
-        <f>K37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AD37" s="13">
-        <f>L37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AE37" s="13">
-        <f>M37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AG37" s="13">
-        <f>O37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AH37" s="13">
-        <f>P37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AI37" s="13">
-        <f>Q37/$AK37</f>
-        <v/>
-      </c>
-      <c r="AJ37" s="12" t="n"/>
-      <c r="AK37" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="38" ht="15" customHeight="1">
       <c r="B38" s="11" t="inlineStr">
@@ -3916,62 +2569,6 @@
         <v>1245</v>
       </c>
       <c r="S38" s="12" t="n"/>
-      <c r="T38" s="11">
-        <f>B38</f>
-        <v/>
-      </c>
-      <c r="U38" s="13">
-        <f>C38/$AK38</f>
-        <v/>
-      </c>
-      <c r="V38" s="13">
-        <f>D38/$AK38</f>
-        <v/>
-      </c>
-      <c r="W38" s="13">
-        <f>E38/$AK38</f>
-        <v/>
-      </c>
-      <c r="Y38" s="13">
-        <f>G38/$AK38</f>
-        <v/>
-      </c>
-      <c r="Z38" s="13">
-        <f>H38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AA38" s="13">
-        <f>I38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AC38" s="13">
-        <f>K38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AD38" s="13">
-        <f>L38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AE38" s="13">
-        <f>M38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AG38" s="13">
-        <f>O38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AH38" s="13">
-        <f>P38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AI38" s="13">
-        <f>Q38/$AK38</f>
-        <v/>
-      </c>
-      <c r="AJ38" s="12" t="n"/>
-      <c r="AK38" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="39" ht="15" customHeight="1">
       <c r="B39" s="11" t="inlineStr">
@@ -4019,62 +2616,6 @@
         <v>1260</v>
       </c>
       <c r="S39" s="12" t="n"/>
-      <c r="T39" s="11">
-        <f>B39</f>
-        <v/>
-      </c>
-      <c r="U39" s="13">
-        <f>C39/$AK39</f>
-        <v/>
-      </c>
-      <c r="V39" s="13">
-        <f>D39/$AK39</f>
-        <v/>
-      </c>
-      <c r="W39" s="13">
-        <f>E39/$AK39</f>
-        <v/>
-      </c>
-      <c r="Y39" s="13">
-        <f>G39/$AK39</f>
-        <v/>
-      </c>
-      <c r="Z39" s="13">
-        <f>H39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AA39" s="13">
-        <f>I39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AC39" s="13">
-        <f>K39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AD39" s="13">
-        <f>L39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AE39" s="13">
-        <f>M39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AG39" s="13">
-        <f>O39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AH39" s="13">
-        <f>P39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AI39" s="13">
-        <f>Q39/$AK39</f>
-        <v/>
-      </c>
-      <c r="AJ39" s="12" t="n"/>
-      <c r="AK39" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="40" ht="15" customHeight="1">
       <c r="B40" s="11" t="inlineStr">
@@ -4122,62 +2663,6 @@
         <v>2103</v>
       </c>
       <c r="S40" s="12" t="n"/>
-      <c r="T40" s="11">
-        <f>B40</f>
-        <v/>
-      </c>
-      <c r="U40" s="13">
-        <f>C40/$AK40</f>
-        <v/>
-      </c>
-      <c r="V40" s="13">
-        <f>D40/$AK40</f>
-        <v/>
-      </c>
-      <c r="W40" s="13">
-        <f>E40/$AK40</f>
-        <v/>
-      </c>
-      <c r="Y40" s="13">
-        <f>G40/$AK40</f>
-        <v/>
-      </c>
-      <c r="Z40" s="13">
-        <f>H40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AA40" s="13">
-        <f>I40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AC40" s="13">
-        <f>K40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AD40" s="13">
-        <f>L40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AE40" s="13">
-        <f>M40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AG40" s="13">
-        <f>O40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AH40" s="13">
-        <f>P40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AI40" s="13">
-        <f>Q40/$AK40</f>
-        <v/>
-      </c>
-      <c r="AJ40" s="12" t="n"/>
-      <c r="AK40" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="B41" s="11" t="inlineStr">
@@ -4225,62 +2710,6 @@
         <v>2447</v>
       </c>
       <c r="S41" s="12" t="n"/>
-      <c r="T41" s="11">
-        <f>B41</f>
-        <v/>
-      </c>
-      <c r="U41" s="13">
-        <f>C41/$AK41</f>
-        <v/>
-      </c>
-      <c r="V41" s="13">
-        <f>D41/$AK41</f>
-        <v/>
-      </c>
-      <c r="W41" s="13">
-        <f>E41/$AK41</f>
-        <v/>
-      </c>
-      <c r="Y41" s="13">
-        <f>G41/$AK41</f>
-        <v/>
-      </c>
-      <c r="Z41" s="13">
-        <f>H41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AA41" s="13">
-        <f>I41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AC41" s="13">
-        <f>K41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AD41" s="13">
-        <f>L41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AE41" s="13">
-        <f>M41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AG41" s="13">
-        <f>O41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AH41" s="13">
-        <f>P41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AI41" s="13">
-        <f>Q41/$AK41</f>
-        <v/>
-      </c>
-      <c r="AJ41" s="12" t="n"/>
-      <c r="AK41" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="B42" s="11" t="inlineStr">
@@ -4328,62 +2757,6 @@
         <v>2176</v>
       </c>
       <c r="S42" s="12" t="n"/>
-      <c r="T42" s="11">
-        <f>B42</f>
-        <v/>
-      </c>
-      <c r="U42" s="13">
-        <f>C42/$AK42</f>
-        <v/>
-      </c>
-      <c r="V42" s="13">
-        <f>D42/$AK42</f>
-        <v/>
-      </c>
-      <c r="W42" s="13">
-        <f>E42/$AK42</f>
-        <v/>
-      </c>
-      <c r="Y42" s="13">
-        <f>G42/$AK42</f>
-        <v/>
-      </c>
-      <c r="Z42" s="13">
-        <f>H42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AA42" s="13">
-        <f>I42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AC42" s="13">
-        <f>K42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AD42" s="13">
-        <f>L42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AE42" s="13">
-        <f>M42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AG42" s="13">
-        <f>O42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AH42" s="13">
-        <f>P42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AI42" s="13">
-        <f>Q42/$AK42</f>
-        <v/>
-      </c>
-      <c r="AJ42" s="12" t="n"/>
-      <c r="AK42" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="43" ht="15" customHeight="1">
       <c r="B43" s="11" t="inlineStr">
@@ -4431,62 +2804,6 @@
         <v>2402</v>
       </c>
       <c r="S43" s="12" t="n"/>
-      <c r="T43" s="11">
-        <f>B43</f>
-        <v/>
-      </c>
-      <c r="U43" s="13">
-        <f>C43/$AK43</f>
-        <v/>
-      </c>
-      <c r="V43" s="13">
-        <f>D43/$AK43</f>
-        <v/>
-      </c>
-      <c r="W43" s="13">
-        <f>E43/$AK43</f>
-        <v/>
-      </c>
-      <c r="Y43" s="13">
-        <f>G43/$AK43</f>
-        <v/>
-      </c>
-      <c r="Z43" s="13">
-        <f>H43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AA43" s="13">
-        <f>I43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AC43" s="13">
-        <f>K43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AD43" s="13">
-        <f>L43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AE43" s="13">
-        <f>M43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AG43" s="13">
-        <f>O43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AH43" s="13">
-        <f>P43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AI43" s="13">
-        <f>Q43/$AK43</f>
-        <v/>
-      </c>
-      <c r="AJ43" s="12" t="n"/>
-      <c r="AK43" s="27" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="44" ht="15" customHeight="1">
       <c r="B44" s="11" t="inlineStr">
@@ -4534,62 +2851,6 @@
         <v>2094</v>
       </c>
       <c r="S44" s="12" t="n"/>
-      <c r="T44" s="11">
-        <f>B44</f>
-        <v/>
-      </c>
-      <c r="U44" s="13">
-        <f>C44/$AK44</f>
-        <v/>
-      </c>
-      <c r="V44" s="13">
-        <f>D44/$AK44</f>
-        <v/>
-      </c>
-      <c r="W44" s="13">
-        <f>E44/$AK44</f>
-        <v/>
-      </c>
-      <c r="Y44" s="13">
-        <f>G44/$AK44</f>
-        <v/>
-      </c>
-      <c r="Z44" s="13">
-        <f>H44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AA44" s="13">
-        <f>I44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AC44" s="13">
-        <f>K44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AD44" s="13">
-        <f>L44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AE44" s="13">
-        <f>M44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AG44" s="13">
-        <f>O44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AH44" s="13">
-        <f>P44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AI44" s="13">
-        <f>Q44/$AK44</f>
-        <v/>
-      </c>
-      <c r="AJ44" s="12" t="n"/>
-      <c r="AK44" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="45" ht="15" customHeight="1">
       <c r="B45" s="11" t="inlineStr">
@@ -4637,61 +2898,6 @@
         <v>2190</v>
       </c>
       <c r="S45" s="12" t="n"/>
-      <c r="T45" s="11">
-        <f>B45</f>
-        <v/>
-      </c>
-      <c r="U45" s="13">
-        <f>C45/$AK45</f>
-        <v/>
-      </c>
-      <c r="V45" s="13">
-        <f>D45/$AK45</f>
-        <v/>
-      </c>
-      <c r="W45" s="13">
-        <f>E45/$AK45</f>
-        <v/>
-      </c>
-      <c r="Y45" s="13">
-        <f>G45/$AK45</f>
-        <v/>
-      </c>
-      <c r="Z45" s="13">
-        <f>H45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AA45" s="13">
-        <f>I45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AC45" s="13">
-        <f>K45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AD45" s="13">
-        <f>L45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AE45" s="13">
-        <f>M45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AG45" s="13">
-        <f>O45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AH45" s="13">
-        <f>P45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AI45" s="13">
-        <f>Q45/$AK45</f>
-        <v/>
-      </c>
-      <c r="AK45" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="46" ht="15" customHeight="1">
       <c r="B46" s="11" t="inlineStr">
@@ -4739,61 +2945,6 @@
         <v>2467</v>
       </c>
       <c r="S46" s="12" t="n"/>
-      <c r="T46" s="11">
-        <f>B46</f>
-        <v/>
-      </c>
-      <c r="U46" s="13">
-        <f>C46/$AK46</f>
-        <v/>
-      </c>
-      <c r="V46" s="13">
-        <f>D46/$AK46</f>
-        <v/>
-      </c>
-      <c r="W46" s="13">
-        <f>E46/$AK46</f>
-        <v/>
-      </c>
-      <c r="Y46" s="13">
-        <f>G46/$AK46</f>
-        <v/>
-      </c>
-      <c r="Z46" s="13">
-        <f>H46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AA46" s="13">
-        <f>I46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AC46" s="13">
-        <f>K46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AD46" s="13">
-        <f>L46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AE46" s="13">
-        <f>M46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AG46" s="13">
-        <f>O46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AH46" s="13">
-        <f>P46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AI46" s="13">
-        <f>Q46/$AK46</f>
-        <v/>
-      </c>
-      <c r="AK46" s="27" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="B47" s="11" t="inlineStr">
@@ -4841,61 +2992,6 @@
         <v>2179</v>
       </c>
       <c r="S47" s="12" t="n"/>
-      <c r="T47" s="11">
-        <f>B47</f>
-        <v/>
-      </c>
-      <c r="U47" s="13">
-        <f>C47/$AK47</f>
-        <v/>
-      </c>
-      <c r="V47" s="13">
-        <f>D47/$AK47</f>
-        <v/>
-      </c>
-      <c r="W47" s="13">
-        <f>E47/$AK47</f>
-        <v/>
-      </c>
-      <c r="Y47" s="13">
-        <f>G47/$AK47</f>
-        <v/>
-      </c>
-      <c r="Z47" s="13">
-        <f>H47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AA47" s="13">
-        <f>I47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AC47" s="13">
-        <f>K47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AD47" s="13">
-        <f>L47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AE47" s="13">
-        <f>M47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AG47" s="13">
-        <f>O47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AH47" s="13">
-        <f>P47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AI47" s="13">
-        <f>Q47/$AK47</f>
-        <v/>
-      </c>
-      <c r="AK47" s="27" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="B48" s="11" t="inlineStr">
@@ -4943,61 +3039,6 @@
         <v>1999</v>
       </c>
       <c r="S48" s="12" t="n"/>
-      <c r="T48" s="11">
-        <f>B48</f>
-        <v/>
-      </c>
-      <c r="U48" s="13">
-        <f>C48/$AK48</f>
-        <v/>
-      </c>
-      <c r="V48" s="13">
-        <f>D48/$AK48</f>
-        <v/>
-      </c>
-      <c r="W48" s="13">
-        <f>E48/$AK48</f>
-        <v/>
-      </c>
-      <c r="Y48" s="13">
-        <f>G48/$AK48</f>
-        <v/>
-      </c>
-      <c r="Z48" s="13">
-        <f>H48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AA48" s="13">
-        <f>I48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AC48" s="13">
-        <f>K48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AD48" s="13">
-        <f>L48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AE48" s="13">
-        <f>M48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AG48" s="13">
-        <f>O48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AH48" s="13">
-        <f>P48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AI48" s="13">
-        <f>Q48/$AK48</f>
-        <v/>
-      </c>
-      <c r="AK48" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="B49" s="11" t="inlineStr">
@@ -5045,61 +3086,6 @@
         <v>2321</v>
       </c>
       <c r="S49" s="12" t="n"/>
-      <c r="T49" s="11">
-        <f>B49</f>
-        <v/>
-      </c>
-      <c r="U49" s="13">
-        <f>C49/$AK49</f>
-        <v/>
-      </c>
-      <c r="V49" s="13">
-        <f>D49/$AK49</f>
-        <v/>
-      </c>
-      <c r="W49" s="13">
-        <f>E49/$AK49</f>
-        <v/>
-      </c>
-      <c r="Y49" s="13">
-        <f>G49/$AK49</f>
-        <v/>
-      </c>
-      <c r="Z49" s="13">
-        <f>H49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AA49" s="13">
-        <f>I49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AC49" s="13">
-        <f>K49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AD49" s="13">
-        <f>L49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AE49" s="13">
-        <f>M49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AG49" s="13">
-        <f>O49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AH49" s="13">
-        <f>P49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AI49" s="13">
-        <f>Q49/$AK49</f>
-        <v/>
-      </c>
-      <c r="AK49" s="27" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="B50" s="11" t="inlineStr">
@@ -5147,61 +3133,6 @@
         <v>2162</v>
       </c>
       <c r="S50" s="12" t="n"/>
-      <c r="T50" s="11">
-        <f>B50</f>
-        <v/>
-      </c>
-      <c r="U50" s="13">
-        <f>C50/$AK50</f>
-        <v/>
-      </c>
-      <c r="V50" s="13">
-        <f>D50/$AK50</f>
-        <v/>
-      </c>
-      <c r="W50" s="13">
-        <f>E50/$AK50</f>
-        <v/>
-      </c>
-      <c r="Y50" s="13">
-        <f>G50/$AK50</f>
-        <v/>
-      </c>
-      <c r="Z50" s="13">
-        <f>H50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AA50" s="13">
-        <f>I50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AC50" s="13">
-        <f>K50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AD50" s="13">
-        <f>L50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AE50" s="13">
-        <f>M50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AG50" s="13">
-        <f>O50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AH50" s="13">
-        <f>P50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AI50" s="13">
-        <f>Q50/$AK50</f>
-        <v/>
-      </c>
-      <c r="AK50" s="27" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="51">
       <c r="B51" s="11" t="inlineStr">
@@ -6017,16 +3948,12 @@
       <c r="E122" s="12" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="6">
     <mergeCell ref="O14:Q14"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="U14:W14"/>
     <mergeCell ref="G14:I14"/>
-    <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="C10:Q10"/>
-    <mergeCell ref="AC14:AE14"/>
     <mergeCell ref="K14:M14"/>
-    <mergeCell ref="AG14:AI14"/>
     <mergeCell ref="C11:Q11"/>
   </mergeCells>
   <conditionalFormatting sqref="C16:Q50">
@@ -6037,4 +3964,2329 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="E11:V49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16.85546875" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="8"/>
+    <col width="11.7109375" customWidth="1" min="10" max="12"/>
+    <col width="11.85546875" customWidth="1" min="14" max="16"/>
+    <col width="12.85546875" customWidth="1" min="18" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="E11" s="46" t="inlineStr">
+        <is>
+          <t>Specialist Advice Activity by measure, per working day</t>
+        </is>
+      </c>
+      <c r="F11" s="43" t="n"/>
+      <c r="G11" s="43" t="n"/>
+      <c r="H11" s="43" t="n"/>
+      <c r="I11" s="43" t="n"/>
+      <c r="J11" s="47" t="n"/>
+      <c r="K11" s="43" t="n"/>
+      <c r="L11" s="43" t="n"/>
+      <c r="M11" s="43" t="n"/>
+      <c r="N11" s="43" t="n"/>
+      <c r="O11" s="43" t="n"/>
+      <c r="P11" s="43" t="n"/>
+      <c r="Q11" s="43" t="n"/>
+      <c r="R11" s="43" t="n"/>
+      <c r="S11" s="43" t="n"/>
+      <c r="T11" s="43" t="n"/>
+      <c r="U11" s="43" t="n"/>
+      <c r="V11" s="43" t="n"/>
+    </row>
+    <row r="12">
+      <c r="E12" s="1" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="1" t="n"/>
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="1" t="n"/>
+      <c r="K12" s="1" t="n"/>
+      <c r="L12" s="1" t="n"/>
+      <c r="M12" s="1" t="n"/>
+      <c r="N12" s="1" t="n"/>
+      <c r="O12" s="1" t="n"/>
+      <c r="P12" s="1" t="n"/>
+      <c r="Q12" s="1" t="n"/>
+      <c r="R12" s="1" t="n"/>
+      <c r="S12" s="1" t="n"/>
+      <c r="T12" s="1" t="n"/>
+      <c r="U12" s="1" t="n"/>
+      <c r="V12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="59" t="inlineStr">
+        <is>
+          <t>All types of Specialist Advice</t>
+        </is>
+      </c>
+      <c r="I13" s="21" t="n"/>
+      <c r="J13" s="60" t="inlineStr">
+        <is>
+          <t>Pre Referral Specialist Advice (e.g. Advice &amp; Guidance)</t>
+        </is>
+      </c>
+      <c r="K13" s="63" t="n"/>
+      <c r="L13" s="64" t="n"/>
+      <c r="M13" s="21" t="n"/>
+      <c r="N13" s="61" t="inlineStr">
+        <is>
+          <t>Post Referral Specialist Advice</t>
+        </is>
+      </c>
+      <c r="O13" s="63" t="n"/>
+      <c r="P13" s="64" t="n"/>
+      <c r="Q13" s="21" t="n"/>
+      <c r="R13" s="61" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="S13" s="63" t="n"/>
+      <c r="T13" s="64" t="n"/>
+      <c r="U13" s="1" t="n"/>
+      <c r="V13" s="1" t="n"/>
+    </row>
+    <row r="14" ht="90" customHeight="1">
+      <c r="E14" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Month </t>
+        </is>
+      </c>
+      <c r="F14" s="9" t="inlineStr">
+        <is>
+          <t>Total Requests 
+per working day</t>
+        </is>
+      </c>
+      <c r="G14" s="9" t="inlineStr">
+        <is>
+          <t>Processed Requests per working day</t>
+        </is>
+      </c>
+      <c r="H14" s="9" t="inlineStr">
+        <is>
+          <t>Diverted Requests per working day</t>
+        </is>
+      </c>
+      <c r="I14" s="22" t="n"/>
+      <c r="J14" s="61" t="inlineStr">
+        <is>
+          <t>Total Requests 
+per working day</t>
+        </is>
+      </c>
+      <c r="K14" s="61" t="inlineStr">
+        <is>
+          <t>Processed Requests per working day</t>
+        </is>
+      </c>
+      <c r="L14" s="61" t="inlineStr">
+        <is>
+          <t>Diverted Requests per working day</t>
+        </is>
+      </c>
+      <c r="M14" s="22" t="n"/>
+      <c r="N14" s="61" t="inlineStr">
+        <is>
+          <t>Total Requests 
+per working day</t>
+        </is>
+      </c>
+      <c r="O14" s="61" t="inlineStr">
+        <is>
+          <t>Processed Requests per working day</t>
+        </is>
+      </c>
+      <c r="P14" s="61" t="inlineStr">
+        <is>
+          <t>Diverted Requests per working day</t>
+        </is>
+      </c>
+      <c r="Q14" s="22" t="n"/>
+      <c r="R14" s="61" t="inlineStr">
+        <is>
+          <t>Total Requests 
+per working day</t>
+        </is>
+      </c>
+      <c r="S14" s="61" t="inlineStr">
+        <is>
+          <t>Processed Requests per working day</t>
+        </is>
+      </c>
+      <c r="T14" s="61" t="inlineStr">
+        <is>
+          <t>Diverted Requests per working day</t>
+        </is>
+      </c>
+      <c r="U14" s="1" t="n"/>
+      <c r="V14" s="28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No. of working days </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" s="11">
+        <f>'England | Specialist Advice'!B16</f>
+        <v/>
+      </c>
+      <c r="F15" s="13">
+        <f>'England | Specialist Advice'!C16/$V15</f>
+        <v/>
+      </c>
+      <c r="G15" s="13">
+        <f>'England | Specialist Advice'!D16/$V15</f>
+        <v/>
+      </c>
+      <c r="H15" s="13">
+        <f>'England | Specialist Advice'!E16/$V15</f>
+        <v/>
+      </c>
+      <c r="I15" s="1" t="n"/>
+      <c r="J15" s="13">
+        <f>'England | Specialist Advice'!G16/$V15</f>
+        <v/>
+      </c>
+      <c r="K15" s="13">
+        <f>'England | Specialist Advice'!H16/$V15</f>
+        <v/>
+      </c>
+      <c r="L15" s="13">
+        <f>'England | Specialist Advice'!I16/$V15</f>
+        <v/>
+      </c>
+      <c r="M15" s="1" t="n"/>
+      <c r="N15" s="13">
+        <f>'England | Specialist Advice'!K16/$V15</f>
+        <v/>
+      </c>
+      <c r="O15" s="13">
+        <f>'England | Specialist Advice'!L16/$V15</f>
+        <v/>
+      </c>
+      <c r="P15" s="13">
+        <f>'England | Specialist Advice'!M16/$V15</f>
+        <v/>
+      </c>
+      <c r="Q15" s="1" t="n"/>
+      <c r="R15" s="13">
+        <f>'England | Specialist Advice'!O16/$V15</f>
+        <v/>
+      </c>
+      <c r="S15" s="13">
+        <f>'England | Specialist Advice'!P16/$V15</f>
+        <v/>
+      </c>
+      <c r="T15" s="13">
+        <f>'England | Specialist Advice'!Q16/$V15</f>
+        <v/>
+      </c>
+      <c r="U15" s="12" t="n"/>
+      <c r="V15" s="27" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" s="11">
+        <f>'England | Specialist Advice'!B17</f>
+        <v/>
+      </c>
+      <c r="F16" s="13">
+        <f>'England | Specialist Advice'!C17/$V16</f>
+        <v/>
+      </c>
+      <c r="G16" s="13">
+        <f>'England | Specialist Advice'!D17/$V16</f>
+        <v/>
+      </c>
+      <c r="H16" s="13">
+        <f>'England | Specialist Advice'!E17/$V16</f>
+        <v/>
+      </c>
+      <c r="I16" s="1" t="n"/>
+      <c r="J16" s="13">
+        <f>'England | Specialist Advice'!G17/$V16</f>
+        <v/>
+      </c>
+      <c r="K16" s="13">
+        <f>'England | Specialist Advice'!H17/$V16</f>
+        <v/>
+      </c>
+      <c r="L16" s="13">
+        <f>'England | Specialist Advice'!I17/$V16</f>
+        <v/>
+      </c>
+      <c r="M16" s="1" t="n"/>
+      <c r="N16" s="13">
+        <f>'England | Specialist Advice'!K17/$V16</f>
+        <v/>
+      </c>
+      <c r="O16" s="13">
+        <f>'England | Specialist Advice'!L17/$V16</f>
+        <v/>
+      </c>
+      <c r="P16" s="13">
+        <f>'England | Specialist Advice'!M17/$V16</f>
+        <v/>
+      </c>
+      <c r="Q16" s="1" t="n"/>
+      <c r="R16" s="13">
+        <f>'England | Specialist Advice'!O17/$V16</f>
+        <v/>
+      </c>
+      <c r="S16" s="13">
+        <f>'England | Specialist Advice'!P17/$V16</f>
+        <v/>
+      </c>
+      <c r="T16" s="13">
+        <f>'England | Specialist Advice'!Q17/$V16</f>
+        <v/>
+      </c>
+      <c r="U16" s="12" t="n"/>
+      <c r="V16" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" s="11">
+        <f>'England | Specialist Advice'!B18</f>
+        <v/>
+      </c>
+      <c r="F17" s="13">
+        <f>'England | Specialist Advice'!C18/$V17</f>
+        <v/>
+      </c>
+      <c r="G17" s="13">
+        <f>'England | Specialist Advice'!D18/$V17</f>
+        <v/>
+      </c>
+      <c r="H17" s="13">
+        <f>'England | Specialist Advice'!E18/$V17</f>
+        <v/>
+      </c>
+      <c r="I17" s="1" t="n"/>
+      <c r="J17" s="13">
+        <f>'England | Specialist Advice'!G18/$V17</f>
+        <v/>
+      </c>
+      <c r="K17" s="13">
+        <f>'England | Specialist Advice'!H18/$V17</f>
+        <v/>
+      </c>
+      <c r="L17" s="13">
+        <f>'England | Specialist Advice'!I18/$V17</f>
+        <v/>
+      </c>
+      <c r="M17" s="1" t="n"/>
+      <c r="N17" s="13">
+        <f>'England | Specialist Advice'!K18/$V17</f>
+        <v/>
+      </c>
+      <c r="O17" s="13">
+        <f>'England | Specialist Advice'!L18/$V17</f>
+        <v/>
+      </c>
+      <c r="P17" s="13">
+        <f>'England | Specialist Advice'!M18/$V17</f>
+        <v/>
+      </c>
+      <c r="Q17" s="1" t="n"/>
+      <c r="R17" s="13">
+        <f>'England | Specialist Advice'!O18/$V17</f>
+        <v/>
+      </c>
+      <c r="S17" s="13">
+        <f>'England | Specialist Advice'!P18/$V17</f>
+        <v/>
+      </c>
+      <c r="T17" s="13">
+        <f>'England | Specialist Advice'!Q18/$V17</f>
+        <v/>
+      </c>
+      <c r="U17" s="12" t="n"/>
+      <c r="V17" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" s="11">
+        <f>'England | Specialist Advice'!B19</f>
+        <v/>
+      </c>
+      <c r="F18" s="13">
+        <f>'England | Specialist Advice'!C19/$V18</f>
+        <v/>
+      </c>
+      <c r="G18" s="13">
+        <f>'England | Specialist Advice'!D19/$V18</f>
+        <v/>
+      </c>
+      <c r="H18" s="13">
+        <f>'England | Specialist Advice'!E19/$V18</f>
+        <v/>
+      </c>
+      <c r="I18" s="1" t="n"/>
+      <c r="J18" s="13">
+        <f>'England | Specialist Advice'!G19/$V18</f>
+        <v/>
+      </c>
+      <c r="K18" s="13">
+        <f>'England | Specialist Advice'!H19/$V18</f>
+        <v/>
+      </c>
+      <c r="L18" s="13">
+        <f>'England | Specialist Advice'!I19/$V18</f>
+        <v/>
+      </c>
+      <c r="M18" s="1" t="n"/>
+      <c r="N18" s="13">
+        <f>'England | Specialist Advice'!K19/$V18</f>
+        <v/>
+      </c>
+      <c r="O18" s="13">
+        <f>'England | Specialist Advice'!L19/$V18</f>
+        <v/>
+      </c>
+      <c r="P18" s="13">
+        <f>'England | Specialist Advice'!M19/$V18</f>
+        <v/>
+      </c>
+      <c r="Q18" s="1" t="n"/>
+      <c r="R18" s="13">
+        <f>'England | Specialist Advice'!O19/$V18</f>
+        <v/>
+      </c>
+      <c r="S18" s="13">
+        <f>'England | Specialist Advice'!P19/$V18</f>
+        <v/>
+      </c>
+      <c r="T18" s="13">
+        <f>'England | Specialist Advice'!Q19/$V18</f>
+        <v/>
+      </c>
+      <c r="U18" s="12" t="n"/>
+      <c r="V18" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" s="11">
+        <f>'England | Specialist Advice'!B20</f>
+        <v/>
+      </c>
+      <c r="F19" s="13">
+        <f>'England | Specialist Advice'!C20/$V19</f>
+        <v/>
+      </c>
+      <c r="G19" s="13">
+        <f>'England | Specialist Advice'!D20/$V19</f>
+        <v/>
+      </c>
+      <c r="H19" s="13">
+        <f>'England | Specialist Advice'!E20/$V19</f>
+        <v/>
+      </c>
+      <c r="I19" s="1" t="n"/>
+      <c r="J19" s="13">
+        <f>'England | Specialist Advice'!G20/$V19</f>
+        <v/>
+      </c>
+      <c r="K19" s="13">
+        <f>'England | Specialist Advice'!H20/$V19</f>
+        <v/>
+      </c>
+      <c r="L19" s="13">
+        <f>'England | Specialist Advice'!I20/$V19</f>
+        <v/>
+      </c>
+      <c r="M19" s="1" t="n"/>
+      <c r="N19" s="13">
+        <f>'England | Specialist Advice'!K20/$V19</f>
+        <v/>
+      </c>
+      <c r="O19" s="13">
+        <f>'England | Specialist Advice'!L20/$V19</f>
+        <v/>
+      </c>
+      <c r="P19" s="13">
+        <f>'England | Specialist Advice'!M20/$V19</f>
+        <v/>
+      </c>
+      <c r="Q19" s="1" t="n"/>
+      <c r="R19" s="13">
+        <f>'England | Specialist Advice'!O20/$V19</f>
+        <v/>
+      </c>
+      <c r="S19" s="13">
+        <f>'England | Specialist Advice'!P20/$V19</f>
+        <v/>
+      </c>
+      <c r="T19" s="13">
+        <f>'England | Specialist Advice'!Q20/$V19</f>
+        <v/>
+      </c>
+      <c r="U19" s="12" t="n"/>
+      <c r="V19" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" s="11">
+        <f>'England | Specialist Advice'!B21</f>
+        <v/>
+      </c>
+      <c r="F20" s="13">
+        <f>'England | Specialist Advice'!C21/$V20</f>
+        <v/>
+      </c>
+      <c r="G20" s="13">
+        <f>'England | Specialist Advice'!D21/$V20</f>
+        <v/>
+      </c>
+      <c r="H20" s="13">
+        <f>'England | Specialist Advice'!E21/$V20</f>
+        <v/>
+      </c>
+      <c r="I20" s="1" t="n"/>
+      <c r="J20" s="13">
+        <f>'England | Specialist Advice'!G21/$V20</f>
+        <v/>
+      </c>
+      <c r="K20" s="13">
+        <f>'England | Specialist Advice'!H21/$V20</f>
+        <v/>
+      </c>
+      <c r="L20" s="13">
+        <f>'England | Specialist Advice'!I21/$V20</f>
+        <v/>
+      </c>
+      <c r="M20" s="1" t="n"/>
+      <c r="N20" s="13">
+        <f>'England | Specialist Advice'!K21/$V20</f>
+        <v/>
+      </c>
+      <c r="O20" s="13">
+        <f>'England | Specialist Advice'!L21/$V20</f>
+        <v/>
+      </c>
+      <c r="P20" s="13">
+        <f>'England | Specialist Advice'!M21/$V20</f>
+        <v/>
+      </c>
+      <c r="Q20" s="1" t="n"/>
+      <c r="R20" s="13">
+        <f>'England | Specialist Advice'!O21/$V20</f>
+        <v/>
+      </c>
+      <c r="S20" s="13">
+        <f>'England | Specialist Advice'!P21/$V20</f>
+        <v/>
+      </c>
+      <c r="T20" s="13">
+        <f>'England | Specialist Advice'!Q21/$V20</f>
+        <v/>
+      </c>
+      <c r="U20" s="15" t="n"/>
+      <c r="V20" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="11">
+        <f>'England | Specialist Advice'!B22</f>
+        <v/>
+      </c>
+      <c r="F21" s="13">
+        <f>'England | Specialist Advice'!C22/$V21</f>
+        <v/>
+      </c>
+      <c r="G21" s="13">
+        <f>'England | Specialist Advice'!D22/$V21</f>
+        <v/>
+      </c>
+      <c r="H21" s="13">
+        <f>'England | Specialist Advice'!E22/$V21</f>
+        <v/>
+      </c>
+      <c r="I21" s="1" t="n"/>
+      <c r="J21" s="13">
+        <f>'England | Specialist Advice'!G22/$V21</f>
+        <v/>
+      </c>
+      <c r="K21" s="13">
+        <f>'England | Specialist Advice'!H22/$V21</f>
+        <v/>
+      </c>
+      <c r="L21" s="13">
+        <f>'England | Specialist Advice'!I22/$V21</f>
+        <v/>
+      </c>
+      <c r="M21" s="1" t="n"/>
+      <c r="N21" s="13">
+        <f>'England | Specialist Advice'!K22/$V21</f>
+        <v/>
+      </c>
+      <c r="O21" s="13">
+        <f>'England | Specialist Advice'!L22/$V21</f>
+        <v/>
+      </c>
+      <c r="P21" s="13">
+        <f>'England | Specialist Advice'!M22/$V21</f>
+        <v/>
+      </c>
+      <c r="Q21" s="1" t="n"/>
+      <c r="R21" s="13">
+        <f>'England | Specialist Advice'!O22/$V21</f>
+        <v/>
+      </c>
+      <c r="S21" s="13">
+        <f>'England | Specialist Advice'!P22/$V21</f>
+        <v/>
+      </c>
+      <c r="T21" s="13">
+        <f>'England | Specialist Advice'!Q22/$V21</f>
+        <v/>
+      </c>
+      <c r="U21" s="15" t="n"/>
+      <c r="V21" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" s="11">
+        <f>'England | Specialist Advice'!B23</f>
+        <v/>
+      </c>
+      <c r="F22" s="13">
+        <f>'England | Specialist Advice'!C23/$V22</f>
+        <v/>
+      </c>
+      <c r="G22" s="13">
+        <f>'England | Specialist Advice'!D23/$V22</f>
+        <v/>
+      </c>
+      <c r="H22" s="13">
+        <f>'England | Specialist Advice'!E23/$V22</f>
+        <v/>
+      </c>
+      <c r="I22" s="1" t="n"/>
+      <c r="J22" s="13">
+        <f>'England | Specialist Advice'!G23/$V22</f>
+        <v/>
+      </c>
+      <c r="K22" s="13">
+        <f>'England | Specialist Advice'!H23/$V22</f>
+        <v/>
+      </c>
+      <c r="L22" s="13">
+        <f>'England | Specialist Advice'!I23/$V22</f>
+        <v/>
+      </c>
+      <c r="M22" s="1" t="n"/>
+      <c r="N22" s="13">
+        <f>'England | Specialist Advice'!K23/$V22</f>
+        <v/>
+      </c>
+      <c r="O22" s="13">
+        <f>'England | Specialist Advice'!L23/$V22</f>
+        <v/>
+      </c>
+      <c r="P22" s="13">
+        <f>'England | Specialist Advice'!M23/$V22</f>
+        <v/>
+      </c>
+      <c r="Q22" s="1" t="n"/>
+      <c r="R22" s="13">
+        <f>'England | Specialist Advice'!O23/$V22</f>
+        <v/>
+      </c>
+      <c r="S22" s="13">
+        <f>'England | Specialist Advice'!P23/$V22</f>
+        <v/>
+      </c>
+      <c r="T22" s="13">
+        <f>'England | Specialist Advice'!Q23/$V22</f>
+        <v/>
+      </c>
+      <c r="U22" s="15" t="n"/>
+      <c r="V22" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" s="11">
+        <f>'England | Specialist Advice'!B24</f>
+        <v/>
+      </c>
+      <c r="F23" s="13">
+        <f>'England | Specialist Advice'!C24/$V23</f>
+        <v/>
+      </c>
+      <c r="G23" s="13">
+        <f>'England | Specialist Advice'!D24/$V23</f>
+        <v/>
+      </c>
+      <c r="H23" s="13">
+        <f>'England | Specialist Advice'!E24/$V23</f>
+        <v/>
+      </c>
+      <c r="I23" s="1" t="n"/>
+      <c r="J23" s="13">
+        <f>'England | Specialist Advice'!G24/$V23</f>
+        <v/>
+      </c>
+      <c r="K23" s="13">
+        <f>'England | Specialist Advice'!H24/$V23</f>
+        <v/>
+      </c>
+      <c r="L23" s="13">
+        <f>'England | Specialist Advice'!I24/$V23</f>
+        <v/>
+      </c>
+      <c r="M23" s="1" t="n"/>
+      <c r="N23" s="13">
+        <f>'England | Specialist Advice'!K24/$V23</f>
+        <v/>
+      </c>
+      <c r="O23" s="13">
+        <f>'England | Specialist Advice'!L24/$V23</f>
+        <v/>
+      </c>
+      <c r="P23" s="13">
+        <f>'England | Specialist Advice'!M24/$V23</f>
+        <v/>
+      </c>
+      <c r="Q23" s="1" t="n"/>
+      <c r="R23" s="13">
+        <f>'England | Specialist Advice'!O24/$V23</f>
+        <v/>
+      </c>
+      <c r="S23" s="13">
+        <f>'England | Specialist Advice'!P24/$V23</f>
+        <v/>
+      </c>
+      <c r="T23" s="13">
+        <f>'England | Specialist Advice'!Q24/$V23</f>
+        <v/>
+      </c>
+      <c r="U23" s="15" t="n"/>
+      <c r="V23" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" s="11">
+        <f>'England | Specialist Advice'!B25</f>
+        <v/>
+      </c>
+      <c r="F24" s="13">
+        <f>'England | Specialist Advice'!C25/$V24</f>
+        <v/>
+      </c>
+      <c r="G24" s="13">
+        <f>'England | Specialist Advice'!D25/$V24</f>
+        <v/>
+      </c>
+      <c r="H24" s="13">
+        <f>'England | Specialist Advice'!E25/$V24</f>
+        <v/>
+      </c>
+      <c r="I24" s="1" t="n"/>
+      <c r="J24" s="13">
+        <f>'England | Specialist Advice'!G25/$V24</f>
+        <v/>
+      </c>
+      <c r="K24" s="13">
+        <f>'England | Specialist Advice'!H25/$V24</f>
+        <v/>
+      </c>
+      <c r="L24" s="13">
+        <f>'England | Specialist Advice'!I25/$V24</f>
+        <v/>
+      </c>
+      <c r="M24" s="1" t="n"/>
+      <c r="N24" s="13">
+        <f>'England | Specialist Advice'!K25/$V24</f>
+        <v/>
+      </c>
+      <c r="O24" s="13">
+        <f>'England | Specialist Advice'!L25/$V24</f>
+        <v/>
+      </c>
+      <c r="P24" s="13">
+        <f>'England | Specialist Advice'!M25/$V24</f>
+        <v/>
+      </c>
+      <c r="Q24" s="1" t="n"/>
+      <c r="R24" s="13">
+        <f>'England | Specialist Advice'!O25/$V24</f>
+        <v/>
+      </c>
+      <c r="S24" s="13">
+        <f>'England | Specialist Advice'!P25/$V24</f>
+        <v/>
+      </c>
+      <c r="T24" s="13">
+        <f>'England | Specialist Advice'!Q25/$V24</f>
+        <v/>
+      </c>
+      <c r="U24" s="15" t="n"/>
+      <c r="V24" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" s="11">
+        <f>'England | Specialist Advice'!B26</f>
+        <v/>
+      </c>
+      <c r="F25" s="13">
+        <f>'England | Specialist Advice'!C26/$V25</f>
+        <v/>
+      </c>
+      <c r="G25" s="13">
+        <f>'England | Specialist Advice'!D26/$V25</f>
+        <v/>
+      </c>
+      <c r="H25" s="13">
+        <f>'England | Specialist Advice'!E26/$V25</f>
+        <v/>
+      </c>
+      <c r="I25" s="1" t="n"/>
+      <c r="J25" s="13">
+        <f>'England | Specialist Advice'!G26/$V25</f>
+        <v/>
+      </c>
+      <c r="K25" s="13">
+        <f>'England | Specialist Advice'!H26/$V25</f>
+        <v/>
+      </c>
+      <c r="L25" s="13">
+        <f>'England | Specialist Advice'!I26/$V25</f>
+        <v/>
+      </c>
+      <c r="M25" s="1" t="n"/>
+      <c r="N25" s="13">
+        <f>'England | Specialist Advice'!K26/$V25</f>
+        <v/>
+      </c>
+      <c r="O25" s="13">
+        <f>'England | Specialist Advice'!L26/$V25</f>
+        <v/>
+      </c>
+      <c r="P25" s="13">
+        <f>'England | Specialist Advice'!M26/$V25</f>
+        <v/>
+      </c>
+      <c r="Q25" s="1" t="n"/>
+      <c r="R25" s="13">
+        <f>'England | Specialist Advice'!O26/$V25</f>
+        <v/>
+      </c>
+      <c r="S25" s="13">
+        <f>'England | Specialist Advice'!P26/$V25</f>
+        <v/>
+      </c>
+      <c r="T25" s="13">
+        <f>'England | Specialist Advice'!Q26/$V25</f>
+        <v/>
+      </c>
+      <c r="U25" s="15" t="n"/>
+      <c r="V25" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" s="11">
+        <f>'England | Specialist Advice'!B27</f>
+        <v/>
+      </c>
+      <c r="F26" s="13">
+        <f>'England | Specialist Advice'!C27/$V26</f>
+        <v/>
+      </c>
+      <c r="G26" s="13">
+        <f>'England | Specialist Advice'!D27/$V26</f>
+        <v/>
+      </c>
+      <c r="H26" s="13">
+        <f>'England | Specialist Advice'!E27/$V26</f>
+        <v/>
+      </c>
+      <c r="I26" s="1" t="n"/>
+      <c r="J26" s="13">
+        <f>'England | Specialist Advice'!G27/$V26</f>
+        <v/>
+      </c>
+      <c r="K26" s="13">
+        <f>'England | Specialist Advice'!H27/$V26</f>
+        <v/>
+      </c>
+      <c r="L26" s="13">
+        <f>'England | Specialist Advice'!I27/$V26</f>
+        <v/>
+      </c>
+      <c r="M26" s="1" t="n"/>
+      <c r="N26" s="13">
+        <f>'England | Specialist Advice'!K27/$V26</f>
+        <v/>
+      </c>
+      <c r="O26" s="13">
+        <f>'England | Specialist Advice'!L27/$V26</f>
+        <v/>
+      </c>
+      <c r="P26" s="13">
+        <f>'England | Specialist Advice'!M27/$V26</f>
+        <v/>
+      </c>
+      <c r="Q26" s="1" t="n"/>
+      <c r="R26" s="13">
+        <f>'England | Specialist Advice'!O27/$V26</f>
+        <v/>
+      </c>
+      <c r="S26" s="13">
+        <f>'England | Specialist Advice'!P27/$V26</f>
+        <v/>
+      </c>
+      <c r="T26" s="13">
+        <f>'England | Specialist Advice'!Q27/$V26</f>
+        <v/>
+      </c>
+      <c r="U26" s="15" t="n"/>
+      <c r="V26" s="27" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" s="11">
+        <f>'England | Specialist Advice'!B28</f>
+        <v/>
+      </c>
+      <c r="F27" s="13">
+        <f>'England | Specialist Advice'!C28/$V27</f>
+        <v/>
+      </c>
+      <c r="G27" s="13">
+        <f>'England | Specialist Advice'!D28/$V27</f>
+        <v/>
+      </c>
+      <c r="H27" s="13">
+        <f>'England | Specialist Advice'!E28/$V27</f>
+        <v/>
+      </c>
+      <c r="I27" s="1" t="n"/>
+      <c r="J27" s="13">
+        <f>'England | Specialist Advice'!G28/$V27</f>
+        <v/>
+      </c>
+      <c r="K27" s="13">
+        <f>'England | Specialist Advice'!H28/$V27</f>
+        <v/>
+      </c>
+      <c r="L27" s="13">
+        <f>'England | Specialist Advice'!I28/$V27</f>
+        <v/>
+      </c>
+      <c r="M27" s="1" t="n"/>
+      <c r="N27" s="13">
+        <f>'England | Specialist Advice'!K28/$V27</f>
+        <v/>
+      </c>
+      <c r="O27" s="13">
+        <f>'England | Specialist Advice'!L28/$V27</f>
+        <v/>
+      </c>
+      <c r="P27" s="13">
+        <f>'England | Specialist Advice'!M28/$V27</f>
+        <v/>
+      </c>
+      <c r="Q27" s="1" t="n"/>
+      <c r="R27" s="13">
+        <f>'England | Specialist Advice'!O28/$V27</f>
+        <v/>
+      </c>
+      <c r="S27" s="13">
+        <f>'England | Specialist Advice'!P28/$V27</f>
+        <v/>
+      </c>
+      <c r="T27" s="13">
+        <f>'England | Specialist Advice'!Q28/$V27</f>
+        <v/>
+      </c>
+      <c r="U27" s="15" t="n"/>
+      <c r="V27" s="27" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" s="11">
+        <f>'England | Specialist Advice'!B29</f>
+        <v/>
+      </c>
+      <c r="F28" s="13">
+        <f>'England | Specialist Advice'!C29/$V28</f>
+        <v/>
+      </c>
+      <c r="G28" s="13">
+        <f>'England | Specialist Advice'!D29/$V28</f>
+        <v/>
+      </c>
+      <c r="H28" s="13">
+        <f>'England | Specialist Advice'!E29/$V28</f>
+        <v/>
+      </c>
+      <c r="I28" s="1" t="n"/>
+      <c r="J28" s="13">
+        <f>'England | Specialist Advice'!G29/$V28</f>
+        <v/>
+      </c>
+      <c r="K28" s="13">
+        <f>'England | Specialist Advice'!H29/$V28</f>
+        <v/>
+      </c>
+      <c r="L28" s="13">
+        <f>'England | Specialist Advice'!I29/$V28</f>
+        <v/>
+      </c>
+      <c r="M28" s="1" t="n"/>
+      <c r="N28" s="13">
+        <f>'England | Specialist Advice'!K29/$V28</f>
+        <v/>
+      </c>
+      <c r="O28" s="13">
+        <f>'England | Specialist Advice'!L29/$V28</f>
+        <v/>
+      </c>
+      <c r="P28" s="13">
+        <f>'England | Specialist Advice'!M29/$V28</f>
+        <v/>
+      </c>
+      <c r="Q28" s="1" t="n"/>
+      <c r="R28" s="13">
+        <f>'England | Specialist Advice'!O29/$V28</f>
+        <v/>
+      </c>
+      <c r="S28" s="13">
+        <f>'England | Specialist Advice'!P29/$V28</f>
+        <v/>
+      </c>
+      <c r="T28" s="13">
+        <f>'England | Specialist Advice'!Q29/$V28</f>
+        <v/>
+      </c>
+      <c r="U28" s="15" t="n"/>
+      <c r="V28" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="11">
+        <f>'England | Specialist Advice'!B30</f>
+        <v/>
+      </c>
+      <c r="F29" s="13">
+        <f>'England | Specialist Advice'!C30/$V29</f>
+        <v/>
+      </c>
+      <c r="G29" s="13">
+        <f>'England | Specialist Advice'!D30/$V29</f>
+        <v/>
+      </c>
+      <c r="H29" s="13">
+        <f>'England | Specialist Advice'!E30/$V29</f>
+        <v/>
+      </c>
+      <c r="I29" s="1" t="n"/>
+      <c r="J29" s="13">
+        <f>'England | Specialist Advice'!G30/$V29</f>
+        <v/>
+      </c>
+      <c r="K29" s="13">
+        <f>'England | Specialist Advice'!H30/$V29</f>
+        <v/>
+      </c>
+      <c r="L29" s="13">
+        <f>'England | Specialist Advice'!I30/$V29</f>
+        <v/>
+      </c>
+      <c r="M29" s="1" t="n"/>
+      <c r="N29" s="13">
+        <f>'England | Specialist Advice'!K30/$V29</f>
+        <v/>
+      </c>
+      <c r="O29" s="13">
+        <f>'England | Specialist Advice'!L30/$V29</f>
+        <v/>
+      </c>
+      <c r="P29" s="13">
+        <f>'England | Specialist Advice'!M30/$V29</f>
+        <v/>
+      </c>
+      <c r="Q29" s="1" t="n"/>
+      <c r="R29" s="13">
+        <f>'England | Specialist Advice'!O30/$V29</f>
+        <v/>
+      </c>
+      <c r="S29" s="13">
+        <f>'England | Specialist Advice'!P30/$V29</f>
+        <v/>
+      </c>
+      <c r="T29" s="13">
+        <f>'England | Specialist Advice'!Q30/$V29</f>
+        <v/>
+      </c>
+      <c r="U29" s="15" t="n"/>
+      <c r="V29" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" s="11">
+        <f>'England | Specialist Advice'!B31</f>
+        <v/>
+      </c>
+      <c r="F30" s="13">
+        <f>'England | Specialist Advice'!C31/$V30</f>
+        <v/>
+      </c>
+      <c r="G30" s="13">
+        <f>'England | Specialist Advice'!D31/$V30</f>
+        <v/>
+      </c>
+      <c r="H30" s="13">
+        <f>'England | Specialist Advice'!E31/$V30</f>
+        <v/>
+      </c>
+      <c r="I30" s="1" t="n"/>
+      <c r="J30" s="13">
+        <f>'England | Specialist Advice'!G31/$V30</f>
+        <v/>
+      </c>
+      <c r="K30" s="13">
+        <f>'England | Specialist Advice'!H31/$V30</f>
+        <v/>
+      </c>
+      <c r="L30" s="13">
+        <f>'England | Specialist Advice'!I31/$V30</f>
+        <v/>
+      </c>
+      <c r="M30" s="1" t="n"/>
+      <c r="N30" s="13">
+        <f>'England | Specialist Advice'!K31/$V30</f>
+        <v/>
+      </c>
+      <c r="O30" s="13">
+        <f>'England | Specialist Advice'!L31/$V30</f>
+        <v/>
+      </c>
+      <c r="P30" s="13">
+        <f>'England | Specialist Advice'!M31/$V30</f>
+        <v/>
+      </c>
+      <c r="Q30" s="1" t="n"/>
+      <c r="R30" s="13">
+        <f>'England | Specialist Advice'!O31/$V30</f>
+        <v/>
+      </c>
+      <c r="S30" s="13">
+        <f>'England | Specialist Advice'!P31/$V30</f>
+        <v/>
+      </c>
+      <c r="T30" s="13">
+        <f>'England | Specialist Advice'!Q31/$V30</f>
+        <v/>
+      </c>
+      <c r="U30" s="15" t="n"/>
+      <c r="V30" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" s="11">
+        <f>'England | Specialist Advice'!B32</f>
+        <v/>
+      </c>
+      <c r="F31" s="13">
+        <f>'England | Specialist Advice'!C32/$V31</f>
+        <v/>
+      </c>
+      <c r="G31" s="13">
+        <f>'England | Specialist Advice'!D32/$V31</f>
+        <v/>
+      </c>
+      <c r="H31" s="13">
+        <f>'England | Specialist Advice'!E32/$V31</f>
+        <v/>
+      </c>
+      <c r="I31" s="1" t="n"/>
+      <c r="J31" s="13">
+        <f>'England | Specialist Advice'!G32/$V31</f>
+        <v/>
+      </c>
+      <c r="K31" s="13">
+        <f>'England | Specialist Advice'!H32/$V31</f>
+        <v/>
+      </c>
+      <c r="L31" s="13">
+        <f>'England | Specialist Advice'!I32/$V31</f>
+        <v/>
+      </c>
+      <c r="M31" s="1" t="n"/>
+      <c r="N31" s="13">
+        <f>'England | Specialist Advice'!K32/$V31</f>
+        <v/>
+      </c>
+      <c r="O31" s="13">
+        <f>'England | Specialist Advice'!L32/$V31</f>
+        <v/>
+      </c>
+      <c r="P31" s="13">
+        <f>'England | Specialist Advice'!M32/$V31</f>
+        <v/>
+      </c>
+      <c r="Q31" s="1" t="n"/>
+      <c r="R31" s="13">
+        <f>'England | Specialist Advice'!O32/$V31</f>
+        <v/>
+      </c>
+      <c r="S31" s="13">
+        <f>'England | Specialist Advice'!P32/$V31</f>
+        <v/>
+      </c>
+      <c r="T31" s="13">
+        <f>'England | Specialist Advice'!Q32/$V31</f>
+        <v/>
+      </c>
+      <c r="U31" s="15" t="n"/>
+      <c r="V31" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" s="11">
+        <f>'England | Specialist Advice'!B33</f>
+        <v/>
+      </c>
+      <c r="F32" s="13">
+        <f>'England | Specialist Advice'!C33/$V32</f>
+        <v/>
+      </c>
+      <c r="G32" s="13">
+        <f>'England | Specialist Advice'!D33/$V32</f>
+        <v/>
+      </c>
+      <c r="H32" s="13">
+        <f>'England | Specialist Advice'!E33/$V32</f>
+        <v/>
+      </c>
+      <c r="I32" s="1" t="n"/>
+      <c r="J32" s="13">
+        <f>'England | Specialist Advice'!G33/$V32</f>
+        <v/>
+      </c>
+      <c r="K32" s="13">
+        <f>'England | Specialist Advice'!H33/$V32</f>
+        <v/>
+      </c>
+      <c r="L32" s="13">
+        <f>'England | Specialist Advice'!I33/$V32</f>
+        <v/>
+      </c>
+      <c r="M32" s="1" t="n"/>
+      <c r="N32" s="13">
+        <f>'England | Specialist Advice'!K33/$V32</f>
+        <v/>
+      </c>
+      <c r="O32" s="13">
+        <f>'England | Specialist Advice'!L33/$V32</f>
+        <v/>
+      </c>
+      <c r="P32" s="13">
+        <f>'England | Specialist Advice'!M33/$V32</f>
+        <v/>
+      </c>
+      <c r="Q32" s="1" t="n"/>
+      <c r="R32" s="13">
+        <f>'England | Specialist Advice'!O33/$V32</f>
+        <v/>
+      </c>
+      <c r="S32" s="13">
+        <f>'England | Specialist Advice'!P33/$V32</f>
+        <v/>
+      </c>
+      <c r="T32" s="13">
+        <f>'England | Specialist Advice'!Q33/$V32</f>
+        <v/>
+      </c>
+      <c r="U32" s="12" t="n"/>
+      <c r="V32" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" s="11">
+        <f>'England | Specialist Advice'!B34</f>
+        <v/>
+      </c>
+      <c r="F33" s="13">
+        <f>'England | Specialist Advice'!C34/$V33</f>
+        <v/>
+      </c>
+      <c r="G33" s="13">
+        <f>'England | Specialist Advice'!D34/$V33</f>
+        <v/>
+      </c>
+      <c r="H33" s="13">
+        <f>'England | Specialist Advice'!E34/$V33</f>
+        <v/>
+      </c>
+      <c r="I33" s="1" t="n"/>
+      <c r="J33" s="13">
+        <f>'England | Specialist Advice'!G34/$V33</f>
+        <v/>
+      </c>
+      <c r="K33" s="13">
+        <f>'England | Specialist Advice'!H34/$V33</f>
+        <v/>
+      </c>
+      <c r="L33" s="13">
+        <f>'England | Specialist Advice'!I34/$V33</f>
+        <v/>
+      </c>
+      <c r="M33" s="1" t="n"/>
+      <c r="N33" s="13">
+        <f>'England | Specialist Advice'!K34/$V33</f>
+        <v/>
+      </c>
+      <c r="O33" s="13">
+        <f>'England | Specialist Advice'!L34/$V33</f>
+        <v/>
+      </c>
+      <c r="P33" s="13">
+        <f>'England | Specialist Advice'!M34/$V33</f>
+        <v/>
+      </c>
+      <c r="Q33" s="1" t="n"/>
+      <c r="R33" s="13">
+        <f>'England | Specialist Advice'!O34/$V33</f>
+        <v/>
+      </c>
+      <c r="S33" s="13">
+        <f>'England | Specialist Advice'!P34/$V33</f>
+        <v/>
+      </c>
+      <c r="T33" s="13">
+        <f>'England | Specialist Advice'!Q34/$V33</f>
+        <v/>
+      </c>
+      <c r="U33" s="12" t="n"/>
+      <c r="V33" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" s="11">
+        <f>'England | Specialist Advice'!B35</f>
+        <v/>
+      </c>
+      <c r="F34" s="13">
+        <f>'England | Specialist Advice'!C35/$V34</f>
+        <v/>
+      </c>
+      <c r="G34" s="13">
+        <f>'England | Specialist Advice'!D35/$V34</f>
+        <v/>
+      </c>
+      <c r="H34" s="13">
+        <f>'England | Specialist Advice'!E35/$V34</f>
+        <v/>
+      </c>
+      <c r="I34" s="1" t="n"/>
+      <c r="J34" s="13">
+        <f>'England | Specialist Advice'!G35/$V34</f>
+        <v/>
+      </c>
+      <c r="K34" s="13">
+        <f>'England | Specialist Advice'!H35/$V34</f>
+        <v/>
+      </c>
+      <c r="L34" s="13">
+        <f>'England | Specialist Advice'!I35/$V34</f>
+        <v/>
+      </c>
+      <c r="M34" s="1" t="n"/>
+      <c r="N34" s="13">
+        <f>'England | Specialist Advice'!K35/$V34</f>
+        <v/>
+      </c>
+      <c r="O34" s="13">
+        <f>'England | Specialist Advice'!L35/$V34</f>
+        <v/>
+      </c>
+      <c r="P34" s="13">
+        <f>'England | Specialist Advice'!M35/$V34</f>
+        <v/>
+      </c>
+      <c r="Q34" s="1" t="n"/>
+      <c r="R34" s="13">
+        <f>'England | Specialist Advice'!O35/$V34</f>
+        <v/>
+      </c>
+      <c r="S34" s="13">
+        <f>'England | Specialist Advice'!P35/$V34</f>
+        <v/>
+      </c>
+      <c r="T34" s="13">
+        <f>'England | Specialist Advice'!Q35/$V34</f>
+        <v/>
+      </c>
+      <c r="U34" s="12" t="n"/>
+      <c r="V34" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" s="11">
+        <f>'England | Specialist Advice'!B36</f>
+        <v/>
+      </c>
+      <c r="F35" s="13">
+        <f>'England | Specialist Advice'!C36/$V35</f>
+        <v/>
+      </c>
+      <c r="G35" s="13">
+        <f>'England | Specialist Advice'!D36/$V35</f>
+        <v/>
+      </c>
+      <c r="H35" s="13">
+        <f>'England | Specialist Advice'!E36/$V35</f>
+        <v/>
+      </c>
+      <c r="I35" s="1" t="n"/>
+      <c r="J35" s="13">
+        <f>'England | Specialist Advice'!G36/$V35</f>
+        <v/>
+      </c>
+      <c r="K35" s="13">
+        <f>'England | Specialist Advice'!H36/$V35</f>
+        <v/>
+      </c>
+      <c r="L35" s="13">
+        <f>'England | Specialist Advice'!I36/$V35</f>
+        <v/>
+      </c>
+      <c r="M35" s="1" t="n"/>
+      <c r="N35" s="13">
+        <f>'England | Specialist Advice'!K36/$V35</f>
+        <v/>
+      </c>
+      <c r="O35" s="13">
+        <f>'England | Specialist Advice'!L36/$V35</f>
+        <v/>
+      </c>
+      <c r="P35" s="13">
+        <f>'England | Specialist Advice'!M36/$V35</f>
+        <v/>
+      </c>
+      <c r="Q35" s="1" t="n"/>
+      <c r="R35" s="13">
+        <f>'England | Specialist Advice'!O36/$V35</f>
+        <v/>
+      </c>
+      <c r="S35" s="13">
+        <f>'England | Specialist Advice'!P36/$V35</f>
+        <v/>
+      </c>
+      <c r="T35" s="13">
+        <f>'England | Specialist Advice'!Q36/$V35</f>
+        <v/>
+      </c>
+      <c r="U35" s="12" t="n"/>
+      <c r="V35" s="27" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" s="11">
+        <f>'England | Specialist Advice'!B37</f>
+        <v/>
+      </c>
+      <c r="F36" s="13">
+        <f>'England | Specialist Advice'!C37/$V36</f>
+        <v/>
+      </c>
+      <c r="G36" s="13">
+        <f>'England | Specialist Advice'!D37/$V36</f>
+        <v/>
+      </c>
+      <c r="H36" s="13">
+        <f>'England | Specialist Advice'!E37/$V36</f>
+        <v/>
+      </c>
+      <c r="I36" s="1" t="n"/>
+      <c r="J36" s="13">
+        <f>'England | Specialist Advice'!G37/$V36</f>
+        <v/>
+      </c>
+      <c r="K36" s="13">
+        <f>'England | Specialist Advice'!H37/$V36</f>
+        <v/>
+      </c>
+      <c r="L36" s="13">
+        <f>'England | Specialist Advice'!I37/$V36</f>
+        <v/>
+      </c>
+      <c r="M36" s="1" t="n"/>
+      <c r="N36" s="13">
+        <f>'England | Specialist Advice'!K37/$V36</f>
+        <v/>
+      </c>
+      <c r="O36" s="13">
+        <f>'England | Specialist Advice'!L37/$V36</f>
+        <v/>
+      </c>
+      <c r="P36" s="13">
+        <f>'England | Specialist Advice'!M37/$V36</f>
+        <v/>
+      </c>
+      <c r="Q36" s="1" t="n"/>
+      <c r="R36" s="13">
+        <f>'England | Specialist Advice'!O37/$V36</f>
+        <v/>
+      </c>
+      <c r="S36" s="13">
+        <f>'England | Specialist Advice'!P37/$V36</f>
+        <v/>
+      </c>
+      <c r="T36" s="13">
+        <f>'England | Specialist Advice'!Q37/$V36</f>
+        <v/>
+      </c>
+      <c r="U36" s="12" t="n"/>
+      <c r="V36" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" s="11">
+        <f>'England | Specialist Advice'!B38</f>
+        <v/>
+      </c>
+      <c r="F37" s="13">
+        <f>'England | Specialist Advice'!C38/$V37</f>
+        <v/>
+      </c>
+      <c r="G37" s="13">
+        <f>'England | Specialist Advice'!D38/$V37</f>
+        <v/>
+      </c>
+      <c r="H37" s="13">
+        <f>'England | Specialist Advice'!E38/$V37</f>
+        <v/>
+      </c>
+      <c r="I37" s="1" t="n"/>
+      <c r="J37" s="13">
+        <f>'England | Specialist Advice'!G38/$V37</f>
+        <v/>
+      </c>
+      <c r="K37" s="13">
+        <f>'England | Specialist Advice'!H38/$V37</f>
+        <v/>
+      </c>
+      <c r="L37" s="13">
+        <f>'England | Specialist Advice'!I38/$V37</f>
+        <v/>
+      </c>
+      <c r="M37" s="1" t="n"/>
+      <c r="N37" s="13">
+        <f>'England | Specialist Advice'!K38/$V37</f>
+        <v/>
+      </c>
+      <c r="O37" s="13">
+        <f>'England | Specialist Advice'!L38/$V37</f>
+        <v/>
+      </c>
+      <c r="P37" s="13">
+        <f>'England | Specialist Advice'!M38/$V37</f>
+        <v/>
+      </c>
+      <c r="Q37" s="1" t="n"/>
+      <c r="R37" s="13">
+        <f>'England | Specialist Advice'!O38/$V37</f>
+        <v/>
+      </c>
+      <c r="S37" s="13">
+        <f>'England | Specialist Advice'!P38/$V37</f>
+        <v/>
+      </c>
+      <c r="T37" s="13">
+        <f>'England | Specialist Advice'!Q38/$V37</f>
+        <v/>
+      </c>
+      <c r="U37" s="12" t="n"/>
+      <c r="V37" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" s="11">
+        <f>'England | Specialist Advice'!B39</f>
+        <v/>
+      </c>
+      <c r="F38" s="13">
+        <f>'England | Specialist Advice'!C39/$V38</f>
+        <v/>
+      </c>
+      <c r="G38" s="13">
+        <f>'England | Specialist Advice'!D39/$V38</f>
+        <v/>
+      </c>
+      <c r="H38" s="13">
+        <f>'England | Specialist Advice'!E39/$V38</f>
+        <v/>
+      </c>
+      <c r="I38" s="1" t="n"/>
+      <c r="J38" s="13">
+        <f>'England | Specialist Advice'!G39/$V38</f>
+        <v/>
+      </c>
+      <c r="K38" s="13">
+        <f>'England | Specialist Advice'!H39/$V38</f>
+        <v/>
+      </c>
+      <c r="L38" s="13">
+        <f>'England | Specialist Advice'!I39/$V38</f>
+        <v/>
+      </c>
+      <c r="M38" s="1" t="n"/>
+      <c r="N38" s="13">
+        <f>'England | Specialist Advice'!K39/$V38</f>
+        <v/>
+      </c>
+      <c r="O38" s="13">
+        <f>'England | Specialist Advice'!L39/$V38</f>
+        <v/>
+      </c>
+      <c r="P38" s="13">
+        <f>'England | Specialist Advice'!M39/$V38</f>
+        <v/>
+      </c>
+      <c r="Q38" s="1" t="n"/>
+      <c r="R38" s="13">
+        <f>'England | Specialist Advice'!O39/$V38</f>
+        <v/>
+      </c>
+      <c r="S38" s="13">
+        <f>'England | Specialist Advice'!P39/$V38</f>
+        <v/>
+      </c>
+      <c r="T38" s="13">
+        <f>'England | Specialist Advice'!Q39/$V38</f>
+        <v/>
+      </c>
+      <c r="U38" s="12" t="n"/>
+      <c r="V38" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" s="11">
+        <f>'England | Specialist Advice'!B40</f>
+        <v/>
+      </c>
+      <c r="F39" s="13">
+        <f>'England | Specialist Advice'!C40/$V39</f>
+        <v/>
+      </c>
+      <c r="G39" s="13">
+        <f>'England | Specialist Advice'!D40/$V39</f>
+        <v/>
+      </c>
+      <c r="H39" s="13">
+        <f>'England | Specialist Advice'!E40/$V39</f>
+        <v/>
+      </c>
+      <c r="I39" s="1" t="n"/>
+      <c r="J39" s="13">
+        <f>'England | Specialist Advice'!G40/$V39</f>
+        <v/>
+      </c>
+      <c r="K39" s="13">
+        <f>'England | Specialist Advice'!H40/$V39</f>
+        <v/>
+      </c>
+      <c r="L39" s="13">
+        <f>'England | Specialist Advice'!I40/$V39</f>
+        <v/>
+      </c>
+      <c r="M39" s="1" t="n"/>
+      <c r="N39" s="13">
+        <f>'England | Specialist Advice'!K40/$V39</f>
+        <v/>
+      </c>
+      <c r="O39" s="13">
+        <f>'England | Specialist Advice'!L40/$V39</f>
+        <v/>
+      </c>
+      <c r="P39" s="13">
+        <f>'England | Specialist Advice'!M40/$V39</f>
+        <v/>
+      </c>
+      <c r="Q39" s="1" t="n"/>
+      <c r="R39" s="13">
+        <f>'England | Specialist Advice'!O40/$V39</f>
+        <v/>
+      </c>
+      <c r="S39" s="13">
+        <f>'England | Specialist Advice'!P40/$V39</f>
+        <v/>
+      </c>
+      <c r="T39" s="13">
+        <f>'England | Specialist Advice'!Q40/$V39</f>
+        <v/>
+      </c>
+      <c r="U39" s="12" t="n"/>
+      <c r="V39" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" s="11">
+        <f>'England | Specialist Advice'!B41</f>
+        <v/>
+      </c>
+      <c r="F40" s="13">
+        <f>'England | Specialist Advice'!C41/$V40</f>
+        <v/>
+      </c>
+      <c r="G40" s="13">
+        <f>'England | Specialist Advice'!D41/$V40</f>
+        <v/>
+      </c>
+      <c r="H40" s="13">
+        <f>'England | Specialist Advice'!E41/$V40</f>
+        <v/>
+      </c>
+      <c r="I40" s="1" t="n"/>
+      <c r="J40" s="13">
+        <f>'England | Specialist Advice'!G41/$V40</f>
+        <v/>
+      </c>
+      <c r="K40" s="13">
+        <f>'England | Specialist Advice'!H41/$V40</f>
+        <v/>
+      </c>
+      <c r="L40" s="13">
+        <f>'England | Specialist Advice'!I41/$V40</f>
+        <v/>
+      </c>
+      <c r="M40" s="1" t="n"/>
+      <c r="N40" s="13">
+        <f>'England | Specialist Advice'!K41/$V40</f>
+        <v/>
+      </c>
+      <c r="O40" s="13">
+        <f>'England | Specialist Advice'!L41/$V40</f>
+        <v/>
+      </c>
+      <c r="P40" s="13">
+        <f>'England | Specialist Advice'!M41/$V40</f>
+        <v/>
+      </c>
+      <c r="Q40" s="1" t="n"/>
+      <c r="R40" s="13">
+        <f>'England | Specialist Advice'!O41/$V40</f>
+        <v/>
+      </c>
+      <c r="S40" s="13">
+        <f>'England | Specialist Advice'!P41/$V40</f>
+        <v/>
+      </c>
+      <c r="T40" s="13">
+        <f>'England | Specialist Advice'!Q41/$V40</f>
+        <v/>
+      </c>
+      <c r="U40" s="12" t="n"/>
+      <c r="V40" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" s="11">
+        <f>'England | Specialist Advice'!B42</f>
+        <v/>
+      </c>
+      <c r="F41" s="13">
+        <f>'England | Specialist Advice'!C42/$V41</f>
+        <v/>
+      </c>
+      <c r="G41" s="13">
+        <f>'England | Specialist Advice'!D42/$V41</f>
+        <v/>
+      </c>
+      <c r="H41" s="13">
+        <f>'England | Specialist Advice'!E42/$V41</f>
+        <v/>
+      </c>
+      <c r="I41" s="1" t="n"/>
+      <c r="J41" s="13">
+        <f>'England | Specialist Advice'!G42/$V41</f>
+        <v/>
+      </c>
+      <c r="K41" s="13">
+        <f>'England | Specialist Advice'!H42/$V41</f>
+        <v/>
+      </c>
+      <c r="L41" s="13">
+        <f>'England | Specialist Advice'!I42/$V41</f>
+        <v/>
+      </c>
+      <c r="M41" s="1" t="n"/>
+      <c r="N41" s="13">
+        <f>'England | Specialist Advice'!K42/$V41</f>
+        <v/>
+      </c>
+      <c r="O41" s="13">
+        <f>'England | Specialist Advice'!L42/$V41</f>
+        <v/>
+      </c>
+      <c r="P41" s="13">
+        <f>'England | Specialist Advice'!M42/$V41</f>
+        <v/>
+      </c>
+      <c r="Q41" s="1" t="n"/>
+      <c r="R41" s="13">
+        <f>'England | Specialist Advice'!O42/$V41</f>
+        <v/>
+      </c>
+      <c r="S41" s="13">
+        <f>'England | Specialist Advice'!P42/$V41</f>
+        <v/>
+      </c>
+      <c r="T41" s="13">
+        <f>'England | Specialist Advice'!Q42/$V41</f>
+        <v/>
+      </c>
+      <c r="U41" s="12" t="n"/>
+      <c r="V41" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" s="11">
+        <f>'England | Specialist Advice'!B43</f>
+        <v/>
+      </c>
+      <c r="F42" s="13">
+        <f>'England | Specialist Advice'!C43/$V42</f>
+        <v/>
+      </c>
+      <c r="G42" s="13">
+        <f>'England | Specialist Advice'!D43/$V42</f>
+        <v/>
+      </c>
+      <c r="H42" s="13">
+        <f>'England | Specialist Advice'!E43/$V42</f>
+        <v/>
+      </c>
+      <c r="I42" s="1" t="n"/>
+      <c r="J42" s="13">
+        <f>'England | Specialist Advice'!G43/$V42</f>
+        <v/>
+      </c>
+      <c r="K42" s="13">
+        <f>'England | Specialist Advice'!H43/$V42</f>
+        <v/>
+      </c>
+      <c r="L42" s="13">
+        <f>'England | Specialist Advice'!I43/$V42</f>
+        <v/>
+      </c>
+      <c r="M42" s="1" t="n"/>
+      <c r="N42" s="13">
+        <f>'England | Specialist Advice'!K43/$V42</f>
+        <v/>
+      </c>
+      <c r="O42" s="13">
+        <f>'England | Specialist Advice'!L43/$V42</f>
+        <v/>
+      </c>
+      <c r="P42" s="13">
+        <f>'England | Specialist Advice'!M43/$V42</f>
+        <v/>
+      </c>
+      <c r="Q42" s="1" t="n"/>
+      <c r="R42" s="13">
+        <f>'England | Specialist Advice'!O43/$V42</f>
+        <v/>
+      </c>
+      <c r="S42" s="13">
+        <f>'England | Specialist Advice'!P43/$V42</f>
+        <v/>
+      </c>
+      <c r="T42" s="13">
+        <f>'England | Specialist Advice'!Q43/$V42</f>
+        <v/>
+      </c>
+      <c r="U42" s="12" t="n"/>
+      <c r="V42" s="27" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" s="11">
+        <f>'England | Specialist Advice'!B44</f>
+        <v/>
+      </c>
+      <c r="F43" s="13">
+        <f>'England | Specialist Advice'!C44/$V43</f>
+        <v/>
+      </c>
+      <c r="G43" s="13">
+        <f>'England | Specialist Advice'!D44/$V43</f>
+        <v/>
+      </c>
+      <c r="H43" s="13">
+        <f>'England | Specialist Advice'!E44/$V43</f>
+        <v/>
+      </c>
+      <c r="I43" s="1" t="n"/>
+      <c r="J43" s="13">
+        <f>'England | Specialist Advice'!G44/$V43</f>
+        <v/>
+      </c>
+      <c r="K43" s="13">
+        <f>'England | Specialist Advice'!H44/$V43</f>
+        <v/>
+      </c>
+      <c r="L43" s="13">
+        <f>'England | Specialist Advice'!I44/$V43</f>
+        <v/>
+      </c>
+      <c r="M43" s="1" t="n"/>
+      <c r="N43" s="13">
+        <f>'England | Specialist Advice'!K44/$V43</f>
+        <v/>
+      </c>
+      <c r="O43" s="13">
+        <f>'England | Specialist Advice'!L44/$V43</f>
+        <v/>
+      </c>
+      <c r="P43" s="13">
+        <f>'England | Specialist Advice'!M44/$V43</f>
+        <v/>
+      </c>
+      <c r="Q43" s="1" t="n"/>
+      <c r="R43" s="13">
+        <f>'England | Specialist Advice'!O44/$V43</f>
+        <v/>
+      </c>
+      <c r="S43" s="13">
+        <f>'England | Specialist Advice'!P44/$V43</f>
+        <v/>
+      </c>
+      <c r="T43" s="13">
+        <f>'England | Specialist Advice'!Q44/$V43</f>
+        <v/>
+      </c>
+      <c r="U43" s="12" t="n"/>
+      <c r="V43" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" s="11">
+        <f>'England | Specialist Advice'!B45</f>
+        <v/>
+      </c>
+      <c r="F44" s="13">
+        <f>'England | Specialist Advice'!C45/$V44</f>
+        <v/>
+      </c>
+      <c r="G44" s="13">
+        <f>'England | Specialist Advice'!D45/$V44</f>
+        <v/>
+      </c>
+      <c r="H44" s="13">
+        <f>'England | Specialist Advice'!E45/$V44</f>
+        <v/>
+      </c>
+      <c r="I44" s="1" t="n"/>
+      <c r="J44" s="13">
+        <f>'England | Specialist Advice'!G45/$V44</f>
+        <v/>
+      </c>
+      <c r="K44" s="13">
+        <f>'England | Specialist Advice'!H45/$V44</f>
+        <v/>
+      </c>
+      <c r="L44" s="13">
+        <f>'England | Specialist Advice'!I45/$V44</f>
+        <v/>
+      </c>
+      <c r="M44" s="1" t="n"/>
+      <c r="N44" s="13">
+        <f>'England | Specialist Advice'!K45/$V44</f>
+        <v/>
+      </c>
+      <c r="O44" s="13">
+        <f>'England | Specialist Advice'!L45/$V44</f>
+        <v/>
+      </c>
+      <c r="P44" s="13">
+        <f>'England | Specialist Advice'!M45/$V44</f>
+        <v/>
+      </c>
+      <c r="Q44" s="1" t="n"/>
+      <c r="R44" s="13">
+        <f>'England | Specialist Advice'!O45/$V44</f>
+        <v/>
+      </c>
+      <c r="S44" s="13">
+        <f>'England | Specialist Advice'!P45/$V44</f>
+        <v/>
+      </c>
+      <c r="T44" s="13">
+        <f>'England | Specialist Advice'!Q45/$V44</f>
+        <v/>
+      </c>
+      <c r="U44" s="1" t="n"/>
+      <c r="V44" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" s="11">
+        <f>'England | Specialist Advice'!B46</f>
+        <v/>
+      </c>
+      <c r="F45" s="13">
+        <f>'England | Specialist Advice'!C46/$V45</f>
+        <v/>
+      </c>
+      <c r="G45" s="13">
+        <f>'England | Specialist Advice'!D46/$V45</f>
+        <v/>
+      </c>
+      <c r="H45" s="13">
+        <f>'England | Specialist Advice'!E46/$V45</f>
+        <v/>
+      </c>
+      <c r="I45" s="1" t="n"/>
+      <c r="J45" s="13">
+        <f>'England | Specialist Advice'!G46/$V45</f>
+        <v/>
+      </c>
+      <c r="K45" s="13">
+        <f>'England | Specialist Advice'!H46/$V45</f>
+        <v/>
+      </c>
+      <c r="L45" s="13">
+        <f>'England | Specialist Advice'!I46/$V45</f>
+        <v/>
+      </c>
+      <c r="M45" s="1" t="n"/>
+      <c r="N45" s="13">
+        <f>'England | Specialist Advice'!K46/$V45</f>
+        <v/>
+      </c>
+      <c r="O45" s="13">
+        <f>'England | Specialist Advice'!L46/$V45</f>
+        <v/>
+      </c>
+      <c r="P45" s="13">
+        <f>'England | Specialist Advice'!M46/$V45</f>
+        <v/>
+      </c>
+      <c r="Q45" s="1" t="n"/>
+      <c r="R45" s="13">
+        <f>'England | Specialist Advice'!O46/$V45</f>
+        <v/>
+      </c>
+      <c r="S45" s="13">
+        <f>'England | Specialist Advice'!P46/$V45</f>
+        <v/>
+      </c>
+      <c r="T45" s="13">
+        <f>'England | Specialist Advice'!Q46/$V45</f>
+        <v/>
+      </c>
+      <c r="U45" s="1" t="n"/>
+      <c r="V45" s="27" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" s="11">
+        <f>'England | Specialist Advice'!B47</f>
+        <v/>
+      </c>
+      <c r="F46" s="13">
+        <f>'England | Specialist Advice'!C47/$V46</f>
+        <v/>
+      </c>
+      <c r="G46" s="13">
+        <f>'England | Specialist Advice'!D47/$V46</f>
+        <v/>
+      </c>
+      <c r="H46" s="13">
+        <f>'England | Specialist Advice'!E47/$V46</f>
+        <v/>
+      </c>
+      <c r="I46" s="1" t="n"/>
+      <c r="J46" s="13">
+        <f>'England | Specialist Advice'!G47/$V46</f>
+        <v/>
+      </c>
+      <c r="K46" s="13">
+        <f>'England | Specialist Advice'!H47/$V46</f>
+        <v/>
+      </c>
+      <c r="L46" s="13">
+        <f>'England | Specialist Advice'!I47/$V46</f>
+        <v/>
+      </c>
+      <c r="M46" s="1" t="n"/>
+      <c r="N46" s="13">
+        <f>'England | Specialist Advice'!K47/$V46</f>
+        <v/>
+      </c>
+      <c r="O46" s="13">
+        <f>'England | Specialist Advice'!L47/$V46</f>
+        <v/>
+      </c>
+      <c r="P46" s="13">
+        <f>'England | Specialist Advice'!M47/$V46</f>
+        <v/>
+      </c>
+      <c r="Q46" s="1" t="n"/>
+      <c r="R46" s="13">
+        <f>'England | Specialist Advice'!O47/$V46</f>
+        <v/>
+      </c>
+      <c r="S46" s="13">
+        <f>'England | Specialist Advice'!P47/$V46</f>
+        <v/>
+      </c>
+      <c r="T46" s="13">
+        <f>'England | Specialist Advice'!Q47/$V46</f>
+        <v/>
+      </c>
+      <c r="U46" s="1" t="n"/>
+      <c r="V46" s="27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" s="11">
+        <f>'England | Specialist Advice'!B48</f>
+        <v/>
+      </c>
+      <c r="F47" s="13">
+        <f>'England | Specialist Advice'!C48/$V47</f>
+        <v/>
+      </c>
+      <c r="G47" s="13">
+        <f>'England | Specialist Advice'!D48/$V47</f>
+        <v/>
+      </c>
+      <c r="H47" s="13">
+        <f>'England | Specialist Advice'!E48/$V47</f>
+        <v/>
+      </c>
+      <c r="I47" s="1" t="n"/>
+      <c r="J47" s="13">
+        <f>'England | Specialist Advice'!G48/$V47</f>
+        <v/>
+      </c>
+      <c r="K47" s="13">
+        <f>'England | Specialist Advice'!H48/$V47</f>
+        <v/>
+      </c>
+      <c r="L47" s="13">
+        <f>'England | Specialist Advice'!I48/$V47</f>
+        <v/>
+      </c>
+      <c r="M47" s="1" t="n"/>
+      <c r="N47" s="13">
+        <f>'England | Specialist Advice'!K48/$V47</f>
+        <v/>
+      </c>
+      <c r="O47" s="13">
+        <f>'England | Specialist Advice'!L48/$V47</f>
+        <v/>
+      </c>
+      <c r="P47" s="13">
+        <f>'England | Specialist Advice'!M48/$V47</f>
+        <v/>
+      </c>
+      <c r="Q47" s="1" t="n"/>
+      <c r="R47" s="13">
+        <f>'England | Specialist Advice'!O48/$V47</f>
+        <v/>
+      </c>
+      <c r="S47" s="13">
+        <f>'England | Specialist Advice'!P48/$V47</f>
+        <v/>
+      </c>
+      <c r="T47" s="13">
+        <f>'England | Specialist Advice'!Q48/$V47</f>
+        <v/>
+      </c>
+      <c r="U47" s="1" t="n"/>
+      <c r="V47" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" s="11">
+        <f>'England | Specialist Advice'!B49</f>
+        <v/>
+      </c>
+      <c r="F48" s="13">
+        <f>'England | Specialist Advice'!C49/$V48</f>
+        <v/>
+      </c>
+      <c r="G48" s="13">
+        <f>'England | Specialist Advice'!D49/$V48</f>
+        <v/>
+      </c>
+      <c r="H48" s="13">
+        <f>'England | Specialist Advice'!E49/$V48</f>
+        <v/>
+      </c>
+      <c r="I48" s="1" t="n"/>
+      <c r="J48" s="13">
+        <f>'England | Specialist Advice'!G49/$V48</f>
+        <v/>
+      </c>
+      <c r="K48" s="13">
+        <f>'England | Specialist Advice'!H49/$V48</f>
+        <v/>
+      </c>
+      <c r="L48" s="13">
+        <f>'England | Specialist Advice'!I49/$V48</f>
+        <v/>
+      </c>
+      <c r="M48" s="1" t="n"/>
+      <c r="N48" s="13">
+        <f>'England | Specialist Advice'!K49/$V48</f>
+        <v/>
+      </c>
+      <c r="O48" s="13">
+        <f>'England | Specialist Advice'!L49/$V48</f>
+        <v/>
+      </c>
+      <c r="P48" s="13">
+        <f>'England | Specialist Advice'!M49/$V48</f>
+        <v/>
+      </c>
+      <c r="Q48" s="1" t="n"/>
+      <c r="R48" s="13">
+        <f>'England | Specialist Advice'!O49/$V48</f>
+        <v/>
+      </c>
+      <c r="S48" s="13">
+        <f>'England | Specialist Advice'!P49/$V48</f>
+        <v/>
+      </c>
+      <c r="T48" s="13">
+        <f>'England | Specialist Advice'!Q49/$V48</f>
+        <v/>
+      </c>
+      <c r="U48" s="1" t="n"/>
+      <c r="V48" s="27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" s="11">
+        <f>'England | Specialist Advice'!B50</f>
+        <v/>
+      </c>
+      <c r="F49" s="13">
+        <f>'England | Specialist Advice'!C50/$V49</f>
+        <v/>
+      </c>
+      <c r="G49" s="13">
+        <f>'England | Specialist Advice'!D50/$V49</f>
+        <v/>
+      </c>
+      <c r="H49" s="13">
+        <f>'England | Specialist Advice'!E50/$V49</f>
+        <v/>
+      </c>
+      <c r="I49" s="1" t="n"/>
+      <c r="J49" s="13">
+        <f>'England | Specialist Advice'!G50/$V49</f>
+        <v/>
+      </c>
+      <c r="K49" s="13">
+        <f>'England | Specialist Advice'!H50/$V49</f>
+        <v/>
+      </c>
+      <c r="L49" s="13">
+        <f>'England | Specialist Advice'!I50/$V49</f>
+        <v/>
+      </c>
+      <c r="M49" s="1" t="n"/>
+      <c r="N49" s="13">
+        <f>'England | Specialist Advice'!K50/$V49</f>
+        <v/>
+      </c>
+      <c r="O49" s="13">
+        <f>'England | Specialist Advice'!L50/$V49</f>
+        <v/>
+      </c>
+      <c r="P49" s="13">
+        <f>'England | Specialist Advice'!M50/$V49</f>
+        <v/>
+      </c>
+      <c r="Q49" s="1" t="n"/>
+      <c r="R49" s="13">
+        <f>'England | Specialist Advice'!O50/$V49</f>
+        <v/>
+      </c>
+      <c r="S49" s="13">
+        <f>'England | Specialist Advice'!P50/$V49</f>
+        <v/>
+      </c>
+      <c r="T49" s="13">
+        <f>'England | Specialist Advice'!Q50/$V49</f>
+        <v/>
+      </c>
+      <c r="U49" s="1" t="n"/>
+      <c r="V49" s="27" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="R13:T13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>